<commit_message>
added some more traditional territories
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="567">
   <si>
     <t xml:space="preserve">TRANSMOUNTAIN EXPANSION PROJECT - INDIGENOUS COMMUNITIES _IMC </t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t xml:space="preserve">Chawathil First Nation  ("Shi-Wa-Thill")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chawathil First Nation</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Rhoda Peters, next election July 14, 2022</t>
@@ -249,6 +252,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Chiyom Agassiz (Cheam) First Nation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Andrew Victor, next election November 29, 2021. Councillors; Bruce (BJ), Douglas, Darwin Jason Douglas, John Lincoln Douglas, Stephanie Fredette, Fredick (Rick) Quipp, </t>
   </si>
   <si>
@@ -268,6 +274,9 @@
   </si>
   <si>
     <t xml:space="preserve">Coldwater First Nation (Nc/etko - the people of the creeks)      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coldwater First Nation</t>
   </si>
   <si>
     <r>
@@ -337,7 +346,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Cook's Ferry Indian Band                                   </t>
+      <t xml:space="preserve">Cook's Ferry Indian Band </t>
     </r>
     <r>
       <rPr>
@@ -346,8 +355,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> Kumcheen (Variation Nkumcheen); Includes Pokheistk (Variation Pakeist, Pokheistsk), Pemynoos (Variation Piminos), Spatsum (Variation Spaptsin), Spence'S Bridge</t>
+      <t xml:space="preserve">Kumcheen (Variation Nkumcheen); Includes Pokheistk (Variation Pakeist, Pokheistsk), Pemynoos (Variation Piminos), Spatsum (Variation Spaptsin), Spence'S Bridge</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cook's Ferry Indian Band</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Christine Minnabarriet, next election December 5, 2022</t>
@@ -400,7 +412,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Ditidaht First Nation                   </t>
+      <t xml:space="preserve">Ditidaht First Nation </t>
     </r>
     <r>
       <rPr>
@@ -409,8 +421,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> Formerly Nitinaht (Pre-1984) (Variation Nitinat)</t>
+      <t xml:space="preserve">Formerly Nitinaht (Pre-1984) (Variation Nitinat)</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ditidaht First Nation</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Councillor Brian Tate, next election July 15, 2023. Councillors; Anne Pettet, Paul Sieber, Kelly Sport, Darryl Tate, </t>
@@ -433,6 +448,9 @@
   </si>
   <si>
     <t xml:space="preserve">Esquimalt Nation (Xwsepsum or Kosapsum)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esquimalt Nation</t>
   </si>
   <si>
     <t xml:space="preserve">Andrew Thomas, Hereditary Chief (appointed January 14, 2019)  Elected Chief Thomas Robert - 4 year term, next election October 1, 2023</t>
@@ -2624,8 +2642,8 @@
   </sheetPr>
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2877,1000 +2895,1059 @@
       <c r="A9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="5" t="str">
-        <f aca="false">A9</f>
-        <v>Chawathil First Nation  ("Shi-Wa-Thill")</v>
+      <c r="B9" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>49.283272</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>-121.291263</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="134.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="5" t="str">
-        <f aca="false">A10</f>
-        <v>Chi:yo:m Agassiz (Cheam) First Nation - meaning "Wild Strawberry Place"</v>
+        <v>62</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>23</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>49.540481</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>-121.7239</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="180" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <f aca="false">A11</f>
-        <v>Coldwater First Nation (Nc/etko - the people of the creeks)</v>
+        <v>69</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>50.027994</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>-120.41473</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="5" t="str">
-        <f aca="false">A12</f>
-        <v>Cook's Ferry Indian Band                                    Kumcheen (Variation Nkumcheen); Includes Pokheistk (Variation Pakeist, Pokheistsk), Pemynoos (Variation Piminos), Spatsum (Variation Spaptsin), Spence'S Bridge</v>
+        <v>76</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>50.032193</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>-120.617392</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="205.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <f aca="false">A13</f>
-        <v>Cowichan Tribes</v>
+        <v>84</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>48.888822</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>-123.752153</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="159.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="5" t="str">
-        <f aca="false">A14</f>
-        <v>Ditidaht First Nation                    Formerly Nitinaht (Pre-1984) (Variation Nitinat)</v>
+        <v>91</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>93</v>
+        <v>98</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>48.890317</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>-124.592686</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <f aca="false">A15</f>
-        <v>Esquimalt Nation (Xwsepsum or Kosapsum)</v>
+        <v>99</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>99</v>
+        <v>105</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>48.688573</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>-123.453132</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="191.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B16" s="5" t="str">
         <f aca="false">A16</f>
         <v>Halalt First Nation</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>106</v>
+        <v>112</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>48.929783</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>-124.479846</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B17" s="5" t="str">
         <f aca="false">A17</f>
         <v>Heiltsuk First Nation</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="13" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="10" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>111</v>
+        <v>117</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>52.337794</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>-127.826237</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="126" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="19" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B18" s="5" t="str">
         <f aca="false">A18</f>
         <v>Huu-ay-aht First Nation</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>117</v>
+        <v>123</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>48.833479</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>-124.929585</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="165.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B19" s="5" t="str">
         <f aca="false">A19</f>
         <v>Katzie First Nation</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H19" s="11"/>
+      <c r="I19" s="0" t="n">
+        <v>49.557619</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>-122.607872</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="19" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B20" s="5" t="str">
         <f aca="false">A20</f>
         <v>Kwantlen First Nation (tireless Runner)</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="160.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="21" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B21" s="5" t="str">
         <f aca="false">A21</f>
         <v>Kwaw -Kwaw-Aplit First Nations</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H21" s="15"/>
     </row>
     <row r="22" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B22" s="5" t="str">
         <f aca="false">A22</f>
         <v>Kwikwetlem First Nation</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="26" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B23" s="5" t="str">
         <f aca="false">A23</f>
         <v>Leq' a: mel First Nation</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="I23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="27" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B24" s="5" t="str">
         <f aca="false">A24</f>
         <v>Little Shuswap Lake Indian Band (Skwlax meaning "Black Bear")</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="195" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B25" s="5" t="str">
         <f aca="false">A25</f>
         <v>Lheidli T'enneh First Nation</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="174.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B26" s="5" t="str">
         <f aca="false">A26</f>
         <v>Lhtako Dene Nation</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="195" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B27" s="5" t="str">
         <f aca="false">A27</f>
         <v>Lower Nicola Indian Band -</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B28" s="5" t="str">
         <f aca="false">A28</f>
         <v>Lower Similkameen #598</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="H28" s="15"/>
     </row>
     <row r="29" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="29" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B29" s="5" t="str">
         <f aca="false">A29</f>
         <v>Lyackson First Nation</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="126.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B30" s="5" t="str">
         <f aca="false">A30</f>
         <v>Malahat First Nation</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="30" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B31" s="5" t="str">
         <f aca="false">A31</f>
         <v>Matsqui First Nation</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H31" s="15"/>
     </row>
     <row r="32" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B32" s="5" t="str">
         <f aca="false">A32</f>
         <v>Musqeam Indian Band</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B33" s="5" t="str">
         <f aca="false">A33</f>
         <v>Neskonlith Indian Band</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B34" s="5" t="str">
         <f aca="false">A34</f>
         <v>Nooaitch Indian Band</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="32" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B35" s="5" t="str">
         <f aca="false">A35</f>
         <v>Osoyoos</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="F35" s="33"/>
       <c r="G35" s="10" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B36" s="5" t="str">
         <f aca="false">A36</f>
         <v>Pacheedaht First Nation</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B37" s="5" t="str">
         <f aca="false">A37</f>
         <v>Pauquachin Nation</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="H37" s="15"/>
     </row>
     <row r="38" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B38" s="5" t="str">
         <f aca="false">A38</f>
         <v>Penticton Indian Band</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B39" s="5" t="str">
         <f aca="false">A39</f>
         <v>Peters Band (Peters First Nation)</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="14" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B40" s="5" t="str">
         <f aca="false">A40</f>
         <v>Penelakut Tribe</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="14" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B41" s="5" t="str">
         <f aca="false">A41</f>
         <v>Popkum First Nation</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="H41" s="15"/>
     </row>
     <row r="42" customFormat="false" ht="127.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="14" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="B42" s="5" t="str">
         <f aca="false">A42</f>
         <v>Qayqayt First Nation (New Westminister)</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="H42" s="15"/>
     </row>
     <row r="43" customFormat="false" ht="98.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="34" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B43" s="5" t="str">
         <f aca="false">A43</f>
         <v>Scia'new First Nation (Beecher Bay First Nation)</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="35" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="B44" s="5" t="str">
         <f aca="false">A44</f>
         <v>Sq'ewlets (Scowlitz) First Nation</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="34" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B45" s="5" t="str">
         <f aca="false">A45</f>
         <v>Seabird Island Band</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="H45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="151.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="17" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="D46" s="13"/>
       <c r="E46" s="36" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="F46" s="36"/>
       <c r="G46" s="37" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="I46" s="2" t="n">
         <v>51.527017</v>
@@ -3881,32 +3958,32 @@
     </row>
     <row r="47" customFormat="false" ht="286.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="17" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B47" s="5" t="str">
         <f aca="false">A47</f>
         <v>Semiahmoo First Nation</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="H47" s="15"/>
     </row>
     <row r="48" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="38" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="B48" s="5" t="str">
         <f aca="false">A48</f>
@@ -3919,7 +3996,7 @@
         <v>14</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>16</v>
@@ -3928,984 +4005,984 @@
         <v>17</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="111.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="34" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
       <c r="B49" s="5" t="str">
         <f aca="false">A49</f>
         <v>Shackan Indian Band</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="F49" s="36"/>
       <c r="G49" s="10" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="183" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="39" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B50" s="5" t="str">
         <f aca="false">A50</f>
         <v>Shxw'owhamel First Nation pronounced "Shwoh-hamel"</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="E50" s="13" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="G50" s="41" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="112.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="42" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="B51" s="5" t="str">
         <f aca="false">A51</f>
         <v>Shxwha:y Villiage</v>
       </c>
       <c r="C51" s="43" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="E51" s="13" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="F51" s="36"/>
       <c r="G51" s="44" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="212.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="34" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="B52" s="5" t="str">
         <f aca="false">A52</f>
         <v>Simpcw First Nation "People of the Rivers"</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="E52" s="13" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="F52" s="45" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="G52" s="45" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="17" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="B53" s="5" t="str">
         <f aca="false">A53</f>
         <v>Siska Indian Band</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="E53" s="13" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="H53" s="15"/>
     </row>
     <row r="54" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="17" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="B54" s="5" t="str">
         <f aca="false">A54</f>
         <v>Skuppah Indian Band</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="E54" s="13" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="H54" s="15"/>
     </row>
     <row r="55" customFormat="false" ht="136.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="17" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B55" s="5" t="str">
         <f aca="false">A55</f>
         <v>Skowkale First Nation</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="E55" s="13" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="124.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="19" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="B56" s="5" t="str">
         <f aca="false">A56</f>
         <v>Shuswap Indian Band</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="19" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B57" s="5" t="str">
         <f aca="false">A57</f>
         <v>Skawahlook First Nation</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="46" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="B58" s="5" t="str">
         <f aca="false">A58</f>
         <v>Skwah First Nation</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="153.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="14" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B59" s="5" t="str">
         <f aca="false">A59</f>
         <v>Snuneymuxw First Nation</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="147" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="19" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="B60" s="5" t="str">
         <f aca="false">A60</f>
         <v>Soowahlie First Nation</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="46" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="B61" s="5" t="str">
         <f aca="false">A61</f>
         <v>Spuzzum First Nation</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="192" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="47" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B62" s="5" t="str">
         <f aca="false">A62</f>
         <v>Squamish First Nation (Squ-Ho-0-meesh)</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="F62" s="10"/>
       <c r="G62" s="10" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="171" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="47" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B63" s="5" t="str">
         <f aca="false">A63</f>
         <v>Squiala First Nation</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="14" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="B64" s="5" t="str">
         <f aca="false">A64</f>
         <v>Stk'emlupsemc Te Secwepemc</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="D64" s="13" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="10" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="19" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="B65" s="5" t="str">
         <f aca="false">A65</f>
         <v>Sts'ailes Band (Chehalls Indian Band)</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="17" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="B66" s="5" t="str">
         <f aca="false">A66</f>
         <v>Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek) pronounced (St-wet-lem- hight-lem)</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="111" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="38" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="B67" s="5" t="str">
         <f aca="false">A67</f>
         <v>St'uxwtews (Bonaparte Indian Band) pronounced (Bone -eh-part)</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="159.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="34" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="B68" s="5" t="str">
         <f aca="false">A68</f>
         <v>Stz'uminus First Nation (ltst uw' hw-nuts'-ul-wun) Chemainus</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="19" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="B69" s="5" t="str">
         <f aca="false">A69</f>
         <v>Sumas First Nation</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="46" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="B70" s="5" t="str">
         <f aca="false">A70</f>
         <v>Toosey Indian Band (Tl'esqox)</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="H70" s="15"/>
     </row>
     <row r="71" customFormat="false" ht="211.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="14" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="B71" s="5" t="str">
         <f aca="false">A71</f>
         <v>Tsartlip First Nation</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="205.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="47" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="B72" s="5" t="str">
         <f aca="false">A72</f>
         <v>Tsawout First Nation</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="121.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="14" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="B73" s="5" t="str">
         <f aca="false">A73</f>
         <v>Tsawwassen First Nation</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="258" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="34" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="B74" s="5" t="str">
         <f aca="false">A74</f>
         <v>Ts'elxweyeqw Tribe Management Limited</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="F74" s="48" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="H74" s="11"/>
     </row>
     <row r="75" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="19" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="B75" s="5" t="str">
         <f aca="false">A75</f>
         <v>Tseycum First Nation</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="46" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="B76" s="5" t="str">
         <f aca="false">A76</f>
         <v>Ts'kwaylaxw (Pavillion Indian Band)</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="F76" s="10"/>
       <c r="G76" s="10" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="195" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="14" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="B77" s="5" t="str">
         <f aca="false">A77</f>
         <v>Tsleil Waututh Nation</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="148.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="14" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="B78" s="5" t="str">
         <f aca="false">A78</f>
         <v>T'Sou-ke Nation</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="139.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="19" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="B79" s="5" t="str">
         <f aca="false">A79</f>
         <v>Tk'emlups te Secwepemc</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="E79" s="49" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="F79" s="49" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="117.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="19" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="B80" s="5" t="str">
         <f aca="false">A80</f>
         <v>Tzeachten First Nation</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="199.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="19" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="B81" s="5" t="str">
         <f aca="false">A81</f>
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="D81" s="50" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="19" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="B82" s="5" t="str">
         <f aca="false">A82</f>
         <v>Union Bar First Nations</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="H82" s="15"/>
     </row>
     <row r="83" customFormat="false" ht="117.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="19" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="B83" s="5" t="str">
         <f aca="false">A83</f>
         <v>Upper Nicola Indian Band</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="F83" s="10"/>
       <c r="G83" s="10" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="46" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="B84" s="5" t="str">
         <f aca="false">A84</f>
         <v>Upper Similkameen Indian Band</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="D84" s="15" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="H84" s="15" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="341.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="14" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B85" s="5" t="str">
         <f aca="false">A85</f>
         <v>Whispering Pines/Clinton Indian Bands</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="341.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="51" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="B86" s="5" t="str">
         <f aca="false">A86</f>
@@ -4919,106 +4996,106 @@
     </row>
     <row r="87" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="14" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="B87" s="5" t="str">
         <f aca="false">A87</f>
         <v>Williams Lake Indian Band</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="D87" s="10"/>
       <c r="E87" s="10" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="F87" s="10"/>
       <c r="G87" s="10" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="19" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="B88" s="5" t="str">
         <f aca="false">A88</f>
         <v>Yakweakwioose First Nation</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="H88" s="15" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="19" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="B89" s="5" t="str">
         <f aca="false">A89</f>
         <v>Yale First Nation</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="E89" s="10" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="H89" s="11" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="129" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="19" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="B90" s="5" t="str">
         <f aca="false">A90</f>
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="E90" s="52" t="s">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="F90" s="10" t="s">
-        <v>554</v>
+        <v>560</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="H90" s="11" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5033,7 +5110,7 @@
     </row>
     <row r="92" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="19" t="s">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="B92" s="19"/>
       <c r="E92" s="57"/>
@@ -5042,7 +5119,7 @@
     </row>
     <row r="93" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="B93" s="10"/>
       <c r="E93" s="57"/>
@@ -5050,7 +5127,7 @@
     </row>
     <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>559</v>
+        <v>565</v>
       </c>
       <c r="B94" s="10"/>
       <c r="E94" s="57"/>
@@ -5058,7 +5135,7 @@
     </row>
     <row r="95" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="B95" s="10"/>
       <c r="E95" s="57"/>

</xml_diff>

<commit_message>
switched to es6 pattern and added some traditional territories
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="580">
   <si>
     <t xml:space="preserve">TRANSMOUNTAIN EXPANSION PROJECT - INDIGENOUS COMMUNITIES _IMC </t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aitchelitz Band (a-che-leetz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shxwháy Village</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Angie Bailey (June 4, 2010) Election: Hereditary - Custom</t>
@@ -540,6 +543,9 @@
     <t xml:space="preserve">Kwantlen First Nation (tireless Runner)</t>
   </si>
   <si>
+    <t xml:space="preserve">Kwantlen First Nation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Marilyn Gabriel (November 30, 1993) Councillors; Leslie Antone, Tumia Knott</t>
   </si>
   <si>
@@ -561,6 +567,9 @@
     <t xml:space="preserve">Kwaw -Kwaw-Aplit First Nations </t>
   </si>
   <si>
+    <t xml:space="preserve">Kwaw-Kwaw-Aplit First Nations</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Randy Leon - next election August 24, 2022</t>
   </si>
   <si>
@@ -598,6 +607,9 @@
   </si>
   <si>
     <t xml:space="preserve">Leq' a: mel First Nation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leq'amel First Nation</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Alice Thompson - next election March 2025 </t>
@@ -621,6 +633,9 @@
     <t xml:space="preserve">Little Shuswap Lake Indian Band (Skwlax meaning "Black Bear")</t>
   </si>
   <si>
+    <t xml:space="preserve">Little Shuswap Lake Indian Band</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Oliver Arnouse - next election October 23, 2021</t>
   </si>
   <si>
@@ -642,6 +657,9 @@
     <t xml:space="preserve">Lheidli T'enneh First Nation</t>
   </si>
   <si>
+    <t xml:space="preserve">Lheidli Tenneh First Nation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Dolleen Logan - next election April 09, 2023</t>
   </si>
   <si>
@@ -682,6 +700,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lower Nicola Indian Band -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower Nicola Indian Band</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Stuart Jackson - next election September 30, 2022</t>
@@ -706,6 +727,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lower Similkameen #598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LowerSimilkameen598</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Keith Crow - next election December 6, 2021. Councillor Janet Terbasket December 6, 2021, Councillors; Ira Edward, John Louie November 04, 2023</t>
@@ -791,6 +815,9 @@
     <t xml:space="preserve">Musqeam Indian Band</t>
   </si>
   <si>
+    <t xml:space="preserve">Musqueam Indian Band</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Wayne Sparrow - next election Nov 30, 2024</t>
   </si>
   <si>
@@ -933,6 +960,9 @@
     <t xml:space="preserve">Peters Band (Peters First Nation)</t>
   </si>
   <si>
+    <t xml:space="preserve">Peters Band</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Norma Jean Webb - next election December 22, 2021</t>
   </si>
   <si>
@@ -1005,6 +1035,9 @@
   </si>
   <si>
     <t xml:space="preserve">Scia'new First Nation (Beecher Bay First Nation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sc'ia'new First Nation</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Russ Chipps - next election: October 8, 2023</t>
@@ -1133,6 +1166,9 @@
     <t xml:space="preserve">Shxw'owhamel First Nation pronounced "Shwoh-hamel"</t>
   </si>
   <si>
+    <t xml:space="preserve">Shxw'owhamel First Nation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Leaders are called Si:yá:m. The Si:yá:m government/council system provides all families equal representation at the Council table level.  June 18, 2010,   Si:yam  Melody Andrews, Lucille Casimir, Lenora Fraser, Alfred James, Dean Jones, Lenona Kelly, Sonny Mchalsie, , Louise Mussell, Brenda Peters, Shawna Peters, Irene Smith</t>
   </si>
   <si>
@@ -1176,6 +1212,9 @@
   </si>
   <si>
     <t xml:space="preserve">Simpcw First Nation "People of the Rivers"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simpcw First Nation</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Shelly Ann Loring - next election May 31, 2024. Councillors; Edward (Eddie) Celesta, Christine (Tina) Donald, Lori Eustache, Alison Eustache (Green), George Lampreau, Ronald (Ron Jr.)  Lampreau, </t>
@@ -1972,7 +2011,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2011,12 +2050,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
@@ -2046,11 +2079,24 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF4D415C"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2321,11 +2367,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2350,10 +2396,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2370,7 +2412,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2378,119 +2420,127 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2498,15 +2548,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2522,11 +2572,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2550,7 +2600,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2642,8 +2692,8 @@
   </sheetPr>
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2697,29 +2747,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="110.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="2" t="n">
@@ -2729,64 +2779,63 @@
         <v>-120.076953</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="140.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+    <row r="4" customFormat="false" ht="40.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5" t="str">
-        <f aca="false">A4</f>
-        <v>Aitchelitz Band (a-che-leetz)</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="G4" s="9" t="s">
         <v>25</v>
       </c>
+      <c r="H4" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="I4" s="0" t="n">
-        <v>49.065977</v>
+        <v>49.087557</v>
       </c>
       <c r="J4" s="0" t="n">
-        <v>-121.888063</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>26</v>
+        <v>-121.829723</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="21.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B5" s="5" t="str">
         <f aca="false">A5</f>
         <v>Ashcroft Indian Band</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="G5" s="9" t="s">
         <v>32</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>50.404267</v>
@@ -2795,31 +2844,31 @@
         <v>-120.678195</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="5" t="str">
         <f aca="false">A6</f>
         <v>Boothroyd Band</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="E6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="F6" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="G6" s="9" t="s">
         <v>39</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>49.963059</v>
@@ -2828,30 +2877,30 @@
         <v>-121.484624</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="110.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7" s="5" t="str">
         <f aca="false">A7</f>
         <v>Boston Bar First Nations</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="F7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="15"/>
+      <c r="G7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="14"/>
       <c r="I7" s="0" t="n">
         <v>49.621761</v>
       </c>
@@ -2859,30 +2908,30 @@
         <v>-120.95154</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="165" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>46</v>
+    <row r="8" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="C8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="17" t="s">
         <v>53</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>51.770937</v>
@@ -2892,29 +2941,29 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="131.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
-        <v>54</v>
+      <c r="A9" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="F9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="G9" s="9" t="s">
         <v>61</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>49.283272</v>
@@ -2925,28 +2974,28 @@
     </row>
     <row r="10" customFormat="false" ht="134.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="F10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>68</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>49.540481</v>
@@ -2956,29 +3005,29 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="180" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>69</v>
+      <c r="A11" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="D11" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="F11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>75</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>50.027994</v>
@@ -2988,29 +3037,29 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
-        <v>76</v>
+      <c r="A12" s="16" t="s">
+        <v>77</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="D12" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="E12" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="F12" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="G12" s="9" t="s">
         <v>83</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>50.032193</v>
@@ -3020,29 +3069,29 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="205.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19" t="s">
-        <v>84</v>
+      <c r="A13" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="G13" s="12" t="s">
         <v>90</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>48.888822</v>
@@ -3052,29 +3101,29 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="159.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
-        <v>91</v>
+      <c r="A14" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="D14" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="E14" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="G14" s="9" t="s">
         <v>98</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>48.890317</v>
@@ -3084,29 +3133,29 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="s">
-        <v>99</v>
+      <c r="A15" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C15" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="D15" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G15" s="10" t="s">
+      <c r="E15" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="F15" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>105</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>48.688573</v>
@@ -3116,30 +3165,30 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="191.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
-        <v>106</v>
+      <c r="A16" s="18" t="s">
+        <v>107</v>
       </c>
       <c r="B16" s="5" t="str">
         <f aca="false">A16</f>
         <v>Halalt First Nation</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="D16" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="E16" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="G16" s="9" t="s">
         <v>112</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>48.929783</v>
@@ -3149,26 +3198,26 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19" t="s">
-        <v>113</v>
+      <c r="A17" s="18" t="s">
+        <v>114</v>
       </c>
       <c r="B17" s="5" t="str">
         <f aca="false">A17</f>
         <v>Heiltsuk First Nation</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="13" t="s">
+      <c r="C17" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="10" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="F17" s="19"/>
+      <c r="G17" s="9" t="s">
         <v>117</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>52.337794</v>
@@ -3178,30 +3227,30 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="126" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="s">
-        <v>118</v>
+      <c r="A18" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="B18" s="5" t="str">
         <f aca="false">A18</f>
         <v>Huu-ay-aht First Nation</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="D18" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="10" t="s">
+      <c r="E18" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="F18" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>123</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>48.833479</v>
@@ -3212,28 +3261,28 @@
     </row>
     <row r="19" customFormat="false" ht="165.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B19" s="5" t="str">
         <f aca="false">A19</f>
         <v>Katzie First Nation</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="G19" s="13" t="s">
+      <c r="E19" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="H19" s="11"/>
+      <c r="F19" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="10"/>
       <c r="I19" s="0" t="n">
         <v>49.557619</v>
       </c>
@@ -3242,712 +3291,850 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" s="5" t="str">
-        <f aca="false">A20</f>
-        <v>Kwantlen First Nation (tireless Runner)</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="A20" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="B20" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="C20" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="D20" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="E20" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="F20" s="12" t="s">
         <v>135</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>49.476845</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>-122.296959</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="160.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="B21" s="5" t="str">
-        <f aca="false">A21</f>
-        <v>Kwaw -Kwaw-Aplit First Nations</v>
+        <v>138</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>139</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="F21" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="D21" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="H21" s="15"/>
+      <c r="E21" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="14"/>
+      <c r="I21" s="0" t="n">
+        <v>49.516226</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>-121.756432</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B22" s="5" t="str">
         <f aca="false">A22</f>
         <v>Kwikwetlem First Nation</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="G22" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="E22" s="12" t="s">
         <v>148</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>49.451741</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>-122.657791</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <f aca="false">A23</f>
-        <v>Leq' a: mel First Nation</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="F23" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="G23" s="10" t="s">
+      <c r="B23" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="I23" s="10"/>
+      <c r="D23" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" s="9" t="n">
+        <v>49.348358</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>-122.106774</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="B24" s="5" t="str">
-        <f aca="false">A24</f>
-        <v>Little Shuswap Lake Indian Band (Skwlax meaning "Black Bear")</v>
+        <v>159</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>160</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="H24" s="15" t="s">
         <v>161</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>51.287872</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>-118.990533</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="195" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="B25" s="5" t="str">
-        <f aca="false">A25</f>
-        <v>Lheidli T'enneh First Nation</v>
+        <v>167</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>53.944696</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>-121.694171</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="174.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>169</v>
+      <c r="A26" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="B26" s="5" t="str">
         <f aca="false">A26</f>
         <v>Lhtako Dene Nation</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>175</v>
+      <c r="C26" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>52.953049</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>-122.449172</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="195" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="B27" s="5" t="str">
-        <f aca="false">A27</f>
-        <v>Lower Nicola Indian Band -</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="H27" s="11" t="s">
+      <c r="A27" s="18" t="s">
         <v>182</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>50.006984</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>-121.261538</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28" s="5" t="str">
-        <f aca="false">A28</f>
-        <v>Lower Similkameen #598</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="H28" s="15"/>
+        <v>190</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H28" s="14"/>
+      <c r="I28" s="0" t="n">
+        <v>49.845148</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>-118.987733</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="29" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B29" s="5" t="str">
         <f aca="false">A29</f>
         <v>Lyackson First Nation</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>195</v>
+      <c r="C29" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>48.941803</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>-123.490134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="126.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14" t="s">
-        <v>196</v>
+      <c r="A30" s="13" t="s">
+        <v>204</v>
       </c>
       <c r="B30" s="5" t="str">
         <f aca="false">A30</f>
         <v>Malahat First Nation</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>201</v>
+      <c r="C30" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>48.655944</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>-124.000524</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="30" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B31" s="5" t="str">
         <f aca="false">A31</f>
         <v>Matsqui First Nation</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="H31" s="15"/>
+      <c r="C31" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="0" t="n">
+        <v>49.290611</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>-122.361868</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="B32" s="5" t="str">
-        <f aca="false">A32</f>
-        <v>Musqeam Indian Band</v>
+      <c r="A32" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>209</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>214</v>
+        <v>218</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>49.353225</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>-123.012956</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
-        <v>215</v>
+      <c r="A33" s="13" t="s">
+        <v>224</v>
       </c>
       <c r="B33" s="5" t="str">
         <f aca="false">A33</f>
         <v>Neskonlith Indian Band</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>220</v>
+      <c r="C33" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>51.21274</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>-118.846623</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
-        <v>221</v>
+      <c r="A34" s="13" t="s">
+        <v>230</v>
       </c>
       <c r="B34" s="5" t="str">
         <f aca="false">A34</f>
         <v>Nooaitch Indian Band</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>227</v>
+      <c r="C34" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>49.690318</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>-120.648292</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="32" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B35" s="5" t="str">
         <f aca="false">A35</f>
         <v>Osoyoos</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>231</v>
+      <c r="C35" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>240</v>
       </c>
       <c r="F35" s="33"/>
-      <c r="G35" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>233</v>
+      <c r="G35" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>49.114526</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>-118.489264</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="14" t="s">
-        <v>234</v>
+      <c r="A36" s="13" t="s">
+        <v>243</v>
       </c>
       <c r="B36" s="5" t="str">
         <f aca="false">A36</f>
         <v>Pacheedaht First Nation</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>239</v>
+      <c r="C36" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>48.572918</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>-124.39459</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14" t="s">
-        <v>240</v>
+      <c r="A37" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="B37" s="5" t="str">
         <f aca="false">A37</f>
         <v>Pauquachin Nation</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="H37" s="15"/>
+      <c r="C37" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H37" s="14"/>
+      <c r="I37" s="0" t="n">
+        <v>48.724102</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>-123.324246</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14" t="s">
-        <v>246</v>
+      <c r="A38" s="13" t="s">
+        <v>255</v>
       </c>
       <c r="B38" s="5" t="str">
         <f aca="false">A38</f>
         <v>Penticton Indian Band</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>251</v>
+      <c r="C38" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>49.732366</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>-119.25376</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="B39" s="5" t="str">
-        <f aca="false">A39</f>
-        <v>Peters Band (Peters First Nation)</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>257</v>
+      <c r="A39" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>49.505163</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>-121.482617</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14" t="s">
-        <v>258</v>
+      <c r="A40" s="13" t="s">
+        <v>268</v>
       </c>
       <c r="B40" s="5" t="str">
         <f aca="false">A40</f>
         <v>Penelakut Tribe</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>263</v>
+      <c r="C40" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>48.892388</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>-123.675652</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14" t="s">
-        <v>264</v>
+      <c r="A41" s="13" t="s">
+        <v>274</v>
       </c>
       <c r="B41" s="5" t="str">
         <f aca="false">A41</f>
         <v>Popkum First Nation</v>
       </c>
-      <c r="C41" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="H41" s="15"/>
+      <c r="C41" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="H41" s="14"/>
+      <c r="I41" s="0" t="n">
+        <v>49.57071</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>-121.506875</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="127.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
-        <v>269</v>
+      <c r="A42" s="13" t="s">
+        <v>279</v>
       </c>
       <c r="B42" s="5" t="str">
         <f aca="false">A42</f>
         <v>Qayqayt First Nation (New Westminister)</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="H42" s="15"/>
+      <c r="C42" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="H42" s="14"/>
     </row>
     <row r="43" customFormat="false" ht="98.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="34" t="s">
-        <v>274</v>
-      </c>
-      <c r="B43" s="5" t="str">
-        <f aca="false">A43</f>
-        <v>Scia'new First Nation (Beecher Bay First Nation)</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>280</v>
+        <v>284</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>48.440888</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>-123.676887</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="35" t="s">
-        <v>281</v>
-      </c>
-      <c r="B44" s="5" t="str">
-        <f aca="false">A44</f>
-        <v>Sq'ewlets (Scowlitz) First Nation</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>287</v>
+        <v>292</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>49.25517</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>-121.964821</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="34" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="B45" s="5" t="str">
         <f aca="false">A45</f>
         <v>Seabird Island Band</v>
       </c>
-      <c r="C45" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="H45" s="15"/>
+      <c r="C45" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="H45" s="14"/>
+      <c r="I45" s="0" t="n">
+        <v>49.262475</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>-121.724003</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="151.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="17" t="s">
-        <v>293</v>
+      <c r="A46" s="16" t="s">
+        <v>304</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C46" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="D46" s="13"/>
+      <c r="C46" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D46" s="12"/>
       <c r="E46" s="36" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="F46" s="36"/>
       <c r="G46" s="37" t="s">
-        <v>296</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>297</v>
+        <v>307</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>308</v>
       </c>
       <c r="I46" s="2" t="n">
         <v>51.527017</v>
@@ -3957,1195 +4144,1249 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="286.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="17" t="s">
-        <v>298</v>
+      <c r="A47" s="16" t="s">
+        <v>309</v>
       </c>
       <c r="B47" s="5" t="str">
         <f aca="false">A47</f>
         <v>Semiahmoo First Nation</v>
       </c>
-      <c r="C47" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="F47" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="H47" s="15"/>
+      <c r="C47" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="H47" s="14"/>
+      <c r="I47" s="0" t="n">
+        <v>49.012447</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>-122.767315</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="38" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="B48" s="5" t="str">
         <f aca="false">A48</f>
         <v>Sexqeltqin (Adams Lake Indian Band)</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="F48" s="10" t="s">
+      <c r="E48" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F48" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="15" t="s">
-        <v>305</v>
+      <c r="H48" s="14" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="111.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="34" t="s">
-        <v>306</v>
-      </c>
-      <c r="B49" s="5" t="str">
-        <f aca="false">A49</f>
-        <v>Shackan Indian Band</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>309</v>
+        <v>317</v>
+      </c>
+      <c r="B49" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>320</v>
       </c>
       <c r="F49" s="36"/>
-      <c r="G49" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>311</v>
+      <c r="G49" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>49.963059</v>
+      </c>
+      <c r="J49" s="0" t="n">
+        <v>-121.484624</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="183" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="39" t="s">
-        <v>312</v>
-      </c>
-      <c r="B50" s="5" t="str">
-        <f aca="false">A50</f>
-        <v>Shxw'owhamel First Nation pronounced "Shwoh-hamel"</v>
-      </c>
-      <c r="C50" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="F50" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="G50" s="41" t="s">
-        <v>317</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>318</v>
+      <c r="A50" s="40" t="s">
+        <v>323</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C50" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="G50" s="42" t="s">
+        <v>329</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>49.339668</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>-121.60638</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="112.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="42" t="s">
-        <v>319</v>
-      </c>
-      <c r="B51" s="5" t="str">
-        <f aca="false">A51</f>
-        <v>Shxwha:y Villiage</v>
-      </c>
-      <c r="C51" s="43" t="s">
-        <v>320</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>322</v>
+      <c r="A51" s="43" t="s">
+        <v>331</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>334</v>
       </c>
       <c r="F51" s="36"/>
-      <c r="G51" s="44" t="s">
-        <v>323</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>324</v>
+      <c r="G51" s="45" t="s">
+        <v>335</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>49.087557</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>-121.829723</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="212.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="34" t="s">
-        <v>325</v>
-      </c>
-      <c r="B52" s="5" t="str">
-        <f aca="false">A52</f>
-        <v>Simpcw First Nation "People of the Rivers"</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>328</v>
-      </c>
-      <c r="F52" s="45" t="s">
-        <v>327</v>
-      </c>
-      <c r="G52" s="45" t="s">
-        <v>329</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>330</v>
+        <v>337</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="F52" s="46" t="s">
+        <v>340</v>
+      </c>
+      <c r="G52" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>52.634393</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>-119.699777</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="17" t="s">
-        <v>331</v>
+      <c r="A53" s="16" t="s">
+        <v>344</v>
       </c>
       <c r="B53" s="5" t="str">
         <f aca="false">A53</f>
         <v>Siska Indian Band</v>
       </c>
-      <c r="C53" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="F53" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="H53" s="15"/>
+      <c r="C53" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="H53" s="14"/>
+      <c r="I53" s="0" t="n">
+        <v>50.117565</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>-120.838519</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="17" t="s">
-        <v>337</v>
-      </c>
-      <c r="B54" s="5" t="str">
-        <f aca="false">A54</f>
-        <v>Skuppah Indian Band</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="F54" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="H54" s="15"/>
+      <c r="A54" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="B54" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>352</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="H54" s="14"/>
+      <c r="I54" s="0" t="n">
+        <v>49.963059</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>-121.484624</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="136.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="B55" s="5" t="str">
-        <f aca="false">A55</f>
-        <v>Skowkale First Nation</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="E55" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="F55" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>348</v>
+      <c r="A55" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>358</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>49.087557</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <v>-121.829723</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="124.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="19" t="s">
-        <v>349</v>
+      <c r="A56" s="18" t="s">
+        <v>362</v>
       </c>
       <c r="B56" s="5" t="str">
         <f aca="false">A56</f>
         <v>Shuswap Indian Band</v>
       </c>
-      <c r="C56" s="13" t="s">
-        <v>350</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="G56" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="H56" s="11" t="s">
-        <v>355</v>
+      <c r="C56" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>50.367907</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <v>-116.89554</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="19" t="s">
-        <v>356</v>
+      <c r="A57" s="18" t="s">
+        <v>369</v>
       </c>
       <c r="B57" s="5" t="str">
         <f aca="false">A57</f>
         <v>Skawahlook First Nation</v>
       </c>
-      <c r="C57" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="G57" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="H57" s="11" t="s">
-        <v>361</v>
+      <c r="C57" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>49.227586</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>-122.174045</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="46" t="s">
-        <v>362</v>
+      <c r="A58" s="47" t="s">
+        <v>375</v>
       </c>
       <c r="B58" s="5" t="str">
         <f aca="false">A58</f>
         <v>Skwah First Nation</v>
       </c>
-      <c r="C58" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="G58" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="H58" s="11" t="s">
-        <v>367</v>
+      <c r="C58" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="153.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="14" t="s">
-        <v>368</v>
+      <c r="A59" s="13" t="s">
+        <v>381</v>
       </c>
       <c r="B59" s="5" t="str">
         <f aca="false">A59</f>
         <v>Snuneymuxw First Nation</v>
       </c>
-      <c r="C59" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>373</v>
+      <c r="C59" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="147" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="19" t="s">
-        <v>374</v>
+      <c r="A60" s="18" t="s">
+        <v>387</v>
       </c>
       <c r="B60" s="5" t="str">
         <f aca="false">A60</f>
         <v>Soowahlie First Nation</v>
       </c>
-      <c r="C60" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="D60" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="G60" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>379</v>
+      <c r="C60" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>389</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>389</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="46" t="s">
-        <v>380</v>
+      <c r="A61" s="47" t="s">
+        <v>393</v>
       </c>
       <c r="B61" s="5" t="str">
         <f aca="false">A61</f>
         <v>Spuzzum First Nation</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>381</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>382</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>384</v>
-      </c>
-      <c r="G61" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>386</v>
+      <c r="C61" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="192" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="47" t="s">
-        <v>387</v>
+      <c r="A62" s="48" t="s">
+        <v>400</v>
       </c>
       <c r="B62" s="5" t="str">
         <f aca="false">A62</f>
         <v>Squamish First Nation (Squ-Ho-0-meesh)</v>
       </c>
-      <c r="C62" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>389</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="H62" s="11" t="s">
-        <v>392</v>
+      <c r="C62" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="171" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="47" t="s">
-        <v>393</v>
+      <c r="A63" s="48" t="s">
+        <v>406</v>
       </c>
       <c r="B63" s="5" t="str">
         <f aca="false">A63</f>
         <v>Squiala First Nation</v>
       </c>
-      <c r="C63" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>397</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>398</v>
+      <c r="C63" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="14" t="s">
-        <v>399</v>
+      <c r="A64" s="13" t="s">
+        <v>412</v>
       </c>
       <c r="B64" s="5" t="str">
         <f aca="false">A64</f>
         <v>Stk'emlupsemc Te Secwepemc</v>
       </c>
-      <c r="C64" s="16" t="s">
-        <v>400</v>
-      </c>
-      <c r="D64" s="13" t="s">
-        <v>401</v>
-      </c>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="G64" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="H64" s="11" t="s">
-        <v>404</v>
+      <c r="C64" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="19" t="s">
-        <v>405</v>
+      <c r="A65" s="18" t="s">
+        <v>418</v>
       </c>
       <c r="B65" s="5" t="str">
         <f aca="false">A65</f>
         <v>Sts'ailes Band (Chehalls Indian Band)</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>407</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>407</v>
-      </c>
-      <c r="G65" s="10" t="s">
-        <v>409</v>
-      </c>
-      <c r="H65" s="11" t="s">
-        <v>410</v>
+      <c r="C65" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="17" t="s">
-        <v>411</v>
+      <c r="A66" s="16" t="s">
+        <v>424</v>
       </c>
       <c r="B66" s="5" t="str">
         <f aca="false">A66</f>
         <v>Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek) pronounced (St-wet-lem- hight-lem)</v>
       </c>
-      <c r="C66" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="F66" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="G66" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="H66" s="11" t="s">
-        <v>417</v>
+      <c r="C66" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="111" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="38" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="B67" s="5" t="str">
         <f aca="false">A67</f>
         <v>St'uxwtews (Bonaparte Indian Band) pronounced (Bone -eh-part)</v>
       </c>
-      <c r="C67" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="E67" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>423</v>
+      <c r="C67" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="159.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="34" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="B68" s="5" t="str">
         <f aca="false">A68</f>
         <v>Stz'uminus First Nation (ltst uw' hw-nuts'-ul-wun) Chemainus</v>
       </c>
-      <c r="C68" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="F68" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="H68" s="11" t="s">
-        <v>429</v>
+      <c r="C68" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="H68" s="10" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="19" t="s">
-        <v>430</v>
+      <c r="A69" s="18" t="s">
+        <v>443</v>
       </c>
       <c r="B69" s="5" t="str">
         <f aca="false">A69</f>
         <v>Sumas First Nation</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>431</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="F69" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="G69" s="10" t="s">
-        <v>434</v>
-      </c>
-      <c r="H69" s="11" t="s">
-        <v>435</v>
+        <v>444</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="46" t="s">
-        <v>436</v>
+      <c r="A70" s="47" t="s">
+        <v>449</v>
       </c>
       <c r="B70" s="5" t="str">
         <f aca="false">A70</f>
         <v>Toosey Indian Band (Tl'esqox)</v>
       </c>
-      <c r="C70" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="F70" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="G70" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="H70" s="15"/>
+      <c r="C70" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="H70" s="14"/>
     </row>
     <row r="71" customFormat="false" ht="211.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="14" t="s">
-        <v>441</v>
+      <c r="A71" s="13" t="s">
+        <v>454</v>
       </c>
       <c r="B71" s="5" t="str">
         <f aca="false">A71</f>
         <v>Tsartlip First Nation</v>
       </c>
-      <c r="C71" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="F71" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="G71" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="H71" s="11" t="s">
-        <v>446</v>
+      <c r="C71" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="205.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="47" t="s">
-        <v>447</v>
+      <c r="A72" s="48" t="s">
+        <v>460</v>
       </c>
       <c r="B72" s="5" t="str">
         <f aca="false">A72</f>
         <v>Tsawout First Nation</v>
       </c>
-      <c r="C72" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="G72" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="H72" s="11" t="s">
-        <v>452</v>
+      <c r="C72" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="121.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="14" t="s">
-        <v>453</v>
+      <c r="A73" s="13" t="s">
+        <v>466</v>
       </c>
       <c r="B73" s="5" t="str">
         <f aca="false">A73</f>
         <v>Tsawwassen First Nation</v>
       </c>
-      <c r="C73" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>455</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>456</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>457</v>
-      </c>
-      <c r="G73" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="H73" s="11" t="s">
-        <v>459</v>
+      <c r="C73" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H73" s="10" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="258" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="34" t="s">
-        <v>460</v>
+        <v>473</v>
       </c>
       <c r="B74" s="5" t="str">
         <f aca="false">A74</f>
         <v>Ts'elxweyeqw Tribe Management Limited</v>
       </c>
-      <c r="C74" s="10" t="s">
-        <v>461</v>
-      </c>
-      <c r="D74" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>463</v>
-      </c>
-      <c r="F74" s="48" t="s">
-        <v>464</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="H74" s="11"/>
+      <c r="C74" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="F74" s="49" t="s">
+        <v>477</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="H74" s="10"/>
     </row>
     <row r="75" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="19" t="s">
-        <v>466</v>
+      <c r="A75" s="18" t="s">
+        <v>479</v>
       </c>
       <c r="B75" s="5" t="str">
         <f aca="false">A75</f>
         <v>Tseycum First Nation</v>
       </c>
-      <c r="C75" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="D75" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>469</v>
-      </c>
-      <c r="F75" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="G75" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="H75" s="11" t="s">
-        <v>472</v>
+      <c r="C75" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="46" t="s">
-        <v>473</v>
+      <c r="A76" s="47" t="s">
+        <v>486</v>
       </c>
       <c r="B76" s="5" t="str">
         <f aca="false">A76</f>
         <v>Ts'kwaylaxw (Pavillion Indian Band)</v>
       </c>
-      <c r="C76" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="D76" s="10" t="s">
-        <v>475</v>
-      </c>
-      <c r="E76" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10" t="s">
-        <v>477</v>
+      <c r="C76" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="195" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="14" t="s">
-        <v>478</v>
+      <c r="A77" s="13" t="s">
+        <v>491</v>
       </c>
       <c r="B77" s="5" t="str">
         <f aca="false">A77</f>
         <v>Tsleil Waututh Nation</v>
       </c>
-      <c r="C77" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>480</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="F77" s="10" t="s">
-        <v>480</v>
-      </c>
-      <c r="G77" s="10" t="s">
-        <v>482</v>
-      </c>
-      <c r="H77" s="11" t="s">
-        <v>483</v>
+      <c r="C77" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>495</v>
+      </c>
+      <c r="H77" s="10" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="148.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="14" t="s">
-        <v>484</v>
+      <c r="A78" s="13" t="s">
+        <v>497</v>
       </c>
       <c r="B78" s="5" t="str">
         <f aca="false">A78</f>
         <v>T'Sou-ke Nation</v>
       </c>
-      <c r="C78" s="10" t="s">
-        <v>485</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>486</v>
-      </c>
-      <c r="E78" s="13" t="s">
-        <v>487</v>
-      </c>
-      <c r="F78" s="13" t="s">
-        <v>488</v>
-      </c>
-      <c r="G78" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="H78" s="11" t="s">
-        <v>490</v>
+      <c r="C78" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="F78" s="12" t="s">
+        <v>501</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="139.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="19" t="s">
-        <v>491</v>
+      <c r="A79" s="18" t="s">
+        <v>504</v>
       </c>
       <c r="B79" s="5" t="str">
         <f aca="false">A79</f>
         <v>Tk'emlups te Secwepemc</v>
       </c>
-      <c r="C79" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="D79" s="10" t="s">
-        <v>493</v>
-      </c>
-      <c r="E79" s="49" t="s">
-        <v>494</v>
-      </c>
-      <c r="F79" s="49" t="s">
-        <v>495</v>
-      </c>
-      <c r="G79" s="10" t="s">
-        <v>496</v>
-      </c>
-      <c r="H79" s="11" t="s">
-        <v>497</v>
+      <c r="C79" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="E79" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="F79" s="50" t="s">
+        <v>508</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="H79" s="10" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="117.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="19" t="s">
-        <v>498</v>
+      <c r="A80" s="18" t="s">
+        <v>511</v>
       </c>
       <c r="B80" s="5" t="str">
         <f aca="false">A80</f>
         <v>Tzeachten First Nation</v>
       </c>
-      <c r="C80" s="10" t="s">
-        <v>499</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>500</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>501</v>
-      </c>
-      <c r="F80" s="10" t="s">
-        <v>502</v>
-      </c>
-      <c r="G80" s="10" t="s">
-        <v>503</v>
-      </c>
-      <c r="H80" s="11" t="s">
-        <v>504</v>
+      <c r="C80" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>514</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="H80" s="10" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="199.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="19" t="s">
-        <v>505</v>
+      <c r="A81" s="18" t="s">
+        <v>518</v>
       </c>
       <c r="B81" s="5" t="str">
         <f aca="false">A81</f>
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
-      <c r="C81" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="D81" s="50" t="s">
-        <v>507</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>508</v>
-      </c>
-      <c r="F81" s="10" t="s">
-        <v>509</v>
-      </c>
-      <c r="G81" s="10" t="s">
-        <v>510</v>
-      </c>
-      <c r="H81" s="11" t="s">
-        <v>511</v>
+      <c r="C81" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="D81" s="51" t="s">
+        <v>520</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="H81" s="10" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="19" t="s">
-        <v>512</v>
+      <c r="A82" s="18" t="s">
+        <v>525</v>
       </c>
       <c r="B82" s="5" t="str">
         <f aca="false">A82</f>
         <v>Union Bar First Nations</v>
       </c>
-      <c r="C82" s="10" t="s">
-        <v>513</v>
-      </c>
-      <c r="D82" s="10" t="s">
-        <v>514</v>
-      </c>
-      <c r="E82" s="10" t="s">
-        <v>515</v>
-      </c>
-      <c r="F82" s="10" t="s">
-        <v>516</v>
-      </c>
-      <c r="G82" s="10" t="s">
-        <v>517</v>
-      </c>
-      <c r="H82" s="15"/>
+      <c r="C82" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>527</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="H82" s="14"/>
     </row>
     <row r="83" customFormat="false" ht="117.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="19" t="s">
-        <v>518</v>
+      <c r="A83" s="18" t="s">
+        <v>531</v>
       </c>
       <c r="B83" s="5" t="str">
         <f aca="false">A83</f>
         <v>Upper Nicola Indian Band</v>
       </c>
-      <c r="C83" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="D83" s="10" t="s">
-        <v>520</v>
-      </c>
-      <c r="E83" s="10" t="s">
-        <v>521</v>
-      </c>
-      <c r="F83" s="10"/>
-      <c r="G83" s="10" t="s">
-        <v>522</v>
-      </c>
-      <c r="H83" s="11" t="s">
-        <v>523</v>
+      <c r="C83" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="H83" s="10" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="46" t="s">
-        <v>524</v>
+      <c r="A84" s="47" t="s">
+        <v>537</v>
       </c>
       <c r="B84" s="5" t="str">
         <f aca="false">A84</f>
         <v>Upper Similkameen Indian Band</v>
       </c>
-      <c r="C84" s="10" t="s">
-        <v>525</v>
-      </c>
-      <c r="D84" s="15" t="s">
-        <v>526</v>
-      </c>
-      <c r="E84" s="10" t="s">
-        <v>527</v>
-      </c>
-      <c r="F84" s="15" t="s">
-        <v>526</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>528</v>
-      </c>
-      <c r="H84" s="15" t="s">
-        <v>529</v>
+      <c r="C84" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>539</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="H84" s="14" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="341.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="14" t="s">
-        <v>530</v>
+      <c r="A85" s="13" t="s">
+        <v>543</v>
       </c>
       <c r="B85" s="5" t="str">
         <f aca="false">A85</f>
         <v>Whispering Pines/Clinton Indian Bands</v>
       </c>
-      <c r="C85" s="10" t="s">
-        <v>531</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>532</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>533</v>
-      </c>
-      <c r="F85" s="10" t="s">
-        <v>532</v>
-      </c>
-      <c r="G85" s="10" t="s">
-        <v>534</v>
-      </c>
-      <c r="H85" s="11" t="s">
-        <v>535</v>
+      <c r="C85" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="341.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="51" t="s">
-        <v>536</v>
+      <c r="A86" s="52" t="s">
+        <v>549</v>
       </c>
       <c r="B86" s="5" t="str">
         <f aca="false">A86</f>
         <v>Whispering Pines/Clinton Indian Bands  - Continued</v>
       </c>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="10"/>
-      <c r="H86" s="11"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="H86" s="10"/>
     </row>
     <row r="87" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="14" t="s">
-        <v>537</v>
+      <c r="A87" s="13" t="s">
+        <v>550</v>
       </c>
       <c r="B87" s="5" t="str">
         <f aca="false">A87</f>
         <v>Williams Lake Indian Band</v>
       </c>
-      <c r="C87" s="10" t="s">
-        <v>538</v>
-      </c>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10" t="s">
-        <v>539</v>
-      </c>
-      <c r="F87" s="10"/>
-      <c r="G87" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="H87" s="11" t="s">
-        <v>541</v>
+      <c r="C87" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="H87" s="10" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="19" t="s">
-        <v>542</v>
+      <c r="A88" s="18" t="s">
+        <v>555</v>
       </c>
       <c r="B88" s="5" t="str">
         <f aca="false">A88</f>
         <v>Yakweakwioose First Nation</v>
       </c>
-      <c r="C88" s="10" t="s">
-        <v>543</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>545</v>
-      </c>
-      <c r="F88" s="10" t="s">
-        <v>546</v>
-      </c>
-      <c r="G88" s="10" t="s">
-        <v>547</v>
-      </c>
-      <c r="H88" s="15" t="s">
-        <v>548</v>
+      <c r="C88" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="H88" s="14" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="19" t="s">
-        <v>549</v>
+      <c r="A89" s="18" t="s">
+        <v>562</v>
       </c>
       <c r="B89" s="5" t="str">
         <f aca="false">A89</f>
         <v>Yale First Nation</v>
       </c>
-      <c r="C89" s="10" t="s">
-        <v>550</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>551</v>
-      </c>
-      <c r="E89" s="10" t="s">
-        <v>552</v>
-      </c>
-      <c r="F89" s="10" t="s">
-        <v>553</v>
-      </c>
-      <c r="G89" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="H89" s="11" t="s">
-        <v>555</v>
+      <c r="C89" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="H89" s="10" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="129" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="19" t="s">
-        <v>556</v>
+      <c r="A90" s="18" t="s">
+        <v>569</v>
       </c>
       <c r="B90" s="5" t="str">
         <f aca="false">A90</f>
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
-      <c r="C90" s="10" t="s">
-        <v>557</v>
-      </c>
-      <c r="D90" s="10" t="s">
-        <v>558</v>
-      </c>
-      <c r="E90" s="52" t="s">
-        <v>559</v>
-      </c>
-      <c r="F90" s="10" t="s">
-        <v>560</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>561</v>
-      </c>
-      <c r="H90" s="11" t="s">
-        <v>562</v>
+      <c r="C90" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="E90" s="53" t="s">
+        <v>572</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="53"/>
-      <c r="B91" s="53"/>
-      <c r="C91" s="54"/>
-      <c r="D91" s="54"/>
-      <c r="E91" s="55"/>
-      <c r="F91" s="55"/>
-      <c r="G91" s="54"/>
-      <c r="H91" s="56"/>
+      <c r="A91" s="54"/>
+      <c r="B91" s="54"/>
+      <c r="C91" s="55"/>
+      <c r="D91" s="55"/>
+      <c r="E91" s="56"/>
+      <c r="F91" s="56"/>
+      <c r="G91" s="55"/>
+      <c r="H91" s="57"/>
     </row>
     <row r="92" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="19" t="s">
-        <v>563</v>
-      </c>
-      <c r="B92" s="19"/>
-      <c r="E92" s="57"/>
-      <c r="F92" s="57"/>
-      <c r="H92" s="10"/>
+      <c r="A92" s="18" t="s">
+        <v>576</v>
+      </c>
+      <c r="B92" s="18"/>
+      <c r="E92" s="58"/>
+      <c r="F92" s="58"/>
+      <c r="H92" s="9"/>
     </row>
     <row r="93" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="10" t="s">
-        <v>564</v>
-      </c>
-      <c r="B93" s="10"/>
-      <c r="E93" s="57"/>
-      <c r="F93" s="57"/>
+      <c r="A93" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="B93" s="9"/>
+      <c r="E93" s="58"/>
+      <c r="F93" s="58"/>
     </row>
     <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="10" t="s">
-        <v>565</v>
-      </c>
-      <c r="B94" s="10"/>
-      <c r="E94" s="57"/>
-      <c r="F94" s="57"/>
+      <c r="A94" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="B94" s="9"/>
+      <c r="E94" s="58"/>
+      <c r="F94" s="58"/>
     </row>
     <row r="95" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="10" t="s">
-        <v>566</v>
-      </c>
-      <c r="B95" s="10"/>
-      <c r="E95" s="57"/>
-      <c r="F95" s="57"/>
+      <c r="A95" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="B95" s="9"/>
+      <c r="E95" s="58"/>
+      <c r="F95" s="58"/>
     </row>
     <row r="96" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="10"/>
-      <c r="B96" s="10"/>
-      <c r="E96" s="57"/>
-      <c r="F96" s="57"/>
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+      <c r="E96" s="58"/>
+      <c r="F96" s="58"/>
     </row>
     <row r="97" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="98" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fixed disclaimer icon and added more territories
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="618">
   <si>
     <t xml:space="preserve">TRANSMOUNTAIN EXPANSION PROJECT - INDIGENOUS COMMUNITIES _IMC </t>
   </si>
@@ -1473,6 +1473,9 @@
     <t xml:space="preserve">Spuzzum First Nation</t>
   </si>
   <si>
+    <t xml:space="preserve">Boothroyd Band </t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief James Hobart (Next election May 4, 2022)</t>
   </si>
   <si>
@@ -1498,6 +1501,9 @@
     <t xml:space="preserve">Squamish First Nation (Squ-Ho-0-meesh)</t>
   </si>
   <si>
+    <t xml:space="preserve">Squamish First Nation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Councillor,  Ian Campbell (Next election: December 11, 2021), Councillors; </t>
   </si>
   <si>
@@ -1561,6 +1567,9 @@
     <t xml:space="preserve">Sts'ailes Band (Chehalls Indian Band) </t>
   </si>
   <si>
+    <t xml:space="preserve">Sts'ailes Band</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Ralph Jr. Leon (next election: March 20, 2022)</t>
   </si>
   <si>
@@ -1579,6 +1588,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek) pronounced (St-wet-lem- hight-lem)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sts'wecem'cXgat'tem (Canoe Creek)</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Hillary Adam (next election: June 7, 2024)</t>
@@ -1605,6 +1617,9 @@
     <t xml:space="preserve">St'uxwtews (Bonaparte Indian Band) pronounced (Bone -eh-part)</t>
   </si>
   <si>
+    <t xml:space="preserve">St'uxwtews (Bonaparte Indian Band)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Randy Porter (next election: March 5, 2021)</t>
   </si>
   <si>
@@ -1625,6 +1640,9 @@
     <t xml:space="preserve">Stz'uminus First Nation (ltst uw' hw-nuts'-ul-wun) Chemainus</t>
   </si>
   <si>
+    <t xml:space="preserve">Stz'uminus First Nation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Roxanne Harris (Next election April 6, 2023)</t>
   </si>
   <si>
@@ -1788,6 +1806,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ts'kwaylaxw (Pavillion Indian Band)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ts'kwaylaxw(Pavillion Indian Band</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Justin Kane - election August 14, 2023</t>
@@ -1973,6 +1994,9 @@
   </si>
   <si>
     <t xml:space="preserve">Whispering Pines/Clinton Indian Bands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whispering Pines(Clinton) Indian Band</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Michael LeBourdais (Next election: February 4, 2022) </t>
@@ -2101,7 +2125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2188,6 +2212,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2441,7 +2471,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2714,15 +2744,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2840,15 +2874,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>46800</xdr:colOff>
+      <xdr:colOff>47160</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>497160</xdr:colOff>
+      <xdr:colOff>497520</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>588600</xdr:rowOff>
+      <xdr:rowOff>588960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2861,7 +2895,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="38842560" y="42183360"/>
+          <a:off x="38842920" y="42183720"/>
           <a:ext cx="450360" cy="1612440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2884,8 +2918,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4842,7 +4876,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="64" t="s">
         <v>397</v>
       </c>
@@ -4868,11 +4902,17 @@
       <c r="H58" s="12" t="s">
         <v>402</v>
       </c>
+      <c r="I58" s="0" t="n">
+        <v>49.175281</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>-121.977269</v>
+      </c>
       <c r="K58" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="153.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="51.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="18" t="s">
         <v>403</v>
       </c>
@@ -4898,17 +4938,22 @@
       <c r="H59" s="12" t="s">
         <v>408</v>
       </c>
+      <c r="I59" s="0" t="n">
+        <v>49.107871</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <v>-124.120584</v>
+      </c>
       <c r="K59" s="65" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="147" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="26" t="s">
         <v>409</v>
       </c>
-      <c r="B60" s="6" t="str">
-        <f aca="false">A60</f>
-        <v>Soowahlie First Nation</v>
+      <c r="B60" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>410</v>
@@ -4927,6 +4972,12 @@
       </c>
       <c r="H60" s="12" t="s">
         <v>414</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>49.087557</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>-121.829723</v>
       </c>
       <c r="K60" s="17" t="s">
         <v>29</v>
@@ -4936,85 +4987,100 @@
       <c r="A61" s="64" t="s">
         <v>415</v>
       </c>
-      <c r="B61" s="6" t="str">
-        <f aca="false">A61</f>
-        <v>Spuzzum First Nation</v>
+      <c r="B61" s="6" t="s">
+        <v>416</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F61" s="17" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>421</v>
+        <v>422</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>49.963059</v>
+      </c>
+      <c r="J61" s="0" t="n">
+        <v>-121.484624</v>
       </c>
       <c r="K61" s="13" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="192" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="66" t="s">
-        <v>422</v>
-      </c>
-      <c r="B62" s="6" t="str">
-        <f aca="false">A62</f>
-        <v>Squamish First Nation (Squ-Ho-0-meesh)</v>
+        <v>423</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>424</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="11" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>427</v>
+        <v>429</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>49.807197</v>
+      </c>
+      <c r="J62" s="0" t="n">
+        <v>-123.200082</v>
       </c>
       <c r="K62" s="13" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="171" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="66" t="s">
-        <v>429</v>
-      </c>
-      <c r="B63" s="6" t="str">
-        <f aca="false">A63</f>
-        <v>Squiala First Nation</v>
+        <v>431</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="F63" s="17" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="H63" s="12" t="s">
-        <v>434</v>
+        <v>436</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>49.087557</v>
+      </c>
+      <c r="J63" s="0" t="n">
+        <v>-121.829723</v>
       </c>
       <c r="K63" s="17" t="s">
         <v>29</v>
@@ -5022,29 +5088,35 @@
     </row>
     <row r="64" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="18" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B64" s="6" t="str">
         <f aca="false">A64</f>
         <v>Stk'emlupsemc Te Secwepemc</v>
       </c>
       <c r="C64" s="40" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="F64" s="17" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="H64" s="12" t="s">
-        <v>441</v>
+        <v>443</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>51.341443</v>
+      </c>
+      <c r="J64" s="0" t="n">
+        <v>-121.166411</v>
       </c>
       <c r="K64" s="50" t="s">
         <v>20</v>
@@ -5052,29 +5124,34 @@
     </row>
     <row r="65" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="26" t="s">
-        <v>442</v>
-      </c>
-      <c r="B65" s="6" t="str">
-        <f aca="false">A65</f>
-        <v>Sts'ailes Band (Chehalls Indian Band)</v>
+        <v>444</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>445</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="F65" s="17" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="H65" s="12" t="s">
-        <v>447</v>
+        <v>450</v>
+      </c>
+      <c r="I65" s="0" t="n">
+        <v>49.293578</v>
+      </c>
+      <c r="J65" s="0" t="n">
+        <v>-121.910722</v>
       </c>
       <c r="K65" s="17" t="s">
         <v>29</v>
@@ -5082,87 +5159,102 @@
     </row>
     <row r="66" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="23" t="s">
-        <v>448</v>
-      </c>
-      <c r="B66" s="6" t="str">
-        <f aca="false">A66</f>
-        <v>Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek) pronounced (St-wet-lem- hight-lem)</v>
+        <v>451</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>452</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="F66" s="17" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="H66" s="12" t="s">
-        <v>454</v>
+        <v>458</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <v>51.586232</v>
+      </c>
+      <c r="J66" s="0" t="n">
+        <v>-122.204957</v>
       </c>
       <c r="K66" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="111" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="55" t="s">
-        <v>455</v>
-      </c>
-      <c r="B67" s="6" t="str">
-        <f aca="false">A67</f>
-        <v>St'uxwtews (Bonaparte Indian Band) pronounced (Bone -eh-part)</v>
+        <v>459</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>460</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="F67" s="17"/>
       <c r="G67" s="11" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="H67" s="12" t="s">
-        <v>460</v>
+        <v>465</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <v>50.839863</v>
+      </c>
+      <c r="J67" s="0" t="n">
+        <v>-121.372183</v>
       </c>
       <c r="K67" s="50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="159.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="48" t="s">
-        <v>461</v>
-      </c>
-      <c r="B68" s="6" t="str">
-        <f aca="false">A68</f>
-        <v>Stz'uminus First Nation (ltst uw' hw-nuts'-ul-wun) Chemainus</v>
+        <v>466</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="C68" s="67" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="G68" s="20" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="H68" s="12" t="s">
-        <v>466</v>
+        <v>472</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>48.846385</v>
+      </c>
+      <c r="J68" s="0" t="n">
+        <v>-123.630268</v>
       </c>
       <c r="K68" s="50" t="s">
         <v>20</v>
@@ -5170,29 +5262,35 @@
     </row>
     <row r="69" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="26" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="B69" s="6" t="str">
         <f aca="false">A69</f>
         <v>Sumas First Nation</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="H69" s="12" t="s">
-        <v>472</v>
+        <v>478</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>49.052587</v>
+      </c>
+      <c r="J69" s="0" t="n">
+        <v>-122.193538</v>
       </c>
       <c r="K69" s="17" t="s">
         <v>29</v>
@@ -5200,404 +5298,476 @@
     </row>
     <row r="70" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="64" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="B70" s="6" t="str">
         <f aca="false">A70</f>
         <v>Toosey Indian Band (Tl'esqox)</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="H70" s="21"/>
+      <c r="I70" s="0" t="n">
+        <v>52.195501</v>
+      </c>
+      <c r="J70" s="0" t="n">
+        <v>-123.798415</v>
+      </c>
       <c r="K70" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="211.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="58.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="18" t="s">
-        <v>478</v>
-      </c>
-      <c r="B71" s="6" t="str">
-        <f aca="false">A71</f>
-        <v>Tsartlip First Nation</v>
+        <v>484</v>
+      </c>
+      <c r="B71" s="68" t="s">
+        <v>265</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="H71" s="12" t="s">
-        <v>483</v>
+        <v>489</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>48.724102</v>
+      </c>
+      <c r="J71" s="0" t="n">
+        <v>-123.324246</v>
       </c>
       <c r="K71" s="50" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="205.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="66" t="s">
-        <v>484</v>
-      </c>
-      <c r="B72" s="6" t="str">
-        <f aca="false">A72</f>
-        <v>Tsawout First Nation</v>
+        <v>490</v>
+      </c>
+      <c r="B72" s="68" t="s">
+        <v>265</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="H72" s="12" t="s">
-        <v>489</v>
+        <v>495</v>
+      </c>
+      <c r="I72" s="0" t="n">
+        <v>48.724102</v>
+      </c>
+      <c r="J72" s="0" t="n">
+        <v>-123.324246</v>
       </c>
       <c r="K72" s="50" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="121.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="18" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B73" s="6" t="str">
         <f aca="false">A73</f>
         <v>Tsawwassen First Nation</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="H73" s="12" t="s">
-        <v>497</v>
+        <v>503</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <v>49.042909</v>
+      </c>
+      <c r="J73" s="0" t="n">
+        <v>-123.094409</v>
       </c>
       <c r="K73" s="50" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="258" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="48" t="s">
-        <v>499</v>
-      </c>
-      <c r="B74" s="6" t="str">
-        <f aca="false">A74</f>
-        <v>Ts'elxweyeqw Tribe Management Limited</v>
+        <v>505</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="F74" s="68" t="s">
-        <v>503</v>
+        <v>508</v>
+      </c>
+      <c r="F74" s="69" t="s">
+        <v>509</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="H74" s="12"/>
+      <c r="I74" s="0" t="n">
+        <v>49.087557</v>
+      </c>
+      <c r="J74" s="0" t="n">
+        <v>-121.829723</v>
+      </c>
       <c r="K74" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="26" t="s">
-        <v>505</v>
-      </c>
-      <c r="B75" s="6" t="str">
-        <f aca="false">A75</f>
-        <v>Tseycum First Nation</v>
+        <v>511</v>
+      </c>
+      <c r="B75" s="68" t="s">
+        <v>265</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="H75" s="12" t="s">
-        <v>511</v>
+        <v>517</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>48.724102</v>
+      </c>
+      <c r="J75" s="0" t="n">
+        <v>-123.324246</v>
       </c>
       <c r="K75" s="50" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="64" t="s">
-        <v>512</v>
-      </c>
-      <c r="B76" s="6" t="str">
-        <f aca="false">A76</f>
-        <v>Ts'kwaylaxw (Pavillion Indian Band)</v>
+        <v>518</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>519</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="D76" s="19" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="F76" s="17"/>
       <c r="G76" s="11" t="s">
-        <v>516</v>
+        <v>523</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <v>50.883097</v>
+      </c>
+      <c r="J76" s="0" t="n">
+        <v>-121.842308</v>
       </c>
       <c r="K76" s="50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="195" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="18" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="B77" s="6" t="str">
         <f aca="false">A77</f>
         <v>Tsleil Waututh Nation</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="F77" s="17" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="H77" s="12" t="s">
-        <v>522</v>
+        <v>529</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <v>49.309839</v>
+      </c>
+      <c r="J77" s="0" t="n">
+        <v>-122.980478</v>
       </c>
       <c r="K77" s="50" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="148.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="64.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="18" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="B78" s="6" t="str">
         <f aca="false">A78</f>
         <v>T'Sou-ke Nation</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c r="E78" s="20" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="F78" s="16" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="H78" s="12" t="s">
-        <v>530</v>
+        <v>537</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <v>48.385518</v>
+      </c>
+      <c r="J78" s="0" t="n">
+        <v>-123.696567</v>
       </c>
       <c r="K78" s="50" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="139.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="26" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="B79" s="6" t="str">
         <f aca="false">A79</f>
         <v>Tk'emlups te Secwepemc</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>533</v>
-      </c>
-      <c r="E79" s="69" t="s">
-        <v>534</v>
-      </c>
-      <c r="F79" s="70" t="s">
-        <v>535</v>
+        <v>540</v>
+      </c>
+      <c r="E79" s="70" t="s">
+        <v>541</v>
+      </c>
+      <c r="F79" s="71" t="s">
+        <v>542</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="H79" s="12" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
       <c r="K79" s="50" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="117.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="26" t="s">
-        <v>538</v>
-      </c>
-      <c r="B80" s="6" t="str">
-        <f aca="false">A80</f>
-        <v>Tzeachten First Nation</v>
+        <v>545</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
       <c r="F80" s="17" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="H80" s="12" t="s">
-        <v>544</v>
+        <v>551</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <v>49.087557</v>
+      </c>
+      <c r="J80" s="0" t="n">
+        <v>-121.829723</v>
       </c>
       <c r="K80" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="199.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="76.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="26" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="B81" s="6" t="str">
         <f aca="false">A81</f>
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>546</v>
-      </c>
-      <c r="D81" s="71" t="s">
-        <v>547</v>
+        <v>553</v>
+      </c>
+      <c r="D81" s="72" t="s">
+        <v>554</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
       <c r="H81" s="12" t="s">
-        <v>551</v>
+        <v>558</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <v>52.475488</v>
+      </c>
+      <c r="J81" s="0" t="n">
+        <v>-125.301018</v>
       </c>
       <c r="K81" s="50" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="26" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="B82" s="6" t="str">
         <f aca="false">A82</f>
         <v>Union Bar First Nations</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>557</v>
+        <v>564</v>
       </c>
       <c r="H82" s="21"/>
+      <c r="I82" s="0" t="n">
+        <v>49.210913</v>
+      </c>
+      <c r="J82" s="0" t="n">
+        <v>-121.240262</v>
+      </c>
       <c r="K82" s="50"/>
     </row>
-    <row r="83" customFormat="false" ht="117.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="26" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
       <c r="B83" s="6" t="str">
         <f aca="false">A83</f>
         <v>Upper Nicola Indian Band</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="F83" s="17"/>
       <c r="G83" s="11" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>563</v>
+        <v>570</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>50.167239</v>
+      </c>
+      <c r="J83" s="0" t="n">
+        <v>-120.283533</v>
       </c>
       <c r="K83" s="17" t="s">
         <v>20</v>
@@ -5605,67 +5775,78 @@
     </row>
     <row r="84" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="64" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="B84" s="6" t="str">
         <f aca="false">A84</f>
         <v>Upper Similkameen Indian Band</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="D84" s="24" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>567</v>
-      </c>
-      <c r="F84" s="72" t="s">
-        <v>566</v>
+        <v>574</v>
+      </c>
+      <c r="F84" s="73" t="s">
+        <v>573</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="H84" s="21" t="s">
-        <v>569</v>
+        <v>576</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>49.462883</v>
+      </c>
+      <c r="J84" s="0" t="n">
+        <v>-120.50172</v>
       </c>
       <c r="K84" s="17" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="341.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>571</v>
-      </c>
-      <c r="B85" s="6" t="str">
-        <f aca="false">A85</f>
-        <v>Whispering Pines/Clinton Indian Bands</v>
+        <v>578</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>579</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>573</v>
+        <v>581</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>574</v>
+        <v>582</v>
       </c>
       <c r="F85" s="17" t="s">
-        <v>575</v>
+        <v>583</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>577</v>
+        <v>585</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <v>51.194286</v>
+      </c>
+      <c r="J85" s="0" t="n">
+        <v>-121.613314</v>
       </c>
       <c r="K85" s="13" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="341.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="73" t="s">
-        <v>579</v>
+        <v>586</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="58.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="74" t="s">
+        <v>587</v>
       </c>
       <c r="B86" s="6" t="str">
         <f aca="false">A86</f>
@@ -5677,171 +5858,194 @@
       <c r="F86" s="17"/>
       <c r="H86" s="12"/>
       <c r="K86" s="13" t="s">
-        <v>578</v>
+        <v>586</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="18" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="B87" s="6" t="str">
         <f aca="false">A87</f>
         <v>Williams Lake Indian Band</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="D87" s="11"/>
       <c r="E87" s="11" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="F87" s="17"/>
       <c r="G87" s="11" t="s">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>584</v>
-      </c>
-      <c r="K87" s="74"/>
-    </row>
-    <row r="88" customFormat="false" ht="108.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>592</v>
+      </c>
+      <c r="I87" s="0" t="n">
+        <v>52.10532</v>
+      </c>
+      <c r="J87" s="0" t="n">
+        <v>-121.9905</v>
+      </c>
+      <c r="K87" s="75"/>
+    </row>
+    <row r="88" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="26" t="s">
-        <v>585</v>
-      </c>
-      <c r="B88" s="6" t="str">
-        <f aca="false">A88</f>
-        <v>Yakweakwioose First Nation</v>
+        <v>593</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C88" s="11" t="s">
+        <v>594</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="E88" s="11" t="s">
+        <v>596</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="H88" s="21" t="s">
+        <v>599</v>
+      </c>
+      <c r="I88" s="0" t="n">
+        <v>49.087557</v>
+      </c>
+      <c r="J88" s="0" t="n">
+        <v>-121.829723</v>
+      </c>
+      <c r="K88" s="13" t="s">
         <v>586</v>
-      </c>
-      <c r="D88" s="11" t="s">
-        <v>587</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>588</v>
-      </c>
-      <c r="F88" s="17" t="s">
-        <v>589</v>
-      </c>
-      <c r="G88" s="11" t="s">
-        <v>590</v>
-      </c>
-      <c r="H88" s="21" t="s">
-        <v>591</v>
-      </c>
-      <c r="K88" s="13" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="26" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="B89" s="6" t="str">
         <f aca="false">A89</f>
         <v>Yale First Nation</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="F89" s="17" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>597</v>
+        <v>605</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>598</v>
+        <v>606</v>
+      </c>
+      <c r="I89" s="0" t="n">
+        <v>49.492718</v>
+      </c>
+      <c r="J89" s="0" t="n">
+        <v>-121.423097</v>
       </c>
       <c r="K89" s="13" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="129" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="26" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="B90" s="6" t="str">
         <f aca="false">A90</f>
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="E90" s="67" t="s">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="F90" s="17" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="H90" s="12" t="s">
-        <v>605</v>
+        <v>613</v>
+      </c>
+      <c r="I90" s="0" t="n">
+        <v>52.854978</v>
+      </c>
+      <c r="J90" s="0" t="n">
+        <v>-121.585666</v>
       </c>
       <c r="K90" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="75"/>
-      <c r="B91" s="75"/>
-      <c r="C91" s="76"/>
-      <c r="D91" s="76"/>
-      <c r="E91" s="77"/>
-      <c r="F91" s="77"/>
-      <c r="G91" s="76"/>
-      <c r="H91" s="78"/>
+      <c r="A91" s="76"/>
+      <c r="B91" s="76"/>
+      <c r="C91" s="77"/>
+      <c r="D91" s="77"/>
+      <c r="E91" s="78"/>
+      <c r="F91" s="78"/>
+      <c r="G91" s="77"/>
+      <c r="H91" s="79"/>
     </row>
     <row r="92" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="26" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="B92" s="26"/>
-      <c r="E92" s="79"/>
-      <c r="F92" s="79"/>
+      <c r="E92" s="80"/>
+      <c r="F92" s="80"/>
       <c r="H92" s="11"/>
     </row>
     <row r="93" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="11" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="B93" s="11"/>
-      <c r="E93" s="79"/>
-      <c r="F93" s="79"/>
+      <c r="E93" s="80"/>
+      <c r="F93" s="80"/>
     </row>
     <row r="94" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="11" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="B94" s="11"/>
-      <c r="E94" s="79"/>
-      <c r="F94" s="79"/>
+      <c r="E94" s="80"/>
+      <c r="F94" s="80"/>
     </row>
     <row r="95" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="11" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="B95" s="11"/>
-      <c r="E95" s="79"/>
-      <c r="F95" s="79"/>
+      <c r="E95" s="80"/>
+      <c r="F95" s="80"/>
     </row>
     <row r="96" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="11"/>
       <c r="B96" s="11"/>
-      <c r="E96" s="79"/>
-      <c r="F96" s="79"/>
+      <c r="E96" s="80"/>
+      <c r="F96" s="80"/>
     </row>
     <row r="97" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="98" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
started on pipeline profile
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -2870,45 +2870,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47160</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>497520</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>588960</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Picture 4" descr="http://lyackson.bc.ca/wp-content/uploads/2014/10/Valdes_Island_Modern-land-use-e1412621912214.jpg"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="38842920" y="42183720"/>
-          <a:ext cx="450360" cy="1612440"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2918,8 +2880,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F81" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H86" activeCellId="0" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3187,7 +3149,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="131.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="26" t="s">
         <v>60</v>
       </c>
@@ -3222,7 +3184,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="134.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
@@ -3257,7 +3219,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="180" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
         <v>77</v>
       </c>
@@ -3292,7 +3254,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
         <v>84</v>
       </c>
@@ -3327,7 +3289,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="205.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="62.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="s">
         <v>92</v>
       </c>
@@ -3362,7 +3324,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="159.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="46.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
         <v>100</v>
       </c>
@@ -3397,7 +3359,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="s">
         <v>109</v>
       </c>
@@ -3432,7 +3394,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="191.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
         <v>116</v>
       </c>
@@ -3468,7 +3430,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="26" t="s">
         <v>123</v>
       </c>
@@ -3500,7 +3462,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="126" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="26" t="s">
         <v>128</v>
       </c>
@@ -3536,7 +3498,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="165.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>135</v>
       </c>
@@ -3570,7 +3532,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="50.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="26" t="s">
         <v>141</v>
       </c>
@@ -3605,7 +3567,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="160.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="31" t="s">
         <v>150</v>
       </c>
@@ -3638,7 +3600,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="34" t="s">
         <v>157</v>
       </c>
@@ -3744,7 +3706,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="195" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="34" t="s">
         <v>180</v>
       </c>
@@ -3779,7 +3741,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="174.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
         <v>189</v>
       </c>
@@ -3815,7 +3777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="195" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="s">
         <v>196</v>
       </c>
@@ -3883,7 +3845,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="56.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="41" t="s">
         <v>211</v>
       </c>
@@ -3917,7 +3879,7 @@
       </c>
       <c r="K29" s="13"/>
     </row>
-    <row r="30" customFormat="false" ht="126.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="49.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
         <v>218</v>
       </c>
@@ -3953,7 +3915,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="43" t="s">
         <v>225</v>
       </c>
@@ -3987,7 +3949,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="79.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
         <v>231</v>
       </c>
@@ -4022,7 +3984,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="18" t="s">
         <v>239</v>
       </c>
@@ -4502,7 +4464,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="286.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="80.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="23" t="s">
         <v>328</v>
       </c>
@@ -4599,7 +4561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="183" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="80.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="57" t="s">
         <v>345</v>
       </c>
@@ -4634,7 +4596,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="112.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="60" t="s">
         <v>353</v>
       </c>
@@ -4667,7 +4629,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="212.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="51.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="48" t="s">
         <v>359</v>
       </c>
@@ -4769,7 +4731,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="136.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="23" t="s">
         <v>377</v>
       </c>
@@ -4804,7 +4766,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="124.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="26" t="s">
         <v>384</v>
       </c>
@@ -4840,7 +4802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="150" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="26" t="s">
         <v>391</v>
       </c>
@@ -5157,7 +5119,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="23" t="s">
         <v>451</v>
       </c>

</xml_diff>

<commit_message>
started on mobile and tablet optimization
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BC First Nations" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="706">
   <si>
     <t xml:space="preserve">TRANSMOUNTAIN EXPANSION PROJECT - INDIGENOUS COMMUNITIES _IMC </t>
   </si>
@@ -1920,6 +1920,9 @@
     <t xml:space="preserve">Union Bar First Nations</t>
   </si>
   <si>
+    <t xml:space="preserve">Union Bar First Nation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chief Andrew (Andy) Alex (appointed in 1977)</t>
   </si>
   <si>
@@ -2395,7 +2398,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2488,12 +2491,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2737,7 +2734,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3052,10 +3049,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3142,8 +3135,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B81" activeCellId="0" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5916,24 +5909,23 @@
       <c r="A81" s="23" t="s">
         <v>555</v>
       </c>
-      <c r="B81" s="6" t="str">
-        <f aca="false">A81</f>
-        <v>Union Bar First Nations</v>
+      <c r="B81" s="23" t="s">
+        <v>556</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="H81" s="19"/>
       <c r="I81" s="0" t="n">
@@ -5946,27 +5938,27 @@
     </row>
     <row r="82" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="23" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B82" s="6" t="str">
         <f aca="false">A82</f>
         <v>Upper Nicola Indian Band</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F82" s="17"/>
       <c r="G82" s="11" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="H82" s="12" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="I82" s="0" t="n">
         <v>50.167239</v>
@@ -5980,29 +5972,29 @@
     </row>
     <row r="83" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="59" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B83" s="6" t="str">
         <f aca="false">A83</f>
         <v>Upper Similkameen Indian Band</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D83" s="19" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E83" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="F83" s="68" t="s">
         <v>570</v>
       </c>
-      <c r="F83" s="68" t="s">
-        <v>569</v>
-      </c>
       <c r="G83" s="11" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="H83" s="19" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="I83" s="0" t="n">
         <v>49.462883</v>
@@ -6011,33 +6003,33 @@
         <v>-120.50172</v>
       </c>
       <c r="K83" s="17" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="18" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="I84" s="0" t="n">
         <v>51.194286</v>
@@ -6046,30 +6038,30 @@
         <v>-121.613314</v>
       </c>
       <c r="K84" s="13" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B85" s="6" t="str">
         <f aca="false">A85</f>
         <v>Williams Lake Indian Band</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D85" s="11"/>
       <c r="E85" s="11" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F85" s="17"/>
       <c r="G85" s="11" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="I85" s="0" t="n">
         <v>52.10532</v>
@@ -6081,28 +6073,28 @@
     </row>
     <row r="86" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="23" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="H86" s="19" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="I86" s="0" t="n">
         <v>49.087557</v>
@@ -6111,34 +6103,34 @@
         <v>-121.829723</v>
       </c>
       <c r="K86" s="13" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="23" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B87" s="6" t="str">
         <f aca="false">A87</f>
         <v>Yale First Nation</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="I87" s="0" t="n">
         <v>49.492718</v>
@@ -6152,29 +6144,29 @@
     </row>
     <row r="88" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="23" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B88" s="6" t="str">
         <f aca="false">A88</f>
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="E88" s="63" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F88" s="17" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="G88" s="11" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H88" s="12" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="I88" s="0" t="n">
         <v>52.854978</v>
@@ -6198,7 +6190,7 @@
     </row>
     <row r="90" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="23" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B90" s="23"/>
       <c r="E90" s="74"/>
@@ -6207,7 +6199,7 @@
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B91" s="11"/>
       <c r="E91" s="74"/>
@@ -6215,7 +6207,7 @@
     </row>
     <row r="92" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B92" s="11"/>
       <c r="E92" s="74"/>
@@ -6223,7 +6215,7 @@
     </row>
     <row r="93" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="11" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B93" s="11"/>
       <c r="E93" s="74"/>
@@ -6341,11 +6333,11 @@
   </sheetPr>
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B91" activeCellId="0" sqref="B91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="1" sqref="B81 A80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.31"/>
@@ -6356,13 +6348,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C1" s="75" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6374,10 +6366,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D2" s="77" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6389,10 +6381,10 @@
         <v>21</v>
       </c>
       <c r="C3" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6404,10 +6396,10 @@
         <v>30</v>
       </c>
       <c r="C4" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D4" s="75" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6419,10 +6411,10 @@
         <v>38</v>
       </c>
       <c r="C5" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D5" s="78" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6434,10 +6426,10 @@
         <v>45</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D6" s="75" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6449,10 +6441,10 @@
         <v>52</v>
       </c>
       <c r="C7" s="76" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D7" s="75" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6464,10 +6456,10 @@
         <v>61</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6476,28 +6468,28 @@
         <v>Chi:yo:m Agassiz (Cheam) First Nation - meaning "Wild Strawberry Place"</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C9" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D9" s="75" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
         <f aca="false">'BC First Nations'!A11</f>
-        <v>Coldwater First Nation (Nc/etko - the people of the creeks)      </v>
+        <v>Coldwater First Nation (Nc/etko - the people of the creeks)</v>
       </c>
       <c r="B10" s="75" t="s">
         <v>78</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D10" s="75" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6506,13 +6498,13 @@
         <v>Cook's Ferry Indian Band Kumcheen (Variation Nkumcheen); Includes Pokheistk (Variation Pakeist, Pokheistsk), Pemynoos (Variation Piminos), Spatsum (Variation Spaptsin), Spence'S Bridge</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C11" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D11" s="75" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6524,10 +6516,10 @@
         <v>92</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D12" s="75" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6539,10 +6531,10 @@
         <v>101</v>
       </c>
       <c r="C13" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D13" s="75" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6554,25 +6546,25 @@
         <v>110</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D14" s="78" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="str">
         <f aca="false">'BC First Nations'!A16</f>
-        <v>Halalt First Nation </v>
+        <v>Halalt First Nation</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D15" s="75" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6584,25 +6576,25 @@
         <v>123</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D16" s="75" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="str">
         <f aca="false">'BC First Nations'!A18</f>
-        <v>Huu-ay-aht First Nation </v>
+        <v>Huu-ay-aht First Nation</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D17" s="75" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6614,10 +6606,10 @@
         <v>135</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D18" s="75" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6629,25 +6621,25 @@
         <v>142</v>
       </c>
       <c r="C19" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D19" s="75" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="str">
         <f aca="false">'BC First Nations'!A21</f>
-        <v>Kwaw -Kwaw-Aplit First Nations </v>
+        <v>Kwaw -Kwaw-Aplit First Nations</v>
       </c>
       <c r="B20" s="75" t="s">
         <v>151</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D20" s="75" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6659,10 +6651,10 @@
         <v>157</v>
       </c>
       <c r="C21" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D21" s="75" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6674,10 +6666,10 @@
         <v>165</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D22" s="75" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6689,10 +6681,10 @@
         <v>173</v>
       </c>
       <c r="C23" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D23" s="75" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6704,10 +6696,10 @@
         <v>180</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D24" s="75" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6719,10 +6711,10 @@
         <v>189</v>
       </c>
       <c r="C25" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D25" s="75" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6734,10 +6726,10 @@
         <v>197</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D26" s="75" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6749,10 +6741,10 @@
         <v>204</v>
       </c>
       <c r="C27" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D27" s="75" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6764,10 +6756,10 @@
         <v>211</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D28" s="75" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6779,10 +6771,10 @@
         <v>218</v>
       </c>
       <c r="C29" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D29" s="75" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6794,10 +6786,10 @@
         <v>225</v>
       </c>
       <c r="C30" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D30" s="75" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6809,10 +6801,10 @@
         <v>231</v>
       </c>
       <c r="C31" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D31" s="78" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6824,10 +6816,10 @@
         <v>239</v>
       </c>
       <c r="C32" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D32" s="75" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6839,10 +6831,10 @@
         <v>245</v>
       </c>
       <c r="C33" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D33" s="75" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6854,10 +6846,10 @@
         <v>253</v>
       </c>
       <c r="C34" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D34" s="75" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6869,10 +6861,10 @@
         <v>259</v>
       </c>
       <c r="C35" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D35" s="75" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6884,10 +6876,10 @@
         <v>265</v>
       </c>
       <c r="C36" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D36" s="78" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6899,10 +6891,10 @@
         <v>271</v>
       </c>
       <c r="C37" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D37" s="75" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6914,10 +6906,10 @@
         <v>277</v>
       </c>
       <c r="C38" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D38" s="75" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6929,10 +6921,10 @@
         <v>285</v>
       </c>
       <c r="C39" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D39" s="75" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6944,25 +6936,25 @@
         <v>292</v>
       </c>
       <c r="C40" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D40" s="75" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="str">
         <f aca="false">'BC First Nations'!A42</f>
-        <v>Qayqayt First Nation (New Westminister) </v>
+        <v>Qayqayt First Nation (New Westminister)</v>
       </c>
       <c r="B41" s="75" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C41" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D41" s="78" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6974,10 +6966,10 @@
         <v>304</v>
       </c>
       <c r="C42" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D42" s="75" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6989,10 +6981,10 @@
         <v>312</v>
       </c>
       <c r="C43" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D43" s="75" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7004,10 +6996,10 @@
         <v>319</v>
       </c>
       <c r="C44" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D44" s="75" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7019,10 +7011,10 @@
         <v>324</v>
       </c>
       <c r="C45" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D45" s="78" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7034,25 +7026,25 @@
         <v>329</v>
       </c>
       <c r="C46" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D46" s="78" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="str">
         <f aca="false">'BC First Nations'!A48</f>
-        <v>Shackan Indian Band </v>
+        <v>Shackan Indian Band</v>
       </c>
       <c r="B47" s="75" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C47" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D47" s="78" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7064,10 +7056,10 @@
         <v>342</v>
       </c>
       <c r="C48" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D48" s="75" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7079,10 +7071,10 @@
         <v>349</v>
       </c>
       <c r="C49" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D49" s="75" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7094,10 +7086,10 @@
         <v>356</v>
       </c>
       <c r="C50" s="75" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D50" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7109,25 +7101,25 @@
         <v>362</v>
       </c>
       <c r="C51" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D51" s="75" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="str">
         <f aca="false">'BC First Nations'!A53</f>
-        <v>Skuppah Indian Band </v>
+        <v>Skuppah Indian Band</v>
       </c>
       <c r="B52" s="75" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C52" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D52" s="78" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7139,25 +7131,25 @@
         <v>373</v>
       </c>
       <c r="C53" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D53" s="75" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="str">
         <f aca="false">'BC First Nations'!A55</f>
-        <v>Shuswap Indian Band </v>
+        <v>Shuswap Indian Band</v>
       </c>
       <c r="B54" s="75" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C54" s="75" t="s">
-        <v>618</v>
-      </c>
-      <c r="D54" s="79" t="s">
-        <v>676</v>
+        <v>619</v>
+      </c>
+      <c r="D54" s="75" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7169,10 +7161,10 @@
         <v>387</v>
       </c>
       <c r="C55" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D55" s="75" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7184,10 +7176,10 @@
         <v>393</v>
       </c>
       <c r="C56" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D56" s="75" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7199,10 +7191,10 @@
         <v>399</v>
       </c>
       <c r="C57" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D57" s="75" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7214,10 +7206,10 @@
         <v>405</v>
       </c>
       <c r="C58" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D58" s="75" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7229,10 +7221,10 @@
         <v>411</v>
       </c>
       <c r="C59" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D59" s="78" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7244,10 +7236,10 @@
         <v>420</v>
       </c>
       <c r="C60" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D60" s="75" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7259,40 +7251,40 @@
         <v>427</v>
       </c>
       <c r="C61" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D61" s="75" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="str">
         <f aca="false">'BC First Nations'!A63</f>
-        <v>Stk'emlupsemc Te Secwepemc </v>
+        <v>Stk'emlupsemc Te Secwepemc</v>
       </c>
       <c r="B62" s="75" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C62" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D62" s="75" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="str">
         <f aca="false">'BC First Nations'!A64</f>
-        <v>Sts'ailes Band (Chehalls Indian Band) </v>
+        <v>Sts'ailes Band (Chehalls Indian Band)</v>
       </c>
       <c r="B63" s="75" t="s">
         <v>441</v>
       </c>
       <c r="C63" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D63" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7301,13 +7293,13 @@
         <v>Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek) pronounced (St-wet-lem- hight-lem)</v>
       </c>
       <c r="B64" s="75" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C64" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D64" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7319,10 +7311,10 @@
         <v>456</v>
       </c>
       <c r="C65" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D65" s="75" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7334,10 +7326,10 @@
         <v>463</v>
       </c>
       <c r="C66" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D66" s="75" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7349,10 +7341,10 @@
         <v>469</v>
       </c>
       <c r="C67" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D67" s="75" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7361,13 +7353,13 @@
         <v>Toosey Indian Band (Tl'esqox)</v>
       </c>
       <c r="B68" s="75" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C68" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D68" s="78" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7379,10 +7371,10 @@
         <v>480</v>
       </c>
       <c r="C69" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D69" s="78" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7394,10 +7386,10 @@
         <v>486</v>
       </c>
       <c r="C70" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D70" s="78" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7409,10 +7401,10 @@
         <v>493</v>
       </c>
       <c r="C71" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D71" s="78" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7424,10 +7416,10 @@
         <v>501</v>
       </c>
       <c r="C72" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D72" s="75" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7439,10 +7431,10 @@
         <v>507</v>
       </c>
       <c r="C73" s="75" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D73" s="78" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7454,10 +7446,10 @@
         <v>514</v>
       </c>
       <c r="C74" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D74" s="75" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7469,10 +7461,10 @@
         <v>520</v>
       </c>
       <c r="C75" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D75" s="75" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7484,10 +7476,10 @@
         <v>527</v>
       </c>
       <c r="C76" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D76" s="75" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7499,10 +7491,10 @@
         <v>534</v>
       </c>
       <c r="C77" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D77" s="75" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7514,10 +7506,10 @@
         <v>541</v>
       </c>
       <c r="C78" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D78" s="75" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7529,10 +7521,10 @@
         <v>548</v>
       </c>
       <c r="C79" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D79" s="75" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7544,10 +7536,10 @@
         <v>555</v>
       </c>
       <c r="C80" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D80" s="75" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7556,13 +7548,13 @@
         <v>Upper Nicola Indian Band</v>
       </c>
       <c r="B81" s="75" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C81" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D81" s="75" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7571,13 +7563,13 @@
         <v>Upper Similkameen Indian Band</v>
       </c>
       <c r="B82" s="75" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C82" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D82" s="75" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7586,13 +7578,13 @@
         <v>Whispering Pines/Clinton Indian Bands</v>
       </c>
       <c r="B83" s="75" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C83" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D83" s="75" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7601,13 +7593,13 @@
         <v>Williams Lake Indian Band</v>
       </c>
       <c r="B84" s="75" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C84" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D84" s="75" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7616,28 +7608,28 @@
         <v>Yakweakwioose First Nation</v>
       </c>
       <c r="B85" s="75" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C85" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D85" s="75" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="str">
         <f aca="false">'BC First Nations'!A87</f>
-        <v>Yale First Nation </v>
+        <v>Yale First Nation</v>
       </c>
       <c r="B86" s="75" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C86" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D86" s="75" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7646,13 +7638,13 @@
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
       <c r="B87" s="75" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C87" s="75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D87" s="75" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="G87" s="75"/>
     </row>

</xml_diff>

<commit_message>
improved pop up style and consistency
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="759">
   <si>
     <t xml:space="preserve">TRANSMOUNTAIN EXPANSION PROJECT - INDIGENOUS COMMUNITIES _IMC </t>
   </si>
@@ -1653,6 +1653,9 @@
   </si>
   <si>
     <t xml:space="preserve">Stk'emlupsemc Te Secwepemc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stk'emlupsemc te Secwepemc</t>
   </si>
   <si>
     <t xml:space="preserve">Chief Ronald Ignace</t>
@@ -3291,8 +3294,8 @@
   </sheetPr>
   <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3840,7 +3843,7 @@
       </c>
       <c r="B16" s="6" t="str">
         <f aca="false">A16</f>
-        <v>Halalt First Nation </v>
+        <v>Halalt First Nation</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>123</v>
@@ -3914,7 +3917,7 @@
       </c>
       <c r="B18" s="6" t="str">
         <f aca="false">A18</f>
-        <v>Huu-ay-aht First Nation </v>
+        <v>Huu-ay-aht First Nation</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>137</v>
@@ -5283,7 +5286,7 @@
       </c>
       <c r="B55" s="6" t="str">
         <f aca="false">A55</f>
-        <v>Shuswap Indian Band </v>
+        <v>Shuswap Indian Band</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>415</v>
@@ -5585,28 +5588,27 @@
       <c r="A63" s="18" t="s">
         <v>474</v>
       </c>
-      <c r="B63" s="6" t="str">
-        <f aca="false">A63</f>
-        <v>Stk'emlupsemc Te Secwepemc </v>
+      <c r="B63" s="6" t="s">
+        <v>475</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63" s="36" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="J63" s="0" t="n">
         <v>51.341443</v>
@@ -5620,31 +5622,31 @@
     </row>
     <row r="64" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="23" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F64" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="G64" s="17" t="s">
         <v>486</v>
       </c>
-      <c r="G64" s="17" t="s">
-        <v>485</v>
-      </c>
       <c r="H64" s="11" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="J64" s="0" t="n">
         <v>49.293578</v>
@@ -5658,31 +5660,31 @@
     </row>
     <row r="65" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="21" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="J65" s="0" t="n">
         <v>51.586232</v>
@@ -5696,29 +5698,29 @@
     </row>
     <row r="66" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="62" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="G66" s="17"/>
       <c r="H66" s="11" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="J66" s="0" t="n">
         <v>50.839863</v>
@@ -5732,29 +5734,29 @@
     </row>
     <row r="67" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="44" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="63" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="F67" s="11" t="s">
+        <v>510</v>
+      </c>
+      <c r="G67" s="17" t="s">
         <v>509</v>
       </c>
-      <c r="G67" s="17" t="s">
-        <v>508</v>
-      </c>
       <c r="H67" s="15" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="J67" s="0" t="n">
         <v>48.846385</v>
@@ -5768,7 +5770,7 @@
     </row>
     <row r="68" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="23" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B68" s="6" t="str">
         <f aca="false">A68</f>
@@ -5776,22 +5778,22 @@
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="F68" s="11" t="s">
+        <v>516</v>
+      </c>
+      <c r="G68" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="G68" s="17" t="s">
-        <v>514</v>
-      </c>
       <c r="H68" s="11" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="J68" s="0" t="n">
         <v>49.052587</v>
@@ -5805,7 +5807,7 @@
     </row>
     <row r="69" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="59" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B69" s="6" t="str">
         <f aca="false">A69</f>
@@ -5813,19 +5815,19 @@
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="11" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="F69" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="G69" s="17" t="s">
         <v>521</v>
       </c>
-      <c r="G69" s="17" t="s">
-        <v>520</v>
-      </c>
       <c r="H69" s="11" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="I69" s="19"/>
       <c r="J69" s="0" t="n">
@@ -5840,31 +5842,31 @@
     </row>
     <row r="70" customFormat="false" ht="58.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="18" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>288</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F70" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="G70" s="17" t="s">
         <v>527</v>
       </c>
-      <c r="G70" s="17" t="s">
-        <v>526</v>
-      </c>
       <c r="H70" s="11" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="J70" s="0" t="n">
         <v>48.724102</v>
@@ -5878,31 +5880,31 @@
     </row>
     <row r="71" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="61" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>288</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="F71" s="11" t="s">
+        <v>535</v>
+      </c>
+      <c r="G71" s="17" t="s">
         <v>534</v>
       </c>
-      <c r="G71" s="17" t="s">
-        <v>533</v>
-      </c>
       <c r="H71" s="11" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="I71" s="12" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="J71" s="0" t="n">
         <v>48.724102</v>
@@ -5911,37 +5913,37 @@
         <v>-123.324246</v>
       </c>
       <c r="L71" s="46" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="18" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B72" s="6" t="str">
         <f aca="false">A72</f>
         <v>Tsawwassen First Nation</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="G72" s="17" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="J72" s="0" t="n">
         <v>49.042909</v>
@@ -5950,31 +5952,31 @@
         <v>-123.094409</v>
       </c>
       <c r="L72" s="46" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="44" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="11" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="G73" s="64" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="I73" s="12"/>
       <c r="J73" s="0" t="n">
@@ -5989,31 +5991,31 @@
     </row>
     <row r="74" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="23" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>288</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="J74" s="0" t="n">
         <v>48.724102</v>
@@ -6022,31 +6024,31 @@
         <v>-123.324246</v>
       </c>
       <c r="L74" s="46" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="59" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="G75" s="17"/>
       <c r="H75" s="11" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="J75" s="0" t="n">
         <v>50.883097</v>
@@ -6060,32 +6062,32 @@
     </row>
     <row r="76" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B76" s="6" t="str">
         <f aca="false">A76</f>
         <v>Tsleil Waututh Nation</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F76" s="11" t="s">
+        <v>573</v>
+      </c>
+      <c r="G76" s="17" t="s">
         <v>572</v>
       </c>
-      <c r="G76" s="17" t="s">
-        <v>571</v>
-      </c>
       <c r="H76" s="11" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="I76" s="12" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="J76" s="0" t="n">
         <v>49.309839</v>
@@ -6094,37 +6096,37 @@
         <v>-122.980478</v>
       </c>
       <c r="L76" s="46" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="64.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="18" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B77" s="6" t="str">
         <f aca="false">A77</f>
         <v>T'Sou-ke Nation</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="G77" s="16" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="J77" s="0" t="n">
         <v>48.385518</v>
@@ -6133,12 +6135,12 @@
         <v>-123.696567</v>
       </c>
       <c r="L77" s="46" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="23" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B78" s="6" t="str">
         <f aca="false">A78</f>
@@ -6146,22 +6148,22 @@
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="11" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F78" s="65" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="G78" s="66" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="I78" s="12" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="J78" s="0" t="n">
         <v>50.678844</v>
@@ -6175,31 +6177,31 @@
     </row>
     <row r="79" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="23" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="I79" s="12" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="J79" s="0" t="n">
         <v>49.087557</v>
@@ -6213,32 +6215,32 @@
     </row>
     <row r="80" customFormat="false" ht="76.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="23" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B80" s="6" t="str">
         <f aca="false">A80</f>
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="E80" s="67" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="G80" s="17" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="I80" s="12" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="J80" s="0" t="n">
         <v>52.475488</v>
@@ -6252,26 +6254,26 @@
     </row>
     <row r="81" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="23" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="11" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G81" s="17" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="I81" s="19"/>
       <c r="J81" s="0" t="n">
@@ -6284,7 +6286,7 @@
     </row>
     <row r="82" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="23" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B82" s="6" t="str">
         <f aca="false">A82</f>
@@ -6292,20 +6294,20 @@
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="11" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="G82" s="17"/>
       <c r="H82" s="11" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="I82" s="12" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="J82" s="0" t="n">
         <v>50.167239</v>
@@ -6319,7 +6321,7 @@
     </row>
     <row r="83" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="59" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B83" s="6" t="str">
         <f aca="false">A83</f>
@@ -6329,22 +6331,22 @@
         <v>220</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="F83" s="11" t="s">
+        <v>624</v>
+      </c>
+      <c r="G83" s="68" t="s">
         <v>623</v>
       </c>
-      <c r="G83" s="68" t="s">
-        <v>622</v>
-      </c>
       <c r="H83" s="11" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="I83" s="19" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="J83" s="0" t="n">
         <v>49.462883</v>
@@ -6353,34 +6355,34 @@
         <v>-120.50172</v>
       </c>
       <c r="L83" s="17" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="18" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="11" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="G84" s="17" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="I84" s="12" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="J84" s="0" t="n">
         <v>51.194286</v>
@@ -6389,12 +6391,12 @@
         <v>-121.613314</v>
       </c>
       <c r="L84" s="13" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B85" s="6" t="str">
         <f aca="false">A85</f>
@@ -6402,18 +6404,18 @@
       </c>
       <c r="C85" s="6"/>
       <c r="D85" s="11" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="E85" s="11"/>
       <c r="F85" s="11" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="G85" s="17"/>
       <c r="H85" s="11" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="I85" s="12" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="J85" s="0" t="n">
         <v>52.10532</v>
@@ -6425,31 +6427,31 @@
     </row>
     <row r="86" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="23" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="I86" s="19" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="J86" s="0" t="n">
         <v>49.087557</v>
@@ -6458,35 +6460,35 @@
         <v>-121.829723</v>
       </c>
       <c r="L86" s="13" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="23" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B87" s="6" t="str">
         <f aca="false">A87</f>
-        <v>Yale First Nation </v>
+        <v>Yale First Nation</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="11" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="I87" s="12" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="J87" s="0" t="n">
         <v>49.492718</v>
@@ -6500,7 +6502,7 @@
     </row>
     <row r="88" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="23" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B88" s="6" t="str">
         <f aca="false">A88</f>
@@ -6508,22 +6510,22 @@
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="11" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="F88" s="63" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G88" s="17" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="J88" s="0" t="n">
         <v>52.854978</v>
@@ -6548,7 +6550,7 @@
     </row>
     <row r="90" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="23" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B90" s="23"/>
       <c r="C90" s="23"/>
@@ -6558,7 +6560,7 @@
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
@@ -6567,7 +6569,7 @@
     </row>
     <row r="92" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
@@ -6576,7 +6578,7 @@
     </row>
     <row r="93" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="11" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
@@ -6698,7 +6700,7 @@
       <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.31"/>
@@ -6709,13 +6711,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C1" s="75" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6727,10 +6729,10 @@
         <v>13</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D2" s="77" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6742,10 +6744,10 @@
         <v>22</v>
       </c>
       <c r="C3" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6757,10 +6759,10 @@
         <v>32</v>
       </c>
       <c r="C4" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D4" s="75" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6772,10 +6774,10 @@
         <v>40</v>
       </c>
       <c r="C5" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D5" s="78" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6787,10 +6789,10 @@
         <v>47</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D6" s="75" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6802,10 +6804,10 @@
         <v>54</v>
       </c>
       <c r="C7" s="76" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D7" s="75" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6817,10 +6819,10 @@
         <v>62</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6829,28 +6831,28 @@
         <v>Chi:yo:m Agassiz (Cheam) First Nation - meaning "Wild Strawberry Place"</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C9" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D9" s="75" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
         <f aca="false">'BC First Nations'!A11</f>
-        <v>Coldwater First Nation (Nc/etko - the people of the creeks)      </v>
+        <v>Coldwater First Nation (Nc/etko - the people of the creeks)</v>
       </c>
       <c r="B10" s="75" t="s">
         <v>81</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D10" s="75" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6859,13 +6861,13 @@
         <v>Cook's Ferry Indian Band Kumcheen (Variation Nkumcheen); Includes Pokheistk (Variation Pakeist, Pokheistsk), Pemynoos (Variation Piminos), Spatsum (Variation Spaptsin), Spence'S Bridge</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C11" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D11" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6877,10 +6879,10 @@
         <v>95</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D12" s="75" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6892,10 +6894,10 @@
         <v>105</v>
       </c>
       <c r="C13" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D13" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6907,25 +6909,25 @@
         <v>115</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D14" s="78" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="str">
         <f aca="false">'BC First Nations'!A16</f>
-        <v>Halalt First Nation </v>
+        <v>Halalt First Nation</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D15" s="75" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6937,25 +6939,25 @@
         <v>130</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D16" s="75" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="str">
         <f aca="false">'BC First Nations'!A18</f>
-        <v>Huu-ay-aht First Nation </v>
+        <v>Huu-ay-aht First Nation</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="D17" s="75" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6967,10 +6969,10 @@
         <v>144</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D18" s="75" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6982,25 +6984,25 @@
         <v>152</v>
       </c>
       <c r="C19" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D19" s="75" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="str">
         <f aca="false">'BC First Nations'!A21</f>
-        <v>Kwaw -Kwaw-Aplit First Nations </v>
+        <v>Kwaw -Kwaw-Aplit First Nations</v>
       </c>
       <c r="B20" s="75" t="s">
         <v>161</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D20" s="75" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7012,10 +7014,10 @@
         <v>168</v>
       </c>
       <c r="C21" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D21" s="75" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7027,10 +7029,10 @@
         <v>177</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D22" s="75" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7042,10 +7044,10 @@
         <v>186</v>
       </c>
       <c r="C23" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D23" s="75" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7057,10 +7059,10 @@
         <v>193</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D24" s="75" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7072,10 +7074,10 @@
         <v>203</v>
       </c>
       <c r="C25" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D25" s="75" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7087,10 +7089,10 @@
         <v>211</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D26" s="75" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7102,10 +7104,10 @@
         <v>218</v>
       </c>
       <c r="C27" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D27" s="75" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7117,10 +7119,10 @@
         <v>226</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D28" s="75" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7132,10 +7134,10 @@
         <v>234</v>
       </c>
       <c r="C29" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D29" s="75" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7147,10 +7149,10 @@
         <v>242</v>
       </c>
       <c r="C30" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D30" s="75" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7162,10 +7164,10 @@
         <v>249</v>
       </c>
       <c r="C31" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D31" s="78" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7177,10 +7179,10 @@
         <v>258</v>
       </c>
       <c r="C32" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D32" s="75" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7192,10 +7194,10 @@
         <v>265</v>
       </c>
       <c r="C33" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D33" s="75" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7207,10 +7209,10 @@
         <v>274</v>
       </c>
       <c r="C34" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D34" s="75" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7222,10 +7224,10 @@
         <v>281</v>
       </c>
       <c r="C35" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D35" s="75" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7237,10 +7239,10 @@
         <v>288</v>
       </c>
       <c r="C36" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D36" s="78" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7252,10 +7254,10 @@
         <v>295</v>
       </c>
       <c r="C37" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D37" s="75" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7267,10 +7269,10 @@
         <v>301</v>
       </c>
       <c r="C38" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D38" s="75" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7282,10 +7284,10 @@
         <v>309</v>
       </c>
       <c r="C39" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D39" s="75" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7297,25 +7299,25 @@
         <v>317</v>
       </c>
       <c r="C40" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D40" s="75" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="str">
         <f aca="false">'BC First Nations'!A42</f>
-        <v>Qayqayt First Nation (New Westminister) </v>
+        <v>Qayqayt First Nation (New Westminister)</v>
       </c>
       <c r="B41" s="75" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C41" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D41" s="78" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7327,10 +7329,10 @@
         <v>330</v>
       </c>
       <c r="C42" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D42" s="75" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7342,10 +7344,10 @@
         <v>338</v>
       </c>
       <c r="C43" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D43" s="75" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7357,10 +7359,10 @@
         <v>346</v>
       </c>
       <c r="C44" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D44" s="75" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7372,10 +7374,10 @@
         <v>351</v>
       </c>
       <c r="C45" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D45" s="78" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7387,25 +7389,25 @@
         <v>357</v>
       </c>
       <c r="C46" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D46" s="78" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="str">
         <f aca="false">'BC First Nations'!A48</f>
-        <v>Shackan Indian Band </v>
+        <v>Shackan Indian Band</v>
       </c>
       <c r="B47" s="75" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C47" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D47" s="78" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7417,10 +7419,10 @@
         <v>370</v>
       </c>
       <c r="C48" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D48" s="75" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7432,10 +7434,10 @@
         <v>378</v>
       </c>
       <c r="C49" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D49" s="75" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7447,10 +7449,10 @@
         <v>386</v>
       </c>
       <c r="C50" s="75" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="D50" s="75" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7462,25 +7464,25 @@
         <v>393</v>
       </c>
       <c r="C51" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D51" s="75" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="str">
         <f aca="false">'BC First Nations'!A53</f>
-        <v>Skuppah Indian Band </v>
+        <v>Skuppah Indian Band</v>
       </c>
       <c r="B52" s="75" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C52" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D52" s="78" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7492,25 +7494,25 @@
         <v>406</v>
       </c>
       <c r="C53" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D53" s="75" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="str">
         <f aca="false">'BC First Nations'!A55</f>
-        <v>Shuswap Indian Band </v>
+        <v>Shuswap Indian Band</v>
       </c>
       <c r="B54" s="75" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C54" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D54" s="75" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7522,10 +7524,10 @@
         <v>422</v>
       </c>
       <c r="C55" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D55" s="75" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7537,10 +7539,10 @@
         <v>429</v>
       </c>
       <c r="C56" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D56" s="75" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7552,10 +7554,10 @@
         <v>436</v>
       </c>
       <c r="C57" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D57" s="75" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7567,10 +7569,10 @@
         <v>443</v>
       </c>
       <c r="C58" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D58" s="75" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7582,10 +7584,10 @@
         <v>450</v>
       </c>
       <c r="C59" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D59" s="78" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7597,10 +7599,10 @@
         <v>459</v>
       </c>
       <c r="C60" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D60" s="75" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7612,40 +7614,40 @@
         <v>467</v>
       </c>
       <c r="C61" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D61" s="75" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="str">
         <f aca="false">'BC First Nations'!A63</f>
-        <v>Stk'emlupsemc Te Secwepemc </v>
+        <v>Stk'emlupsemc Te Secwepemc</v>
       </c>
       <c r="B62" s="75" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C62" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D62" s="75" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="str">
         <f aca="false">'BC First Nations'!A64</f>
-        <v>Sts'ailes Band (Chehalls Indian Band) </v>
+        <v>Sts'ailes Band (Chehalls Indian Band)</v>
       </c>
       <c r="B63" s="75" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C63" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D63" s="75" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7654,13 +7656,13 @@
         <v>Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek)</v>
       </c>
       <c r="B64" s="75" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C64" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D64" s="75" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7669,13 +7671,13 @@
         <v>St'uxwtews (Bonaparte Indian Band)</v>
       </c>
       <c r="B65" s="75" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C65" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D65" s="75" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7684,13 +7686,13 @@
         <v>Stz'uminus First Nation (ltst uw' hw-nuts'-ul-wun) Chemainus</v>
       </c>
       <c r="B66" s="75" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C66" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D66" s="75" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7699,13 +7701,13 @@
         <v>Sumas First Nation</v>
       </c>
       <c r="B67" s="75" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C67" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D67" s="75" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7714,13 +7716,13 @@
         <v>Toosey Indian Band (Tl'esqox)</v>
       </c>
       <c r="B68" s="75" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C68" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D68" s="78" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7729,13 +7731,13 @@
         <v>Tsartlip First Nation</v>
       </c>
       <c r="B69" s="75" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C69" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D69" s="78" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7744,13 +7746,13 @@
         <v>Tsawout First Nation</v>
       </c>
       <c r="B70" s="75" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C70" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D70" s="78" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7759,13 +7761,13 @@
         <v>Tsawwassen First Nation</v>
       </c>
       <c r="B71" s="75" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C71" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D71" s="78" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7774,13 +7776,13 @@
         <v>Ts'elxweyeqw Tribe Management Limited</v>
       </c>
       <c r="B72" s="75" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C72" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D72" s="75" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7789,13 +7791,13 @@
         <v>Tseycum First Nation</v>
       </c>
       <c r="B73" s="75" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C73" s="75" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="D73" s="78" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7804,13 +7806,13 @@
         <v>Ts'kwaylaxw (Pavillion Indian Band)</v>
       </c>
       <c r="B74" s="75" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C74" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D74" s="75" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7819,13 +7821,13 @@
         <v>Tsleil Waututh Nation</v>
       </c>
       <c r="B75" s="75" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C75" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D75" s="75" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7834,13 +7836,13 @@
         <v>T'Sou-ke Nation</v>
       </c>
       <c r="B76" s="75" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C76" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D76" s="75" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7849,13 +7851,13 @@
         <v>Tk'emlups te Secwepemc</v>
       </c>
       <c r="B77" s="75" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C77" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D77" s="75" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7864,13 +7866,13 @@
         <v>Tzeachten First Nation</v>
       </c>
       <c r="B78" s="75" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C78" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D78" s="75" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7879,13 +7881,13 @@
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
       <c r="B79" s="75" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C79" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D79" s="75" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7894,13 +7896,13 @@
         <v>Union Bar First Nations</v>
       </c>
       <c r="B80" s="75" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C80" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D80" s="75" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7909,13 +7911,13 @@
         <v>Upper Nicola Indian Band</v>
       </c>
       <c r="B81" s="75" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C81" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D81" s="75" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7924,13 +7926,13 @@
         <v>Upper Similkameen Indian Band</v>
       </c>
       <c r="B82" s="75" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C82" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D82" s="75" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7939,13 +7941,13 @@
         <v>Whispering Pines/Clinton Indian Bands</v>
       </c>
       <c r="B83" s="75" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C83" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D83" s="75" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7954,13 +7956,13 @@
         <v>Williams Lake Indian Band</v>
       </c>
       <c r="B84" s="75" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C84" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D84" s="75" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7969,28 +7971,28 @@
         <v>Yakweakwioose First Nation</v>
       </c>
       <c r="B85" s="75" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C85" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D85" s="75" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="str">
         <f aca="false">'BC First Nations'!A87</f>
-        <v>Yale First Nation </v>
+        <v>Yale First Nation</v>
       </c>
       <c r="B86" s="75" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C86" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D86" s="75" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7999,13 +8001,13 @@
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
       <c r="B87" s="75" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C87" s="75" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D87" s="75" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="G87" s="75"/>
     </row>

</xml_diff>

<commit_message>
added more digital territories and added better territory styles and tooltip
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="771">
   <si>
     <t xml:space="preserve">TRANSMOUNTAIN EXPANSION PROJECT - INDIGENOUS COMMUNITIES _IMC </t>
   </si>
@@ -499,6 +499,9 @@
     <t xml:space="preserve">Vancouver Island</t>
   </si>
   <si>
+    <t xml:space="preserve">ditidaht</t>
+  </si>
+  <si>
     <t xml:space="preserve">Esquimalt Nation (Xwsepsum or Kosapsum)</t>
   </si>
   <si>
@@ -565,6 +568,9 @@
     <t xml:space="preserve">http://www.heiltsuknation.ca/</t>
   </si>
   <si>
+    <t xml:space="preserve">heiltsuk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huu-ay-aht First Nation </t>
   </si>
   <si>
@@ -613,6 +619,9 @@
     <t xml:space="preserve">Spread 6 (KP 1075.1 to 1144.480)</t>
   </si>
   <si>
+    <t xml:space="preserve">katzie</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kwantlen First Nation (tireless Runner)</t>
   </si>
   <si>
@@ -689,6 +698,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lower Mainland - Spread 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kwikwetlem</t>
   </si>
   <si>
     <t xml:space="preserve">Leq' a: mel First Nation</t>
@@ -1044,6 +1056,9 @@
     <t xml:space="preserve">http://pacheedahtfirstnation.com/</t>
   </si>
   <si>
+    <t xml:space="preserve">pacheedaht</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pauquachin Nation</t>
   </si>
   <si>
@@ -1180,6 +1195,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lower Mainland Spread 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qayqayt</t>
   </si>
   <si>
     <t xml:space="preserve">Scia'new First Nation (Beecher Bay First Nation)</t>
@@ -1905,6 +1923,9 @@
     <t xml:space="preserve">Lower Mainland</t>
   </si>
   <si>
+    <t xml:space="preserve">tsawwassen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ts'elxweyeqw Tribe Management Limited</t>
   </si>
   <si>
@@ -1992,6 +2013,9 @@
   </si>
   <si>
     <t xml:space="preserve">Spread 7 Lower Mainland (KP 1180.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tsleil-waututh-səl̓ilwətaɂɬ</t>
   </si>
   <si>
     <t xml:space="preserve">T'Sou-ke Nation</t>
@@ -3306,8 +3330,8 @@
   </sheetPr>
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H70" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N77" activeCellId="0" sqref="N77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3816,34 +3840,37 @@
       <c r="L14" s="17" t="s">
         <v>115</v>
       </c>
+      <c r="M14" s="0" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F15" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>120</v>
-      </c>
       <c r="H15" s="11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>48.688573</v>
@@ -3857,32 +3884,32 @@
     </row>
     <row r="16" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B16" s="6" t="str">
         <f aca="false">A16</f>
         <v>Halalt First Nation</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>48.929783</v>
@@ -3896,28 +3923,28 @@
     </row>
     <row r="17" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B17" s="6" t="str">
         <f aca="false">A17</f>
         <v>Heiltsuk First Nation</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>52.337794</v>
@@ -3928,34 +3955,37 @@
       <c r="L17" s="17" t="s">
         <v>115</v>
       </c>
+      <c r="M17" s="0" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>48.833479</v>
@@ -3964,34 +3994,34 @@
         <v>-124.929585</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B19" s="6" t="str">
         <f aca="false">A19</f>
         <v>Katzie First Nation</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I19" s="12"/>
       <c r="J19" s="0" t="n">
@@ -4001,34 +4031,37 @@
         <v>-122.607872</v>
       </c>
       <c r="L19" s="17" t="s">
-        <v>153</v>
+        <v>155</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="50.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="11" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>49.476845</v>
@@ -4037,33 +4070,33 @@
         <v>-122.296959</v>
       </c>
       <c r="L20" s="17" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="I21" s="19"/>
       <c r="J21" s="0" t="n">
@@ -4073,37 +4106,37 @@
         <v>-121.756432</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="30" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B22" s="6" t="str">
         <f aca="false">A22</f>
         <v>Kwikwetlem First Nation</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>49.451741</v>
@@ -4112,36 +4145,39 @@
         <v>-122.657791</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>179</v>
+        <v>182</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="33" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="J23" s="11" t="n">
         <v>49.348358</v>
@@ -4150,34 +4186,34 @@
         <v>-122.106774</v>
       </c>
       <c r="L23" s="17" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="34" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="35" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>51.287872</v>
@@ -4191,31 +4227,31 @@
     </row>
     <row r="25" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="30" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>53.944696</v>
@@ -4224,12 +4260,12 @@
         <v>-121.694171</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B26" s="6" t="str">
         <f aca="false">A26</f>
@@ -4237,22 +4273,22 @@
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="11" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>52.953049</v>
@@ -4266,29 +4302,29 @@
     </row>
     <row r="27" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="11" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>50.006984</v>
@@ -4302,28 +4338,28 @@
     </row>
     <row r="28" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="I28" s="19"/>
       <c r="J28" s="0" t="n">
@@ -4338,32 +4374,32 @@
     </row>
     <row r="29" customFormat="false" ht="56.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="37" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B29" s="6" t="str">
         <f aca="false">A29</f>
         <v>Lyackson First Nation</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>48.941803</v>
@@ -4375,32 +4411,32 @@
     </row>
     <row r="30" customFormat="false" ht="49.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B30" s="6" t="str">
         <f aca="false">A30</f>
         <v>Malahat First Nation</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>48.655944</v>
@@ -4409,34 +4445,34 @@
         <v>-124.000524</v>
       </c>
       <c r="L30" s="38" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="39" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="B31" s="6" t="str">
         <f aca="false">A31</f>
         <v>Matsqui First Nation</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="0" t="n">
@@ -4446,36 +4482,36 @@
         <v>-122.361868</v>
       </c>
       <c r="L31" s="38" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="79.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>49.353225</v>
@@ -4484,37 +4520,37 @@
         <v>-123.012956</v>
       </c>
       <c r="L32" s="38" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="18" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B33" s="6" t="str">
         <f aca="false">A33</f>
         <v>Neskonlith Indian Band</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>51.21274</v>
@@ -4528,32 +4564,32 @@
     </row>
     <row r="34" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B34" s="6" t="str">
         <f aca="false">A34</f>
         <v>Nooaitch Indian Band</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>49.690318</v>
@@ -4562,35 +4598,35 @@
         <v>-120.648292</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="42" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B35" s="6" t="str">
         <f aca="false">A35</f>
         <v>Osoyoos</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="F35" s="36" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="G35" s="43"/>
       <c r="H35" s="11" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>49.114526</v>
@@ -4599,37 +4635,37 @@
         <v>-118.489264</v>
       </c>
       <c r="L35" s="17" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B36" s="6" t="str">
         <f aca="false">A36</f>
         <v>Pacheedaht First Nation</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>48.572918</v>
@@ -4638,34 +4674,37 @@
         <v>-124.39459</v>
       </c>
       <c r="L36" s="17" t="s">
-        <v>179</v>
+        <v>182</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="B37" s="6" t="str">
         <f aca="false">A37</f>
         <v>Pauquachin Nation</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="I37" s="19"/>
       <c r="J37" s="0" t="n">
@@ -4675,12 +4714,12 @@
         <v>-123.324246</v>
       </c>
       <c r="L37" s="17" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="B38" s="6" t="str">
         <f aca="false">A38</f>
@@ -4688,22 +4727,22 @@
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="11" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>49.732366</v>
@@ -4712,34 +4751,34 @@
         <v>-119.25376</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="18" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="11" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>49.505163</v>
@@ -4748,37 +4787,37 @@
         <v>-121.482617</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="18" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="B40" s="6" t="str">
         <f aca="false">A40</f>
         <v>Penelakut Tribe</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>48.892388</v>
@@ -4787,12 +4826,12 @@
         <v>-123.675652</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="18" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="B41" s="6" t="str">
         <f aca="false">A41</f>
@@ -4800,19 +4839,19 @@
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="15" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="I41" s="19"/>
       <c r="J41" s="0" t="n">
@@ -4822,33 +4861,33 @@
         <v>-121.506875</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="127.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="I42" s="19"/>
       <c r="J42" s="0" t="n">
@@ -4858,34 +4897,37 @@
         <v>-122.910944</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>332</v>
+        <v>337</v>
+      </c>
+      <c r="M42" s="0" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="98.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="44" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="15" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>48.440888</v>
@@ -4894,36 +4936,36 @@
         <v>-123.676887</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="45" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>49.25517</v>
@@ -4932,12 +4974,12 @@
         <v>-121.964821</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="44" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="B45" s="6" t="str">
         <f aca="false">A45</f>
@@ -4945,19 +4987,19 @@
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="15" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="I45" s="19"/>
       <c r="J45" s="0" t="n">
@@ -4967,32 +5009,32 @@
         <v>-121.724003</v>
       </c>
       <c r="L45" s="46" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="151.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="21" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="47" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="G46" s="48"/>
       <c r="H46" s="49" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="J46" s="2" t="n">
         <v>51.527017</v>
@@ -5009,26 +5051,26 @@
     </row>
     <row r="47" customFormat="false" ht="80.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="21" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B47" s="6" t="str">
         <f aca="false">A47</f>
         <v>Semiahmoo First Nation</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="I47" s="19"/>
       <c r="J47" s="0" t="n">
@@ -5038,37 +5080,37 @@
         <v>-122.767315</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="M47" s="0" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="111.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="44" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="B48" s="51" t="s">
         <v>42</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="G48" s="48"/>
       <c r="H48" s="11" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>49.963059</v>
@@ -5082,31 +5124,31 @@
     </row>
     <row r="49" customFormat="false" ht="80.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="52" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="D49" s="53" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="H49" s="54" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>49.339668</v>
@@ -5115,34 +5157,34 @@
         <v>-121.60638</v>
       </c>
       <c r="L49" s="46" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="55" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="D50" s="56" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="G50" s="48"/>
       <c r="H50" s="57" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="J50" s="0" t="n">
         <v>49.087557</v>
@@ -5156,31 +5198,31 @@
     </row>
     <row r="51" customFormat="false" ht="51.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="44" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="G51" s="50" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="H51" s="58" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="J51" s="0" t="n">
         <v>52.634393</v>
@@ -5194,29 +5236,29 @@
     </row>
     <row r="52" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="21" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="B52" s="6" t="str">
         <f aca="false">A52</f>
         <v>Siska Indian Band</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="I52" s="19"/>
       <c r="J52" s="0" t="n">
@@ -5226,33 +5268,33 @@
         <v>-120.838519</v>
       </c>
       <c r="L52" s="13" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="21" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="B53" s="51" t="s">
         <v>42</v>
       </c>
       <c r="C53" s="51" t="s">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="G53" s="16" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="I53" s="19"/>
       <c r="J53" s="0" t="n">
@@ -5262,36 +5304,36 @@
         <v>-121.484624</v>
       </c>
       <c r="L53" s="13" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="21" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="J54" s="0" t="n">
         <v>49.087557</v>
@@ -5305,32 +5347,32 @@
     </row>
     <row r="55" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="23" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="B55" s="6" t="str">
         <f aca="false">A55</f>
         <v>Shuswap Indian Band</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="J55" s="0" t="n">
         <v>50.367907</v>
@@ -5344,32 +5386,32 @@
     </row>
     <row r="56" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="23" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="B56" s="6" t="str">
         <f aca="false">A56</f>
         <v>Skawahlook First Nation</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="J56" s="0" t="n">
         <v>49.227586</v>
@@ -5378,37 +5420,37 @@
         <v>-122.174045</v>
       </c>
       <c r="L56" s="13" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="59" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="B57" s="6" t="str">
         <f aca="false">A57</f>
         <v>Skwah First Nation</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="J57" s="0" t="n">
         <v>49.175281</v>
@@ -5422,32 +5464,32 @@
     </row>
     <row r="58" customFormat="false" ht="51.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="18" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="B58" s="6" t="str">
         <f aca="false">A58</f>
         <v>Snuneymuxw First Nation</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="J58" s="0" t="n">
         <v>49.107871</v>
@@ -5461,31 +5503,31 @@
     </row>
     <row r="59" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="23" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>449</v>
+        <v>455</v>
       </c>
       <c r="E59" s="41" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="G59" s="27" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="J59" s="0" t="n">
         <v>49.087557</v>
@@ -5499,29 +5541,29 @@
     </row>
     <row r="60" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="59" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="11" t="s">
-        <v>456</v>
+        <v>462</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="J60" s="0" t="n">
         <v>49.963059</v>
@@ -5530,34 +5572,34 @@
         <v>-121.484624</v>
       </c>
       <c r="L60" s="13" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="61" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="G61" s="17"/>
       <c r="H61" s="11" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J61" s="0" t="n">
         <v>49.807197</v>
@@ -5566,36 +5608,36 @@
         <v>-123.200082</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="61" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="J62" s="0" t="n">
         <v>49.087557</v>
@@ -5609,29 +5651,29 @@
     </row>
     <row r="63" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="18" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63" s="36" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="J63" s="0" t="n">
         <v>51.341443</v>
@@ -5645,31 +5687,31 @@
     </row>
     <row r="64" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="23" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="G64" s="17" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="J64" s="0" t="n">
         <v>49.293578</v>
@@ -5683,31 +5725,31 @@
     </row>
     <row r="65" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="21" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="J65" s="0" t="n">
         <v>51.586232</v>
@@ -5721,29 +5763,29 @@
     </row>
     <row r="66" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="62" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="G66" s="17"/>
       <c r="H66" s="11" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="J66" s="0" t="n">
         <v>50.839863</v>
@@ -5757,29 +5799,29 @@
     </row>
     <row r="67" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="44" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="63" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="G67" s="17" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="J67" s="0" t="n">
         <v>48.846385</v>
@@ -5793,7 +5835,7 @@
     </row>
     <row r="68" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="23" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="B68" s="6" t="str">
         <f aca="false">A68</f>
@@ -5801,22 +5843,22 @@
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="0" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="G68" s="17" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="J68" s="0" t="n">
         <v>49.052587</v>
@@ -5830,7 +5872,7 @@
     </row>
     <row r="69" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="59" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="B69" s="6" t="str">
         <f aca="false">A69</f>
@@ -5838,19 +5880,19 @@
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="11" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="G69" s="17" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="I69" s="19"/>
       <c r="J69" s="0" t="n">
@@ -5865,31 +5907,31 @@
     </row>
     <row r="70" customFormat="false" ht="58.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="18" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="F70" s="11" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="G70" s="17" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="J70" s="0" t="n">
         <v>48.724102</v>
@@ -5898,36 +5940,36 @@
         <v>-123.324246</v>
       </c>
       <c r="L70" s="46" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="61" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c r="I71" s="12" t="s">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="J71" s="0" t="n">
         <v>48.724102</v>
@@ -5936,37 +5978,37 @@
         <v>-123.324246</v>
       </c>
       <c r="L71" s="46" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="18" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="B72" s="6" t="str">
         <f aca="false">A72</f>
         <v>Tsawwassen First Nation</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="G72" s="17" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="J72" s="0" t="n">
         <v>49.042909</v>
@@ -5975,31 +6017,34 @@
         <v>-123.094409</v>
       </c>
       <c r="L72" s="46" t="s">
-        <v>551</v>
+        <v>557</v>
+      </c>
+      <c r="M72" s="0" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="44" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="11" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="G73" s="64" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>557</v>
+        <v>564</v>
       </c>
       <c r="I73" s="12"/>
       <c r="J73" s="0" t="n">
@@ -6014,31 +6059,31 @@
     </row>
     <row r="74" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="23" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="J74" s="0" t="n">
         <v>48.724102</v>
@@ -6047,31 +6092,31 @@
         <v>-123.324246</v>
       </c>
       <c r="L74" s="46" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="59" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="G75" s="17"/>
       <c r="H75" s="11" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="J75" s="0" t="n">
         <v>50.883097</v>
@@ -6085,32 +6130,32 @@
     </row>
     <row r="76" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="B76" s="6" t="str">
         <f aca="false">A76</f>
         <v>Tsleil Waututh Nation</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>577</v>
+        <v>584</v>
       </c>
       <c r="G76" s="17" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
       <c r="I76" s="12" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="J76" s="0" t="n">
         <v>49.309839</v>
@@ -6119,37 +6164,40 @@
         <v>-122.980478</v>
       </c>
       <c r="L76" s="46" t="s">
-        <v>580</v>
+        <v>587</v>
+      </c>
+      <c r="M76" s="0" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="64.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="18" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="B77" s="6" t="str">
         <f aca="false">A77</f>
         <v>T'Sou-ke Nation</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="G77" s="16" t="s">
-        <v>586</v>
+        <v>594</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>588</v>
+        <v>596</v>
       </c>
       <c r="J77" s="0" t="n">
         <v>48.385518</v>
@@ -6158,12 +6206,12 @@
         <v>-123.696567</v>
       </c>
       <c r="L77" s="46" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="23" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="B78" s="6" t="str">
         <f aca="false">A78</f>
@@ -6171,22 +6219,22 @@
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="11" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>591</v>
+        <v>599</v>
       </c>
       <c r="F78" s="65" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="G78" s="66" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="I78" s="12" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="J78" s="0" t="n">
         <v>50.678844</v>
@@ -6200,31 +6248,31 @@
     </row>
     <row r="79" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="23" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>597</v>
+        <v>605</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="I79" s="12" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="J79" s="0" t="n">
         <v>49.087557</v>
@@ -6238,32 +6286,32 @@
     </row>
     <row r="80" customFormat="false" ht="76.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="23" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="B80" s="6" t="str">
         <f aca="false">A80</f>
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>605</v>
+        <v>613</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="E80" s="67" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="G80" s="17" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="I80" s="12" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="J80" s="0" t="n">
         <v>52.475488</v>
@@ -6272,31 +6320,31 @@
         <v>-125.301018</v>
       </c>
       <c r="L80" s="46" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="23" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="11" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="G81" s="17" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="I81" s="19"/>
       <c r="J81" s="0" t="n">
@@ -6309,7 +6357,7 @@
     </row>
     <row r="82" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="23" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="B82" s="6" t="str">
         <f aca="false">A82</f>
@@ -6317,20 +6365,20 @@
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="11" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="G82" s="17"/>
       <c r="H82" s="11" t="s">
-        <v>623</v>
+        <v>631</v>
       </c>
       <c r="I82" s="12" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="J82" s="0" t="n">
         <v>50.167239</v>
@@ -6344,32 +6392,32 @@
     </row>
     <row r="83" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="59" t="s">
-        <v>625</v>
+        <v>633</v>
       </c>
       <c r="B83" s="6" t="str">
         <f aca="false">A83</f>
         <v>Upper Similkameen Indian Band</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>628</v>
+        <v>636</v>
       </c>
       <c r="G83" s="68" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>629</v>
+        <v>637</v>
       </c>
       <c r="I83" s="19" t="s">
-        <v>630</v>
+        <v>638</v>
       </c>
       <c r="J83" s="0" t="n">
         <v>49.462883</v>
@@ -6378,34 +6426,34 @@
         <v>-120.50172</v>
       </c>
       <c r="L83" s="17" t="s">
-        <v>631</v>
+        <v>639</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="18" t="s">
-        <v>632</v>
+        <v>640</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>633</v>
+        <v>641</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="11" t="s">
-        <v>634</v>
+        <v>642</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>636</v>
+        <v>644</v>
       </c>
       <c r="G84" s="17" t="s">
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>638</v>
+        <v>646</v>
       </c>
       <c r="I84" s="12" t="s">
-        <v>639</v>
+        <v>647</v>
       </c>
       <c r="J84" s="0" t="n">
         <v>51.194286</v>
@@ -6414,12 +6462,12 @@
         <v>-121.613314</v>
       </c>
       <c r="L84" s="13" t="s">
-        <v>640</v>
+        <v>648</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>641</v>
+        <v>649</v>
       </c>
       <c r="B85" s="6" t="str">
         <f aca="false">A85</f>
@@ -6427,18 +6475,18 @@
       </c>
       <c r="C85" s="6"/>
       <c r="D85" s="11" t="s">
-        <v>642</v>
+        <v>650</v>
       </c>
       <c r="E85" s="11"/>
       <c r="F85" s="11" t="s">
-        <v>643</v>
+        <v>651</v>
       </c>
       <c r="G85" s="17"/>
       <c r="H85" s="11" t="s">
-        <v>644</v>
+        <v>652</v>
       </c>
       <c r="I85" s="12" t="s">
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="J85" s="0" t="n">
         <v>52.10532</v>
@@ -6450,31 +6498,31 @@
     </row>
     <row r="86" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="23" t="s">
-        <v>646</v>
+        <v>654</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>647</v>
+        <v>655</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>648</v>
+        <v>656</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>649</v>
+        <v>657</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>650</v>
+        <v>658</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>651</v>
+        <v>659</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>652</v>
+        <v>660</v>
       </c>
       <c r="I86" s="19" t="s">
-        <v>653</v>
+        <v>661</v>
       </c>
       <c r="J86" s="0" t="n">
         <v>49.087557</v>
@@ -6483,12 +6531,12 @@
         <v>-121.829723</v>
       </c>
       <c r="L86" s="13" t="s">
-        <v>640</v>
+        <v>648</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="23" t="s">
-        <v>654</v>
+        <v>662</v>
       </c>
       <c r="B87" s="6" t="str">
         <f aca="false">A87</f>
@@ -6496,22 +6544,22 @@
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="11" t="s">
-        <v>655</v>
+        <v>663</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>656</v>
+        <v>664</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>657</v>
+        <v>665</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>659</v>
+        <v>667</v>
       </c>
       <c r="I87" s="12" t="s">
-        <v>660</v>
+        <v>668</v>
       </c>
       <c r="J87" s="0" t="n">
         <v>49.492718</v>
@@ -6520,12 +6568,12 @@
         <v>-121.423097</v>
       </c>
       <c r="L87" s="13" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="23" t="s">
-        <v>661</v>
+        <v>669</v>
       </c>
       <c r="B88" s="6" t="str">
         <f aca="false">A88</f>
@@ -6533,22 +6581,22 @@
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="11" t="s">
-        <v>662</v>
+        <v>670</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>663</v>
+        <v>671</v>
       </c>
       <c r="F88" s="63" t="s">
-        <v>664</v>
+        <v>672</v>
       </c>
       <c r="G88" s="17" t="s">
-        <v>665</v>
+        <v>673</v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>666</v>
+        <v>674</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>667</v>
+        <v>675</v>
       </c>
       <c r="J88" s="0" t="n">
         <v>52.854978</v>
@@ -6573,7 +6621,7 @@
     </row>
     <row r="90" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="23" t="s">
-        <v>668</v>
+        <v>676</v>
       </c>
       <c r="B90" s="23"/>
       <c r="C90" s="23"/>
@@ -6583,7 +6631,7 @@
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="s">
-        <v>669</v>
+        <v>677</v>
       </c>
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
@@ -6592,7 +6640,7 @@
     </row>
     <row r="92" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
@@ -6601,7 +6649,7 @@
     </row>
     <row r="93" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="11" t="s">
-        <v>671</v>
+        <v>679</v>
       </c>
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
@@ -6734,13 +6782,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>672</v>
+        <v>680</v>
       </c>
       <c r="C1" s="75" t="s">
-        <v>673</v>
+        <v>681</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>674</v>
+        <v>682</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6752,10 +6800,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D2" s="77" t="s">
-        <v>676</v>
+        <v>684</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6767,10 +6815,10 @@
         <v>24</v>
       </c>
       <c r="C3" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6782,10 +6830,10 @@
         <v>34</v>
       </c>
       <c r="C4" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D4" s="75" t="s">
-        <v>679</v>
+        <v>687</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6797,10 +6845,10 @@
         <v>42</v>
       </c>
       <c r="C5" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D5" s="78" t="s">
-        <v>680</v>
+        <v>688</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6812,10 +6860,10 @@
         <v>49</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D6" s="75" t="s">
-        <v>681</v>
+        <v>689</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6827,10 +6875,10 @@
         <v>56</v>
       </c>
       <c r="C7" s="76" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D7" s="75" t="s">
-        <v>682</v>
+        <v>690</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6842,10 +6890,10 @@
         <v>64</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>683</v>
+        <v>691</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6854,13 +6902,13 @@
         <v>Chi:yo:m Agassiz (Cheam) First Nation - meaning "Wild Strawberry Place"</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
       <c r="C9" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D9" s="75" t="s">
-        <v>685</v>
+        <v>693</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6872,10 +6920,10 @@
         <v>83</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D10" s="75" t="s">
-        <v>686</v>
+        <v>694</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6884,13 +6932,13 @@
         <v>Cook's Ferry Indian Band Kumcheen (Variation Nkumcheen); Includes Pokheistk (Variation Pakeist, Pokheistsk), Pemynoos (Variation Piminos), Spatsum (Variation Spaptsin), Spence'S Bridge</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>687</v>
+        <v>695</v>
       </c>
       <c r="C11" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D11" s="75" t="s">
-        <v>688</v>
+        <v>696</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6902,10 +6950,10 @@
         <v>97</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D12" s="75" t="s">
-        <v>689</v>
+        <v>697</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6917,10 +6965,10 @@
         <v>107</v>
       </c>
       <c r="C13" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D13" s="75" t="s">
-        <v>690</v>
+        <v>698</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6929,13 +6977,13 @@
         <v>Esquimalt Nation (Xwsepsum or Kosapsum)</v>
       </c>
       <c r="B14" s="75" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D14" s="78" t="s">
-        <v>691</v>
+        <v>699</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6944,13 +6992,13 @@
         <v>Halalt First Nation</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>692</v>
+        <v>700</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D15" s="75" t="s">
-        <v>693</v>
+        <v>701</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6959,13 +7007,13 @@
         <v>Heiltsuk First Nation</v>
       </c>
       <c r="B16" s="75" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D16" s="75" t="s">
-        <v>694</v>
+        <v>702</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6974,13 +7022,13 @@
         <v>Huu-ay-aht First Nation</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>695</v>
+        <v>703</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>696</v>
+        <v>704</v>
       </c>
       <c r="D17" s="75" t="s">
-        <v>697</v>
+        <v>705</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6989,13 +7037,13 @@
         <v>Katzie First Nation</v>
       </c>
       <c r="B18" s="75" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D18" s="75" t="s">
-        <v>698</v>
+        <v>706</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7004,13 +7052,13 @@
         <v>Kwantlen First Nation (tireless Runner)</v>
       </c>
       <c r="B19" s="75" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C19" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D19" s="75" t="s">
-        <v>699</v>
+        <v>707</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7019,13 +7067,13 @@
         <v>Kwaw -Kwaw-Aplit First Nations</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D20" s="75" t="s">
-        <v>700</v>
+        <v>708</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7034,13 +7082,13 @@
         <v>Kwikwetlem First Nation</v>
       </c>
       <c r="B21" s="75" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C21" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D21" s="75" t="s">
-        <v>701</v>
+        <v>709</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7049,13 +7097,13 @@
         <v>Leq' a: mel First Nation</v>
       </c>
       <c r="B22" s="75" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D22" s="75" t="s">
-        <v>702</v>
+        <v>710</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7064,13 +7112,13 @@
         <v>Little Shuswap Lake Indian Band (Skwlax meaning "Black Bear")</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C23" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D23" s="75" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7079,13 +7127,13 @@
         <v>Lheidli T'enneh First Nation</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D24" s="75" t="s">
-        <v>704</v>
+        <v>712</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7094,13 +7142,13 @@
         <v>Lhtako Dene Nation</v>
       </c>
       <c r="B25" s="75" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C25" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D25" s="75" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7109,13 +7157,13 @@
         <v>Lower Nicola Indian Band -</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D26" s="75" t="s">
-        <v>706</v>
+        <v>714</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7124,13 +7172,13 @@
         <v>Lower Similkameen #598</v>
       </c>
       <c r="B27" s="75" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C27" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D27" s="75" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7139,13 +7187,13 @@
         <v>Lyackson First Nation</v>
       </c>
       <c r="B28" s="75" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D28" s="75" t="s">
-        <v>708</v>
+        <v>716</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7154,13 +7202,13 @@
         <v>Malahat First Nation</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C29" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D29" s="75" t="s">
-        <v>709</v>
+        <v>717</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7169,13 +7217,13 @@
         <v>Matsqui First Nation</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C30" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D30" s="75" t="s">
-        <v>710</v>
+        <v>718</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7184,13 +7232,13 @@
         <v>Musqeam Indian Band</v>
       </c>
       <c r="B31" s="75" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C31" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D31" s="78" t="s">
-        <v>711</v>
+        <v>719</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7199,13 +7247,13 @@
         <v>Neskonlith Indian Band</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C32" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D32" s="75" t="s">
-        <v>712</v>
+        <v>720</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7214,13 +7262,13 @@
         <v>Nooaitch Indian Band</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C33" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D33" s="75" t="s">
-        <v>713</v>
+        <v>721</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7229,13 +7277,13 @@
         <v>Osoyoos</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C34" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D34" s="75" t="s">
-        <v>714</v>
+        <v>722</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7244,13 +7292,13 @@
         <v>Pacheedaht First Nation</v>
       </c>
       <c r="B35" s="75" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="C35" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D35" s="75" t="s">
-        <v>715</v>
+        <v>723</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7259,13 +7307,13 @@
         <v>Pauquachin Nation</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C36" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D36" s="78" t="s">
-        <v>716</v>
+        <v>724</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7274,13 +7322,13 @@
         <v>Penticton Indian Band</v>
       </c>
       <c r="B37" s="75" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C37" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D37" s="75" t="s">
-        <v>717</v>
+        <v>725</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7289,13 +7337,13 @@
         <v>Peters Band (Peters First Nation)</v>
       </c>
       <c r="B38" s="75" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C38" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D38" s="75" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7304,13 +7352,13 @@
         <v>Penelakut Tribe</v>
       </c>
       <c r="B39" s="75" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C39" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D39" s="75" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7319,13 +7367,13 @@
         <v>Popkum First Nation</v>
       </c>
       <c r="B40" s="75" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="C40" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D40" s="75" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7334,13 +7382,13 @@
         <v>Qayqayt First Nation (New Westminister)</v>
       </c>
       <c r="B41" s="75" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="C41" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D41" s="78" t="s">
-        <v>722</v>
+        <v>730</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7349,13 +7397,13 @@
         <v>Scia'new First Nation (Beecher Bay First Nation)</v>
       </c>
       <c r="B42" s="75" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="C42" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D42" s="75" t="s">
-        <v>723</v>
+        <v>731</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7364,13 +7412,13 @@
         <v>Sq'ewlets (Scowlitz) First Nation</v>
       </c>
       <c r="B43" s="75" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C43" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D43" s="75" t="s">
-        <v>724</v>
+        <v>732</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7379,13 +7427,13 @@
         <v>Seabird Island Band</v>
       </c>
       <c r="B44" s="75" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="C44" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D44" s="75" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7394,13 +7442,13 @@
         <v>Secwepmc (suh-Meh-much) of the Secwepmc Nation</v>
       </c>
       <c r="B45" s="75" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="C45" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D45" s="78" t="s">
-        <v>726</v>
+        <v>734</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7409,13 +7457,13 @@
         <v>Semiahmoo First Nation</v>
       </c>
       <c r="B46" s="75" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="C46" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D46" s="78" t="s">
-        <v>727</v>
+        <v>735</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7424,13 +7472,13 @@
         <v>Shackan Indian Band</v>
       </c>
       <c r="B47" s="75" t="s">
-        <v>728</v>
+        <v>736</v>
       </c>
       <c r="C47" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D47" s="78" t="s">
-        <v>729</v>
+        <v>737</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7439,13 +7487,13 @@
         <v>Shxw'owhamel First Nation</v>
       </c>
       <c r="B48" s="75" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="C48" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D48" s="75" t="s">
-        <v>730</v>
+        <v>738</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7454,13 +7502,13 @@
         <v>Shxwha:y Villiage</v>
       </c>
       <c r="B49" s="75" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C49" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D49" s="75" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7469,13 +7517,13 @@
         <v>Simpcw First Nation "People of the Rivers"</v>
       </c>
       <c r="B50" s="75" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="C50" s="75" t="s">
-        <v>696</v>
+        <v>704</v>
       </c>
       <c r="D50" s="75" t="s">
-        <v>731</v>
+        <v>739</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7484,13 +7532,13 @@
         <v>Siska Indian Band</v>
       </c>
       <c r="B51" s="75" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="C51" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D51" s="75" t="s">
-        <v>732</v>
+        <v>740</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7499,13 +7547,13 @@
         <v>Skuppah Indian Band</v>
       </c>
       <c r="B52" s="75" t="s">
-        <v>733</v>
+        <v>741</v>
       </c>
       <c r="C52" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D52" s="78" t="s">
-        <v>680</v>
+        <v>688</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7514,13 +7562,13 @@
         <v>Skowkale First Nation</v>
       </c>
       <c r="B53" s="75" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="C53" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D53" s="75" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7529,13 +7577,13 @@
         <v>Shuswap Indian Band</v>
       </c>
       <c r="B54" s="75" t="s">
-        <v>734</v>
+        <v>742</v>
       </c>
       <c r="C54" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D54" s="75" t="s">
-        <v>735</v>
+        <v>743</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7544,13 +7592,13 @@
         <v>Skawahlook First Nation</v>
       </c>
       <c r="B55" s="75" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="C55" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D55" s="75" t="s">
-        <v>736</v>
+        <v>744</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7559,13 +7607,13 @@
         <v>Skwah First Nation</v>
       </c>
       <c r="B56" s="75" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="C56" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D56" s="75" t="s">
-        <v>737</v>
+        <v>745</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7574,13 +7622,13 @@
         <v>Snuneymuxw First Nation</v>
       </c>
       <c r="B57" s="75" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="C57" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D57" s="75" t="s">
-        <v>738</v>
+        <v>746</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7589,13 +7637,13 @@
         <v>Soowahlie First Nation</v>
       </c>
       <c r="B58" s="75" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="C58" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D58" s="75" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7604,13 +7652,13 @@
         <v>Spuzzum First Nation</v>
       </c>
       <c r="B59" s="75" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="C59" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D59" s="78" t="s">
-        <v>680</v>
+        <v>688</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7619,13 +7667,13 @@
         <v>Squamish First Nation (Squ-Ho-0-meesh)</v>
       </c>
       <c r="B60" s="75" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="C60" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D60" s="75" t="s">
-        <v>739</v>
+        <v>747</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7634,13 +7682,13 @@
         <v>Squiala First Nation</v>
       </c>
       <c r="B61" s="75" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="C61" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D61" s="75" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7649,13 +7697,13 @@
         <v>Stk'emlupsemc Te Secwepemc</v>
       </c>
       <c r="B62" s="75" t="s">
-        <v>740</v>
+        <v>748</v>
       </c>
       <c r="C62" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D62" s="75" t="s">
-        <v>741</v>
+        <v>749</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7664,13 +7712,13 @@
         <v>Sts'ailes Band (Chehalls Indian Band)</v>
       </c>
       <c r="B63" s="75" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="C63" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D63" s="75" t="s">
-        <v>742</v>
+        <v>750</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7679,13 +7727,13 @@
         <v>Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek)</v>
       </c>
       <c r="B64" s="75" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="C64" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D64" s="75" t="s">
-        <v>743</v>
+        <v>751</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7694,13 +7742,13 @@
         <v>St'uxwtews (Bonaparte Indian Band)</v>
       </c>
       <c r="B65" s="75" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="C65" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D65" s="75" t="s">
-        <v>744</v>
+        <v>752</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7709,13 +7757,13 @@
         <v>Stz'uminus First Nation (ltst uw' hw-nuts'-ul-wun) Chemainus</v>
       </c>
       <c r="B66" s="75" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="C66" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D66" s="75" t="s">
-        <v>745</v>
+        <v>753</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7724,13 +7772,13 @@
         <v>Sumas First Nation</v>
       </c>
       <c r="B67" s="75" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="C67" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D67" s="75" t="s">
-        <v>746</v>
+        <v>754</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7739,13 +7787,13 @@
         <v>Toosey Indian Band (Tl'esqox)</v>
       </c>
       <c r="B68" s="75" t="s">
-        <v>747</v>
+        <v>755</v>
       </c>
       <c r="C68" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D68" s="78" t="s">
-        <v>748</v>
+        <v>756</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7754,13 +7802,13 @@
         <v>Tsartlip First Nation</v>
       </c>
       <c r="B69" s="75" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="C69" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D69" s="78" t="s">
-        <v>716</v>
+        <v>724</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7769,13 +7817,13 @@
         <v>Tsawout First Nation</v>
       </c>
       <c r="B70" s="75" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="C70" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D70" s="78" t="s">
-        <v>716</v>
+        <v>724</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7784,13 +7832,13 @@
         <v>Tsawwassen First Nation</v>
       </c>
       <c r="B71" s="75" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="C71" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D71" s="78" t="s">
-        <v>749</v>
+        <v>757</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7799,13 +7847,13 @@
         <v>Ts'elxweyeqw Tribe Management Limited</v>
       </c>
       <c r="B72" s="75" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="C72" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D72" s="75" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7814,13 +7862,13 @@
         <v>Tseycum First Nation</v>
       </c>
       <c r="B73" s="75" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
       <c r="C73" s="75" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="D73" s="78" t="s">
-        <v>716</v>
+        <v>724</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7829,13 +7877,13 @@
         <v>Ts'kwaylaxw (Pavillion Indian Band)</v>
       </c>
       <c r="B74" s="75" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="C74" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D74" s="75" t="s">
-        <v>750</v>
+        <v>758</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7844,13 +7892,13 @@
         <v>Tsleil Waututh Nation</v>
       </c>
       <c r="B75" s="75" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="C75" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D75" s="75" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7859,13 +7907,13 @@
         <v>T'Sou-ke Nation</v>
       </c>
       <c r="B76" s="75" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="C76" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D76" s="75" t="s">
-        <v>752</v>
+        <v>760</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7874,13 +7922,13 @@
         <v>Tk'emlups te Secwepemc</v>
       </c>
       <c r="B77" s="75" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="C77" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D77" s="75" t="s">
-        <v>741</v>
+        <v>749</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7889,13 +7937,13 @@
         <v>Tzeachten First Nation</v>
       </c>
       <c r="B78" s="75" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="C78" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D78" s="75" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7904,13 +7952,13 @@
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
       <c r="B79" s="75" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="C79" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D79" s="75" t="s">
-        <v>753</v>
+        <v>761</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7919,13 +7967,13 @@
         <v>Union Bar First Nations</v>
       </c>
       <c r="B80" s="75" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="C80" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D80" s="75" t="s">
-        <v>754</v>
+        <v>762</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7934,13 +7982,13 @@
         <v>Upper Nicola Indian Band</v>
       </c>
       <c r="B81" s="75" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="C81" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D81" s="75" t="s">
-        <v>755</v>
+        <v>763</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7949,13 +7997,13 @@
         <v>Upper Similkameen Indian Band</v>
       </c>
       <c r="B82" s="75" t="s">
-        <v>625</v>
+        <v>633</v>
       </c>
       <c r="C82" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D82" s="75" t="s">
-        <v>756</v>
+        <v>764</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7964,13 +8012,13 @@
         <v>Whispering Pines/Clinton Indian Bands</v>
       </c>
       <c r="B83" s="75" t="s">
-        <v>632</v>
+        <v>640</v>
       </c>
       <c r="C83" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D83" s="75" t="s">
-        <v>757</v>
+        <v>765</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7979,13 +8027,13 @@
         <v>Williams Lake Indian Band</v>
       </c>
       <c r="B84" s="75" t="s">
-        <v>641</v>
+        <v>649</v>
       </c>
       <c r="C84" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D84" s="75" t="s">
-        <v>758</v>
+        <v>766</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7994,13 +8042,13 @@
         <v>Yakweakwioose First Nation</v>
       </c>
       <c r="B85" s="75" t="s">
-        <v>646</v>
+        <v>654</v>
       </c>
       <c r="C85" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D85" s="75" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8009,13 +8057,13 @@
         <v>Yale First Nation</v>
       </c>
       <c r="B86" s="75" t="s">
-        <v>759</v>
+        <v>767</v>
       </c>
       <c r="C86" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D86" s="75" t="s">
-        <v>760</v>
+        <v>768</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8024,13 +8072,13 @@
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
       <c r="B87" s="75" t="s">
-        <v>761</v>
+        <v>769</v>
       </c>
       <c r="C87" s="75" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="D87" s="75" t="s">
-        <v>762</v>
+        <v>770</v>
       </c>
       <c r="G87" s="75"/>
     </row>

</xml_diff>

<commit_message>
added one more digital territory and improved some language/documentation
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="772">
   <si>
     <t xml:space="preserve">TRANSMOUNTAIN EXPANSION PROJECT - INDIGENOUS COMMUNITIES _IMC </t>
   </si>
@@ -647,6 +647,9 @@
   </si>
   <si>
     <t xml:space="preserve">Lower Mainland - Spread 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kwantlen</t>
   </si>
   <si>
     <t xml:space="preserve">Kwaw -Kwaw-Aplit First Nations </t>
@@ -3330,8 +3333,8 @@
   </sheetPr>
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H70" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N77" activeCellId="0" sqref="N77"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4072,31 +4075,34 @@
       <c r="L20" s="17" t="s">
         <v>165</v>
       </c>
+      <c r="M20" s="0" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I21" s="19"/>
       <c r="J21" s="0" t="n">
@@ -4111,32 +4117,32 @@
     </row>
     <row r="22" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B22" s="6" t="str">
         <f aca="false">A22</f>
         <v>Kwikwetlem First Nation</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>49.451741</v>
@@ -4145,39 +4151,39 @@
         <v>-122.657791</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="33" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F23" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="G23" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>188</v>
-      </c>
       <c r="H23" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J23" s="11" t="n">
         <v>49.348358</v>
@@ -4191,29 +4197,29 @@
     </row>
     <row r="24" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="34" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="35" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>51.287872</v>
@@ -4227,31 +4233,31 @@
     </row>
     <row r="25" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="30" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>53.944696</v>
@@ -4260,12 +4266,12 @@
         <v>-121.694171</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B26" s="6" t="str">
         <f aca="false">A26</f>
@@ -4273,22 +4279,22 @@
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="11" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>52.953049</v>
@@ -4302,29 +4308,29 @@
     </row>
     <row r="27" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>50.006984</v>
@@ -4338,28 +4344,28 @@
     </row>
     <row r="28" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F28" s="36" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I28" s="19"/>
       <c r="J28" s="0" t="n">
@@ -4374,32 +4380,32 @@
     </row>
     <row r="29" customFormat="false" ht="56.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="37" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B29" s="6" t="str">
         <f aca="false">A29</f>
         <v>Lyackson First Nation</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>48.941803</v>
@@ -4411,32 +4417,32 @@
     </row>
     <row r="30" customFormat="false" ht="49.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="18" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B30" s="6" t="str">
         <f aca="false">A30</f>
         <v>Malahat First Nation</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F30" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="G30" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="G30" s="16" t="s">
-        <v>244</v>
-      </c>
       <c r="H30" s="11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>48.655944</v>
@@ -4445,34 +4451,34 @@
         <v>-124.000524</v>
       </c>
       <c r="L30" s="38" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="39" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B31" s="6" t="str">
         <f aca="false">A31</f>
         <v>Matsqui First Nation</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="I31" s="19"/>
       <c r="J31" s="0" t="n">
@@ -4482,36 +4488,36 @@
         <v>-122.361868</v>
       </c>
       <c r="L31" s="38" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="79.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="18" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>49.353225</v>
@@ -4525,32 +4531,32 @@
     </row>
     <row r="33" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="18" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B33" s="6" t="str">
         <f aca="false">A33</f>
         <v>Neskonlith Indian Band</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F33" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="G33" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="G33" s="17" t="s">
-        <v>268</v>
-      </c>
       <c r="H33" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>51.21274</v>
@@ -4564,32 +4570,32 @@
     </row>
     <row r="34" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="18" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B34" s="6" t="str">
         <f aca="false">A34</f>
         <v>Nooaitch Indian Band</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>49.690318</v>
@@ -4598,35 +4604,35 @@
         <v>-120.648292</v>
       </c>
       <c r="L34" s="17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="42" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B35" s="6" t="str">
         <f aca="false">A35</f>
         <v>Osoyoos</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F35" s="36" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G35" s="43"/>
       <c r="H35" s="11" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>49.114526</v>
@@ -4635,37 +4641,37 @@
         <v>-118.489264</v>
       </c>
       <c r="L35" s="17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="18" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B36" s="6" t="str">
         <f aca="false">A36</f>
         <v>Pacheedaht First Nation</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F36" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="G36" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="G36" s="16" t="s">
-        <v>291</v>
-      </c>
       <c r="H36" s="11" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>48.572918</v>
@@ -4674,37 +4680,37 @@
         <v>-124.39459</v>
       </c>
       <c r="L36" s="17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="18" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B37" s="6" t="str">
         <f aca="false">A37</f>
         <v>Pauquachin Nation</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I37" s="19"/>
       <c r="J37" s="0" t="n">
@@ -4714,12 +4720,12 @@
         <v>-123.324246</v>
       </c>
       <c r="L37" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="18" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B38" s="6" t="str">
         <f aca="false">A38</f>
@@ -4727,22 +4733,22 @@
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="11" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F38" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="G38" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="G38" s="16" t="s">
-        <v>305</v>
-      </c>
       <c r="H38" s="11" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>49.732366</v>
@@ -4751,34 +4757,34 @@
         <v>-119.25376</v>
       </c>
       <c r="L38" s="17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="18" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="F39" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="G39" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="G39" s="16" t="s">
-        <v>312</v>
-      </c>
       <c r="H39" s="11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>49.505163</v>
@@ -4787,37 +4793,37 @@
         <v>-121.482617</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="18" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B40" s="6" t="str">
         <f aca="false">A40</f>
         <v>Penelakut Tribe</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="F40" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="G40" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="G40" s="16" t="s">
-        <v>320</v>
-      </c>
       <c r="H40" s="11" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>48.892388</v>
@@ -4826,12 +4832,12 @@
         <v>-123.675652</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="18" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B41" s="6" t="str">
         <f aca="false">A41</f>
@@ -4839,19 +4845,19 @@
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="15" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F41" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G41" s="16" t="s">
         <v>328</v>
       </c>
-      <c r="G41" s="16" t="s">
-        <v>327</v>
-      </c>
       <c r="H41" s="15" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I41" s="19"/>
       <c r="J41" s="0" t="n">
@@ -4861,33 +4867,33 @@
         <v>-121.506875</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="127.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="18" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F42" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="G42" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="G42" s="16" t="s">
-        <v>334</v>
-      </c>
       <c r="H42" s="11" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="I42" s="19"/>
       <c r="J42" s="0" t="n">
@@ -4897,37 +4903,37 @@
         <v>-122.910944</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="M42" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="98.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="44" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="15" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>48.440888</v>
@@ -4936,36 +4942,36 @@
         <v>-123.676887</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="45" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="G44" s="16" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>49.25517</v>
@@ -4974,12 +4980,12 @@
         <v>-121.964821</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="44" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B45" s="6" t="str">
         <f aca="false">A45</f>
@@ -4987,19 +4993,19 @@
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="15" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="F45" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="G45" s="16" t="s">
         <v>358</v>
       </c>
-      <c r="G45" s="16" t="s">
-        <v>357</v>
-      </c>
       <c r="H45" s="11" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="I45" s="19"/>
       <c r="J45" s="0" t="n">
@@ -5009,32 +5015,32 @@
         <v>-121.724003</v>
       </c>
       <c r="L45" s="46" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="151.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="21" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="47" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="G46" s="48"/>
       <c r="H46" s="49" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="I46" s="12" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="J46" s="2" t="n">
         <v>51.527017</v>
@@ -5051,26 +5057,26 @@
     </row>
     <row r="47" customFormat="false" ht="80.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="21" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B47" s="6" t="str">
         <f aca="false">A47</f>
         <v>Semiahmoo First Nation</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F47" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="G47" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="G47" s="16" t="s">
-        <v>368</v>
-      </c>
       <c r="H47" s="11" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="I47" s="19"/>
       <c r="J47" s="0" t="n">
@@ -5080,37 +5086,37 @@
         <v>-122.767315</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M47" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="111.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="44" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B48" s="51" t="s">
         <v>42</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="G48" s="48"/>
       <c r="H48" s="11" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="I48" s="12" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>49.963059</v>
@@ -5124,31 +5130,31 @@
     </row>
     <row r="49" customFormat="false" ht="80.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="52" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D49" s="53" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="H49" s="54" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>49.339668</v>
@@ -5157,34 +5163,34 @@
         <v>-121.60638</v>
       </c>
       <c r="L49" s="46" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="55" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D50" s="56" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="G50" s="48"/>
       <c r="H50" s="57" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="I50" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="J50" s="0" t="n">
         <v>49.087557</v>
@@ -5198,31 +5204,31 @@
     </row>
     <row r="51" customFormat="false" ht="51.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="44" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F51" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="G51" s="50" t="s">
         <v>400</v>
       </c>
-      <c r="G51" s="50" t="s">
-        <v>399</v>
-      </c>
       <c r="H51" s="58" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J51" s="0" t="n">
         <v>52.634393</v>
@@ -5236,29 +5242,29 @@
     </row>
     <row r="52" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="21" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B52" s="6" t="str">
         <f aca="false">A52</f>
         <v>Siska Indian Band</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="I52" s="19"/>
       <c r="J52" s="0" t="n">
@@ -5268,33 +5274,33 @@
         <v>-120.838519</v>
       </c>
       <c r="L52" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="21" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B53" s="51" t="s">
         <v>42</v>
       </c>
       <c r="C53" s="51" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F53" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="G53" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="G53" s="16" t="s">
-        <v>413</v>
-      </c>
       <c r="H53" s="11" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I53" s="19"/>
       <c r="J53" s="0" t="n">
@@ -5304,36 +5310,36 @@
         <v>-121.484624</v>
       </c>
       <c r="L53" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="21" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="J54" s="0" t="n">
         <v>49.087557</v>
@@ -5347,32 +5353,32 @@
     </row>
     <row r="55" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="23" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B55" s="6" t="str">
         <f aca="false">A55</f>
         <v>Shuswap Indian Band</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G55" s="17" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="J55" s="0" t="n">
         <v>50.367907</v>
@@ -5386,32 +5392,32 @@
     </row>
     <row r="56" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="23" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B56" s="6" t="str">
         <f aca="false">A56</f>
         <v>Skawahlook First Nation</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F56" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="G56" s="17" t="s">
         <v>436</v>
       </c>
-      <c r="G56" s="17" t="s">
-        <v>435</v>
-      </c>
       <c r="H56" s="11" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="I56" s="12" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="J56" s="0" t="n">
         <v>49.227586</v>
@@ -5420,37 +5426,37 @@
         <v>-122.174045</v>
       </c>
       <c r="L56" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="59" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B57" s="6" t="str">
         <f aca="false">A57</f>
         <v>Skwah First Nation</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="F57" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="G57" s="17" t="s">
         <v>443</v>
       </c>
-      <c r="G57" s="17" t="s">
-        <v>442</v>
-      </c>
       <c r="H57" s="11" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="J57" s="0" t="n">
         <v>49.175281</v>
@@ -5464,32 +5470,32 @@
     </row>
     <row r="58" customFormat="false" ht="51.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="18" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B58" s="6" t="str">
         <f aca="false">A58</f>
         <v>Snuneymuxw First Nation</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F58" s="11" t="s">
+        <v>451</v>
+      </c>
+      <c r="G58" s="17" t="s">
         <v>450</v>
       </c>
-      <c r="G58" s="17" t="s">
-        <v>449</v>
-      </c>
       <c r="H58" s="11" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="J58" s="0" t="n">
         <v>49.107871</v>
@@ -5503,31 +5509,31 @@
     </row>
     <row r="59" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="23" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E59" s="41" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F59" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="G59" s="27" t="s">
         <v>457</v>
       </c>
-      <c r="G59" s="27" t="s">
-        <v>456</v>
-      </c>
       <c r="H59" s="11" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="J59" s="0" t="n">
         <v>49.087557</v>
@@ -5541,29 +5547,29 @@
     </row>
     <row r="60" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="59" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="11" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="G60" s="17" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="J60" s="0" t="n">
         <v>49.963059</v>
@@ -5572,34 +5578,34 @@
         <v>-121.484624</v>
       </c>
       <c r="L60" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="61" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G61" s="17"/>
       <c r="H61" s="11" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="J61" s="0" t="n">
         <v>49.807197</v>
@@ -5608,36 +5614,36 @@
         <v>-123.200082</v>
       </c>
       <c r="L61" s="13" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="61" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F62" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="G62" s="17" t="s">
         <v>481</v>
       </c>
-      <c r="G62" s="17" t="s">
-        <v>480</v>
-      </c>
       <c r="H62" s="11" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="I62" s="12" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="J62" s="0" t="n">
         <v>49.087557</v>
@@ -5651,29 +5657,29 @@
     </row>
     <row r="63" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="18" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63" s="36" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="I63" s="12" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="J63" s="0" t="n">
         <v>51.341443</v>
@@ -5687,31 +5693,31 @@
     </row>
     <row r="64" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="23" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F64" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="G64" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="G64" s="17" t="s">
-        <v>496</v>
-      </c>
       <c r="H64" s="11" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="I64" s="12" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="J64" s="0" t="n">
         <v>49.293578</v>
@@ -5725,31 +5731,31 @@
     </row>
     <row r="65" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="21" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="G65" s="17" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="I65" s="12" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="J65" s="0" t="n">
         <v>51.586232</v>
@@ -5763,29 +5769,29 @@
     </row>
     <row r="66" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="62" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G66" s="17"/>
       <c r="H66" s="11" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="I66" s="12" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="J66" s="0" t="n">
         <v>50.839863</v>
@@ -5799,29 +5805,29 @@
     </row>
     <row r="67" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="44" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="63" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F67" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="G67" s="17" t="s">
         <v>520</v>
       </c>
-      <c r="G67" s="17" t="s">
-        <v>519</v>
-      </c>
       <c r="H67" s="15" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="I67" s="12" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="J67" s="0" t="n">
         <v>48.846385</v>
@@ -5835,7 +5841,7 @@
     </row>
     <row r="68" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="23" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B68" s="6" t="str">
         <f aca="false">A68</f>
@@ -5843,22 +5849,22 @@
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="F68" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="G68" s="17" t="s">
         <v>526</v>
       </c>
-      <c r="G68" s="17" t="s">
-        <v>525</v>
-      </c>
       <c r="H68" s="11" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="I68" s="12" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="J68" s="0" t="n">
         <v>49.052587</v>
@@ -5872,7 +5878,7 @@
     </row>
     <row r="69" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="59" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B69" s="6" t="str">
         <f aca="false">A69</f>
@@ -5880,19 +5886,19 @@
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="11" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F69" s="11" t="s">
+        <v>533</v>
+      </c>
+      <c r="G69" s="17" t="s">
         <v>532</v>
       </c>
-      <c r="G69" s="17" t="s">
-        <v>531</v>
-      </c>
       <c r="H69" s="11" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="I69" s="19"/>
       <c r="J69" s="0" t="n">
@@ -5907,31 +5913,31 @@
     </row>
     <row r="70" customFormat="false" ht="58.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="18" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="F70" s="11" t="s">
+        <v>539</v>
+      </c>
+      <c r="G70" s="17" t="s">
         <v>538</v>
       </c>
-      <c r="G70" s="17" t="s">
-        <v>537</v>
-      </c>
       <c r="H70" s="11" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="I70" s="12" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="J70" s="0" t="n">
         <v>48.724102</v>
@@ -5940,36 +5946,36 @@
         <v>-123.324246</v>
       </c>
       <c r="L70" s="46" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="61" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="F71" s="11" t="s">
+        <v>546</v>
+      </c>
+      <c r="G71" s="17" t="s">
         <v>545</v>
       </c>
-      <c r="G71" s="17" t="s">
-        <v>544</v>
-      </c>
       <c r="H71" s="11" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="I71" s="12" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="J71" s="0" t="n">
         <v>48.724102</v>
@@ -5978,37 +5984,37 @@
         <v>-123.324246</v>
       </c>
       <c r="L71" s="46" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="18" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B72" s="6" t="str">
         <f aca="false">A72</f>
         <v>Tsawwassen First Nation</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F72" s="11" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="G72" s="17" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="I72" s="12" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="J72" s="0" t="n">
         <v>49.042909</v>
@@ -6017,34 +6023,34 @@
         <v>-123.094409</v>
       </c>
       <c r="L72" s="46" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="M72" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="44" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="11" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="G73" s="64" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="I73" s="12"/>
       <c r="J73" s="0" t="n">
@@ -6059,31 +6065,31 @@
     </row>
     <row r="74" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="23" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="G74" s="17" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="I74" s="12" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="J74" s="0" t="n">
         <v>48.724102</v>
@@ -6092,31 +6098,31 @@
         <v>-123.324246</v>
       </c>
       <c r="L74" s="46" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="59" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="G75" s="17"/>
       <c r="H75" s="11" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="J75" s="0" t="n">
         <v>50.883097</v>
@@ -6130,32 +6136,32 @@
     </row>
     <row r="76" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="18" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B76" s="6" t="str">
         <f aca="false">A76</f>
         <v>Tsleil Waututh Nation</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="F76" s="11" t="s">
+        <v>585</v>
+      </c>
+      <c r="G76" s="17" t="s">
         <v>584</v>
       </c>
-      <c r="G76" s="17" t="s">
-        <v>583</v>
-      </c>
       <c r="H76" s="11" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="I76" s="12" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="J76" s="0" t="n">
         <v>49.309839</v>
@@ -6164,40 +6170,40 @@
         <v>-122.980478</v>
       </c>
       <c r="L76" s="46" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="M76" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="64.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="18" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B77" s="6" t="str">
         <f aca="false">A77</f>
         <v>T'Sou-ke Nation</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="G77" s="16" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="J77" s="0" t="n">
         <v>48.385518</v>
@@ -6206,12 +6212,12 @@
         <v>-123.696567</v>
       </c>
       <c r="L77" s="46" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="23" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B78" s="6" t="str">
         <f aca="false">A78</f>
@@ -6219,22 +6225,22 @@
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="11" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="F78" s="65" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="G78" s="66" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="I78" s="12" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="J78" s="0" t="n">
         <v>50.678844</v>
@@ -6248,31 +6254,31 @@
     </row>
     <row r="79" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="23" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E79" s="11" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="I79" s="12" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="J79" s="0" t="n">
         <v>49.087557</v>
@@ -6286,32 +6292,32 @@
     </row>
     <row r="80" customFormat="false" ht="76.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="23" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B80" s="6" t="str">
         <f aca="false">A80</f>
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="E80" s="67" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="G80" s="17" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="I80" s="12" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="J80" s="0" t="n">
         <v>52.475488</v>
@@ -6320,31 +6326,31 @@
         <v>-125.301018</v>
       </c>
       <c r="L80" s="46" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="23" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="11" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="G81" s="17" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="I81" s="19"/>
       <c r="J81" s="0" t="n">
@@ -6357,7 +6363,7 @@
     </row>
     <row r="82" customFormat="false" ht="43.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="23" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B82" s="6" t="str">
         <f aca="false">A82</f>
@@ -6365,20 +6371,20 @@
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="11" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="G82" s="17"/>
       <c r="H82" s="11" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="I82" s="12" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="J82" s="0" t="n">
         <v>50.167239</v>
@@ -6392,32 +6398,32 @@
     </row>
     <row r="83" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="59" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B83" s="6" t="str">
         <f aca="false">A83</f>
         <v>Upper Similkameen Indian Band</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="F83" s="11" t="s">
+        <v>637</v>
+      </c>
+      <c r="G83" s="68" t="s">
         <v>636</v>
       </c>
-      <c r="G83" s="68" t="s">
-        <v>635</v>
-      </c>
       <c r="H83" s="11" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="I83" s="19" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="J83" s="0" t="n">
         <v>49.462883</v>
@@ -6426,34 +6432,34 @@
         <v>-120.50172</v>
       </c>
       <c r="L83" s="17" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="54.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="18" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="11" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="G84" s="17" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="I84" s="12" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="J84" s="0" t="n">
         <v>51.194286</v>
@@ -6462,12 +6468,12 @@
         <v>-121.613314</v>
       </c>
       <c r="L84" s="13" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="18" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B85" s="6" t="str">
         <f aca="false">A85</f>
@@ -6475,18 +6481,18 @@
       </c>
       <c r="C85" s="6"/>
       <c r="D85" s="11" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="E85" s="11"/>
       <c r="F85" s="11" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="G85" s="17"/>
       <c r="H85" s="11" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="I85" s="12" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="J85" s="0" t="n">
         <v>52.10532</v>
@@ -6498,31 +6504,31 @@
     </row>
     <row r="86" customFormat="false" ht="73.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="23" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="I86" s="19" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="J86" s="0" t="n">
         <v>49.087557</v>
@@ -6531,12 +6537,12 @@
         <v>-121.829723</v>
       </c>
       <c r="L86" s="13" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="23" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B87" s="6" t="str">
         <f aca="false">A87</f>
@@ -6544,22 +6550,22 @@
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="11" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E87" s="11" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="I87" s="12" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="J87" s="0" t="n">
         <v>49.492718</v>
@@ -6568,12 +6574,12 @@
         <v>-121.423097</v>
       </c>
       <c r="L87" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="23" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B88" s="6" t="str">
         <f aca="false">A88</f>
@@ -6581,22 +6587,22 @@
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="11" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="F88" s="63" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="G88" s="17" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="I88" s="12" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="J88" s="0" t="n">
         <v>52.854978</v>
@@ -6621,7 +6627,7 @@
     </row>
     <row r="90" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="23" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B90" s="23"/>
       <c r="C90" s="23"/>
@@ -6631,7 +6637,7 @@
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
@@ -6640,7 +6646,7 @@
     </row>
     <row r="92" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
@@ -6649,7 +6655,7 @@
     </row>
     <row r="93" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="11" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
@@ -6782,13 +6788,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C1" s="75" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="D1" s="76" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6800,10 +6806,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D2" s="77" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6815,10 +6821,10 @@
         <v>24</v>
       </c>
       <c r="C3" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6830,10 +6836,10 @@
         <v>34</v>
       </c>
       <c r="C4" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D4" s="75" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6845,10 +6851,10 @@
         <v>42</v>
       </c>
       <c r="C5" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D5" s="78" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6860,10 +6866,10 @@
         <v>49</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D6" s="75" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6875,10 +6881,10 @@
         <v>56</v>
       </c>
       <c r="C7" s="76" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D7" s="75" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6890,10 +6896,10 @@
         <v>64</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6902,13 +6908,13 @@
         <v>Chi:yo:m Agassiz (Cheam) First Nation - meaning "Wild Strawberry Place"</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C9" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D9" s="75" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6920,10 +6926,10 @@
         <v>83</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D10" s="75" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6932,13 +6938,13 @@
         <v>Cook's Ferry Indian Band Kumcheen (Variation Nkumcheen); Includes Pokheistk (Variation Pakeist, Pokheistsk), Pemynoos (Variation Piminos), Spatsum (Variation Spaptsin), Spence'S Bridge</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C11" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D11" s="75" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6950,10 +6956,10 @@
         <v>97</v>
       </c>
       <c r="C12" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D12" s="75" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6965,10 +6971,10 @@
         <v>107</v>
       </c>
       <c r="C13" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D13" s="75" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6980,10 +6986,10 @@
         <v>118</v>
       </c>
       <c r="C14" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D14" s="78" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6992,13 +6998,13 @@
         <v>Halalt First Nation</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D15" s="75" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7010,10 +7016,10 @@
         <v>133</v>
       </c>
       <c r="C16" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D16" s="75" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7022,13 +7028,13 @@
         <v>Huu-ay-aht First Nation</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="D17" s="75" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7040,10 +7046,10 @@
         <v>149</v>
       </c>
       <c r="C18" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D18" s="75" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7055,10 +7061,10 @@
         <v>158</v>
       </c>
       <c r="C19" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D19" s="75" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7067,13 +7073,13 @@
         <v>Kwaw -Kwaw-Aplit First Nations</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C20" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D20" s="75" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7082,13 +7088,13 @@
         <v>Kwikwetlem First Nation</v>
       </c>
       <c r="B21" s="75" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C21" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D21" s="75" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7097,13 +7103,13 @@
         <v>Leq' a: mel First Nation</v>
       </c>
       <c r="B22" s="75" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D22" s="75" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7112,13 +7118,13 @@
         <v>Little Shuswap Lake Indian Band (Skwlax meaning "Black Bear")</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C23" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D23" s="75" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7127,13 +7133,13 @@
         <v>Lheidli T'enneh First Nation</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D24" s="75" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7142,13 +7148,13 @@
         <v>Lhtako Dene Nation</v>
       </c>
       <c r="B25" s="75" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C25" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D25" s="75" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7157,13 +7163,13 @@
         <v>Lower Nicola Indian Band -</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C26" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D26" s="75" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7172,13 +7178,13 @@
         <v>Lower Similkameen #598</v>
       </c>
       <c r="B27" s="75" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C27" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D27" s="75" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7187,13 +7193,13 @@
         <v>Lyackson First Nation</v>
       </c>
       <c r="B28" s="75" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C28" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D28" s="75" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7202,13 +7208,13 @@
         <v>Malahat First Nation</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C29" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D29" s="75" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7217,13 +7223,13 @@
         <v>Matsqui First Nation</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C30" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D30" s="75" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7232,13 +7238,13 @@
         <v>Musqeam Indian Band</v>
       </c>
       <c r="B31" s="75" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C31" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D31" s="78" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7247,13 +7253,13 @@
         <v>Neskonlith Indian Band</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C32" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D32" s="75" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7262,13 +7268,13 @@
         <v>Nooaitch Indian Band</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C33" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D33" s="75" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7277,13 +7283,13 @@
         <v>Osoyoos</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C34" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D34" s="75" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7292,13 +7298,13 @@
         <v>Pacheedaht First Nation</v>
       </c>
       <c r="B35" s="75" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C35" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D35" s="75" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7307,13 +7313,13 @@
         <v>Pauquachin Nation</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C36" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D36" s="78" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7322,13 +7328,13 @@
         <v>Penticton Indian Band</v>
       </c>
       <c r="B37" s="75" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C37" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D37" s="75" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7337,13 +7343,13 @@
         <v>Peters Band (Peters First Nation)</v>
       </c>
       <c r="B38" s="75" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C38" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D38" s="75" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7352,13 +7358,13 @@
         <v>Penelakut Tribe</v>
       </c>
       <c r="B39" s="75" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C39" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D39" s="75" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7367,13 +7373,13 @@
         <v>Popkum First Nation</v>
       </c>
       <c r="B40" s="75" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C40" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D40" s="75" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7382,13 +7388,13 @@
         <v>Qayqayt First Nation (New Westminister)</v>
       </c>
       <c r="B41" s="75" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C41" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D41" s="78" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7397,13 +7403,13 @@
         <v>Scia'new First Nation (Beecher Bay First Nation)</v>
       </c>
       <c r="B42" s="75" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C42" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D42" s="75" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7412,13 +7418,13 @@
         <v>Sq'ewlets (Scowlitz) First Nation</v>
       </c>
       <c r="B43" s="75" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C43" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D43" s="75" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7427,13 +7433,13 @@
         <v>Seabird Island Band</v>
       </c>
       <c r="B44" s="75" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C44" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D44" s="75" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7442,13 +7448,13 @@
         <v>Secwepmc (suh-Meh-much) of the Secwepmc Nation</v>
       </c>
       <c r="B45" s="75" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C45" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D45" s="78" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7457,13 +7463,13 @@
         <v>Semiahmoo First Nation</v>
       </c>
       <c r="B46" s="75" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C46" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D46" s="78" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7472,13 +7478,13 @@
         <v>Shackan Indian Band</v>
       </c>
       <c r="B47" s="75" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C47" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D47" s="78" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7487,13 +7493,13 @@
         <v>Shxw'owhamel First Nation</v>
       </c>
       <c r="B48" s="75" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C48" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D48" s="75" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7502,13 +7508,13 @@
         <v>Shxwha:y Villiage</v>
       </c>
       <c r="B49" s="75" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C49" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D49" s="75" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7517,13 +7523,13 @@
         <v>Simpcw First Nation "People of the Rivers"</v>
       </c>
       <c r="B50" s="75" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C50" s="75" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="D50" s="75" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7532,13 +7538,13 @@
         <v>Siska Indian Band</v>
       </c>
       <c r="B51" s="75" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C51" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D51" s="75" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7547,13 +7553,13 @@
         <v>Skuppah Indian Band</v>
       </c>
       <c r="B52" s="75" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C52" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D52" s="78" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7562,13 +7568,13 @@
         <v>Skowkale First Nation</v>
       </c>
       <c r="B53" s="75" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C53" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D53" s="75" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7577,13 +7583,13 @@
         <v>Shuswap Indian Band</v>
       </c>
       <c r="B54" s="75" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C54" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D54" s="75" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7592,13 +7598,13 @@
         <v>Skawahlook First Nation</v>
       </c>
       <c r="B55" s="75" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C55" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D55" s="75" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7607,13 +7613,13 @@
         <v>Skwah First Nation</v>
       </c>
       <c r="B56" s="75" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C56" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D56" s="75" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7622,13 +7628,13 @@
         <v>Snuneymuxw First Nation</v>
       </c>
       <c r="B57" s="75" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C57" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D57" s="75" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7637,13 +7643,13 @@
         <v>Soowahlie First Nation</v>
       </c>
       <c r="B58" s="75" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C58" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D58" s="75" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7652,13 +7658,13 @@
         <v>Spuzzum First Nation</v>
       </c>
       <c r="B59" s="75" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C59" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D59" s="78" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7667,13 +7673,13 @@
         <v>Squamish First Nation (Squ-Ho-0-meesh)</v>
       </c>
       <c r="B60" s="75" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C60" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D60" s="75" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7682,13 +7688,13 @@
         <v>Squiala First Nation</v>
       </c>
       <c r="B61" s="75" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C61" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D61" s="75" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7697,13 +7703,13 @@
         <v>Stk'emlupsemc Te Secwepemc</v>
       </c>
       <c r="B62" s="75" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C62" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D62" s="75" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7712,13 +7718,13 @@
         <v>Sts'ailes Band (Chehalls Indian Band)</v>
       </c>
       <c r="B63" s="75" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C63" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D63" s="75" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7727,13 +7733,13 @@
         <v>Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek)</v>
       </c>
       <c r="B64" s="75" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C64" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D64" s="75" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7742,13 +7748,13 @@
         <v>St'uxwtews (Bonaparte Indian Band)</v>
       </c>
       <c r="B65" s="75" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C65" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D65" s="75" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7757,13 +7763,13 @@
         <v>Stz'uminus First Nation (ltst uw' hw-nuts'-ul-wun) Chemainus</v>
       </c>
       <c r="B66" s="75" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C66" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D66" s="75" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7772,13 +7778,13 @@
         <v>Sumas First Nation</v>
       </c>
       <c r="B67" s="75" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C67" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D67" s="75" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7787,13 +7793,13 @@
         <v>Toosey Indian Band (Tl'esqox)</v>
       </c>
       <c r="B68" s="75" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C68" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D68" s="78" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7802,13 +7808,13 @@
         <v>Tsartlip First Nation</v>
       </c>
       <c r="B69" s="75" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C69" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D69" s="78" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7817,13 +7823,13 @@
         <v>Tsawout First Nation</v>
       </c>
       <c r="B70" s="75" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C70" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D70" s="78" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7832,13 +7838,13 @@
         <v>Tsawwassen First Nation</v>
       </c>
       <c r="B71" s="75" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C71" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D71" s="78" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7847,13 +7853,13 @@
         <v>Ts'elxweyeqw Tribe Management Limited</v>
       </c>
       <c r="B72" s="75" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C72" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D72" s="75" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7862,13 +7868,13 @@
         <v>Tseycum First Nation</v>
       </c>
       <c r="B73" s="75" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C73" s="75" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D73" s="78" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7877,13 +7883,13 @@
         <v>Ts'kwaylaxw (Pavillion Indian Band)</v>
       </c>
       <c r="B74" s="75" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C74" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D74" s="75" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7892,13 +7898,13 @@
         <v>Tsleil Waututh Nation</v>
       </c>
       <c r="B75" s="75" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C75" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D75" s="75" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7907,13 +7913,13 @@
         <v>T'Sou-ke Nation</v>
       </c>
       <c r="B76" s="75" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C76" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D76" s="75" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7922,13 +7928,13 @@
         <v>Tk'emlups te Secwepemc</v>
       </c>
       <c r="B77" s="75" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C77" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D77" s="75" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7937,13 +7943,13 @@
         <v>Tzeachten First Nation</v>
       </c>
       <c r="B78" s="75" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C78" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D78" s="75" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7952,13 +7958,13 @@
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
       <c r="B79" s="75" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C79" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D79" s="75" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7967,13 +7973,13 @@
         <v>Union Bar First Nations</v>
       </c>
       <c r="B80" s="75" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C80" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D80" s="75" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7982,13 +7988,13 @@
         <v>Upper Nicola Indian Band</v>
       </c>
       <c r="B81" s="75" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C81" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D81" s="75" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7997,13 +8003,13 @@
         <v>Upper Similkameen Indian Band</v>
       </c>
       <c r="B82" s="75" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C82" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D82" s="75" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8012,13 +8018,13 @@
         <v>Whispering Pines/Clinton Indian Bands</v>
       </c>
       <c r="B83" s="75" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C83" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D83" s="75" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8027,13 +8033,13 @@
         <v>Williams Lake Indian Band</v>
       </c>
       <c r="B84" s="75" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C84" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D84" s="75" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8042,13 +8048,13 @@
         <v>Yakweakwioose First Nation</v>
       </c>
       <c r="B85" s="75" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C85" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D85" s="75" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8057,13 +8063,13 @@
         <v>Yale First Nation</v>
       </c>
       <c r="B86" s="75" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="C86" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D86" s="75" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8072,13 +8078,13 @@
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
       <c r="B87" s="75" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C87" s="75" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D87" s="75" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="G87" s="75"/>
     </row>

</xml_diff>

<commit_message>
started on kp click functionality and updated deps
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BC First Nations" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="image sources" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Spreads" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BC First Nations'!$A$2:$Q$90</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="984">
   <si>
     <t xml:space="preserve">TRANSMOUNTAIN EXPANSION PROJECT - INDIGENOUS COMMUNITIES _IMC </t>
   </si>
@@ -3691,6 +3692,27 @@
   </si>
   <si>
     <t xml:space="preserve">Xat'sull First Nation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
   </si>
 </sst>
 </file>
@@ -4588,8 +4610,8 @@
   </sheetPr>
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G79" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V90" activeCellId="0" sqref="V90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4600,7 +4622,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="27.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="8" style="0" width="14.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="8" style="0" width="14.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="40.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1006" style="0" width="9.14"/>
@@ -5485,7 +5509,7 @@
       </c>
       <c r="V16" s="8" t="str">
         <f aca="false">A16</f>
-        <v>Halalt First Nation</v>
+        <v>Halalt First Nation </v>
       </c>
       <c r="W16" s="8" t="s">
         <v>191</v>
@@ -9947,7 +9971,7 @@
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
         <f aca="false">'BC First Nations'!A11</f>
-        <v>Coldwater First Nation (Nc/etko - the people of the creeks)</v>
+        <v>Coldwater First Nation (Nc/etko - the people of the creeks)      </v>
       </c>
       <c r="B10" s="92" t="s">
         <v>131</v>
@@ -10022,7 +10046,7 @@
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="str">
         <f aca="false">'BC First Nations'!A16</f>
-        <v>Halalt First Nation</v>
+        <v>Halalt First Nation </v>
       </c>
       <c r="B15" s="92" t="s">
         <v>946</v>
@@ -10052,7 +10076,7 @@
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="str">
         <f aca="false">'BC First Nations'!A18</f>
-        <v>Huu-ay-aht First Nation</v>
+        <v>Huu-ay-aht First Nation </v>
       </c>
       <c r="B17" s="92" t="s">
         <v>948</v>
@@ -10097,7 +10121,7 @@
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="str">
         <f aca="false">'BC First Nations'!A21</f>
-        <v>Kwaw -Kwaw-Aplit First Nations</v>
+        <v>Kwaw -Kwaw-Aplit First Nations </v>
       </c>
       <c r="B20" s="92" t="s">
         <v>246</v>
@@ -10412,7 +10436,7 @@
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="str">
         <f aca="false">'BC First Nations'!A42</f>
-        <v>Qayqayt First Nation (New Westminister)</v>
+        <v>Qayqayt First Nation (New Westminister) </v>
       </c>
       <c r="B41" s="92" t="s">
         <v>956</v>
@@ -10502,7 +10526,7 @@
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="str">
         <f aca="false">'BC First Nations'!A49</f>
-        <v>Shackan Indian Band</v>
+        <v>Shackan Indian Band </v>
       </c>
       <c r="B47" s="92" t="s">
         <v>961</v>
@@ -10577,7 +10601,7 @@
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="str">
         <f aca="false">'BC First Nations'!A54</f>
-        <v>Skuppah Indian Band</v>
+        <v>Skuppah Indian Band </v>
       </c>
       <c r="B52" s="92" t="s">
         <v>964</v>
@@ -10607,7 +10631,7 @@
     <row r="54" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="str">
         <f aca="false">'BC First Nations'!A56</f>
-        <v>Shuswap Indian Band</v>
+        <v>Shuswap Indian Band </v>
       </c>
       <c r="B54" s="92" t="s">
         <v>965</v>
@@ -10727,7 +10751,7 @@
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="str">
         <f aca="false">'BC First Nations'!A64</f>
-        <v>Stk'emlupsemc Te Secwepemc</v>
+        <v>Stk'emlupsemc Te Secwepemc </v>
       </c>
       <c r="B62" s="92" t="s">
         <v>970</v>
@@ -10742,7 +10766,7 @@
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="str">
         <f aca="false">'BC First Nations'!A65</f>
-        <v>Sts'ailes Band (Chehalls Indian Band)</v>
+        <v>Sts'ailes Band (Chehalls Indian Band) </v>
       </c>
       <c r="B63" s="92" t="s">
         <v>695</v>
@@ -11087,7 +11111,7 @@
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="str">
         <f aca="false">'BC First Nations'!A89</f>
-        <v>Yale First Nation</v>
+        <v>Yale First Nation </v>
       </c>
       <c r="B86" s="92" t="s">
         <v>975</v>
@@ -11217,4 +11241,215 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>977</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>978</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>979</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>49.114</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>981</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>49.114</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>147.767</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>147.767</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>246.043</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>983</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>246.043</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>337.966</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>981</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>489.16</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>502.443</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>502.443</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>525.579</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>983</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>525.579</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>610.675</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>981</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>610.675</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>690.485</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>690.485</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>764.569</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>981</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>806.471</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>990.273</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>990.273</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1075.731</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1075.122</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1144.48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1144.908</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1180.149</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
started improving community location info
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BC First Nations" sheetId="1" state="visible" r:id="rId2"/>
@@ -3719,8 +3719,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -4141,7 +4142,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="110">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4282,7 +4283,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4291,6 +4324,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4378,8 +4415,32 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -4483,10 +4544,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4610,8 +4667,8 @@
   </sheetPr>
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4623,7 +4680,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="27.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="8" style="0" width="14.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="40.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="40.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.37"/>
@@ -4757,10 +4814,10 @@
         <v>37</v>
       </c>
       <c r="R3" s="18" t="n">
-        <v>51.527017</v>
+        <v>50.8291154794399</v>
       </c>
       <c r="S3" s="14" t="n">
-        <v>-120.076953</v>
+        <v>-119.7016527</v>
       </c>
       <c r="T3" s="14" t="s">
         <v>38</v>
@@ -4821,10 +4878,10 @@
         <v>51</v>
       </c>
       <c r="R4" s="14" t="n">
-        <v>49.087557</v>
+        <v>49.1505413634721</v>
       </c>
       <c r="S4" s="14" t="n">
-        <v>-121.829723</v>
+        <v>-121.987290916937</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>52</v>
@@ -4876,10 +4933,10 @@
         <v>63</v>
       </c>
       <c r="R5" s="14" t="n">
-        <v>50.404267</v>
+        <v>50.7203687204045</v>
       </c>
       <c r="S5" s="14" t="n">
-        <v>-120.678195</v>
+        <v>-121.319688819</v>
       </c>
       <c r="V5" s="8" t="str">
         <f aca="false">A5</f>
@@ -4926,10 +4983,10 @@
         <v>70</v>
       </c>
       <c r="R6" s="14" t="n">
-        <v>49.963059</v>
+        <v>49.9634982583732</v>
       </c>
       <c r="S6" s="14" t="n">
-        <v>-121.484624</v>
+        <v>-121.48397324949</v>
       </c>
       <c r="V6" s="8" t="str">
         <f aca="false">A6</f>
@@ -4976,10 +5033,10 @@
       </c>
       <c r="Q7" s="16"/>
       <c r="R7" s="14" t="n">
-        <v>49.621761</v>
+        <v>49.8613568484276</v>
       </c>
       <c r="S7" s="14" t="n">
-        <v>-120.95154</v>
+        <v>-121.440876627917</v>
       </c>
       <c r="V7" s="8" t="str">
         <f aca="false">A7</f>
@@ -5034,10 +5091,10 @@
         <v>91</v>
       </c>
       <c r="R8" s="14" t="n">
-        <v>51.770937</v>
+        <v>51.7718379529271</v>
       </c>
       <c r="S8" s="14" t="n">
-        <v>-120.993827</v>
+        <v>-120.993991830686</v>
       </c>
       <c r="V8" s="8" t="s">
         <v>92</v>
@@ -5093,10 +5150,10 @@
         <v>105</v>
       </c>
       <c r="R9" s="14" t="n">
-        <v>49.283272</v>
+        <v>49.3702501965451</v>
       </c>
       <c r="S9" s="14" t="n">
-        <v>-121.291263</v>
+        <v>-121.552140153971</v>
       </c>
       <c r="V9" s="8" t="s">
         <v>93</v>
@@ -5154,10 +5211,10 @@
         <v>118</v>
       </c>
       <c r="R10" s="14" t="n">
-        <v>49.540481</v>
+        <v>49.1897365395324</v>
       </c>
       <c r="S10" s="14" t="n">
-        <v>-121.7239</v>
+        <v>-121.784199584657</v>
       </c>
       <c r="V10" s="8" t="s">
         <v>119</v>
@@ -5266,10 +5323,10 @@
         <v>140</v>
       </c>
       <c r="R12" s="14" t="n">
-        <v>50.032193</v>
+        <v>50.4227460817348</v>
       </c>
       <c r="S12" s="14" t="n">
-        <v>-120.617392</v>
+        <v>-121.345103566763</v>
       </c>
       <c r="V12" s="8" t="s">
         <v>141</v>
@@ -5325,10 +5382,10 @@
         <v>153</v>
       </c>
       <c r="R13" s="14" t="n">
-        <v>48.888822</v>
+        <v>48.7759494968352</v>
       </c>
       <c r="S13" s="14" t="n">
-        <v>-123.752153</v>
+        <v>-123.70948550892</v>
       </c>
       <c r="V13" s="8" t="s">
         <v>142</v>
@@ -5386,10 +5443,10 @@
         <v>168</v>
       </c>
       <c r="R14" s="14" t="n">
-        <v>48.890317</v>
+        <v>48.8068671468874</v>
       </c>
       <c r="S14" s="14" t="n">
-        <v>-124.592686</v>
+        <v>-124.667070239226</v>
       </c>
       <c r="T14" s="14" t="s">
         <v>169</v>
@@ -5450,10 +5507,10 @@
         <v>180</v>
       </c>
       <c r="R15" s="14" t="n">
-        <v>48.688573</v>
+        <v>48.4448905662452</v>
       </c>
       <c r="S15" s="14" t="n">
-        <v>-123.453132</v>
+        <v>-123.430239771178</v>
       </c>
       <c r="V15" s="8" t="s">
         <v>181</v>
@@ -5502,14 +5559,14 @@
         <v>190</v>
       </c>
       <c r="R16" s="14" t="n">
-        <v>48.929783</v>
+        <v>48.8744822422848</v>
       </c>
       <c r="S16" s="14" t="n">
-        <v>-124.479846</v>
+        <v>-123.696290570467</v>
       </c>
       <c r="V16" s="8" t="str">
         <f aca="false">A16</f>
-        <v>Halalt First Nation </v>
+        <v>Halalt First Nation</v>
       </c>
       <c r="W16" s="8" t="s">
         <v>191</v>
@@ -5560,10 +5617,10 @@
         <v>199</v>
       </c>
       <c r="R17" s="14" t="n">
-        <v>52.337794</v>
+        <v>52.1625291742136</v>
       </c>
       <c r="S17" s="14" t="n">
-        <v>-127.826237</v>
+        <v>-128.144738642665</v>
       </c>
       <c r="T17" s="14" t="s">
         <v>200</v>
@@ -5617,10 +5674,10 @@
         <v>209</v>
       </c>
       <c r="R18" s="14" t="n">
-        <v>48.833479</v>
+        <v>48.8026460695892</v>
       </c>
       <c r="S18" s="14" t="n">
-        <v>-124.929585</v>
+        <v>-125.127619190205</v>
       </c>
       <c r="V18" s="8" t="s">
         <v>210</v>
@@ -5630,59 +5687,60 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="35" t="s">
         <v>212</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="36" t="s">
         <v>213</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21" t="s">
+      <c r="E19" s="36"/>
+      <c r="F19" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="13" t="s">
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="M19" s="13" t="s">
+      <c r="M19" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13" t="s">
+      <c r="N19" s="39"/>
+      <c r="O19" s="39" t="s">
         <v>219</v>
       </c>
-      <c r="P19" s="20" t="s">
+      <c r="P19" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="14" t="n">
-        <v>49.557619</v>
-      </c>
-      <c r="S19" s="14" t="n">
-        <v>-122.607872</v>
-      </c>
-      <c r="T19" s="14" t="s">
+      <c r="Q19" s="40"/>
+      <c r="R19" s="41" t="n">
+        <v>49.1861077501639</v>
+      </c>
+      <c r="S19" s="41" t="n">
+        <v>-122.695486242878</v>
+      </c>
+      <c r="T19" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="V19" s="8" t="str">
+      <c r="U19" s="42"/>
+      <c r="V19" s="43" t="str">
         <f aca="false">A19</f>
         <v>Katzie First Nation</v>
       </c>
-      <c r="W19" s="8" t="s">
+      <c r="W19" s="43" t="s">
         <v>222</v>
       </c>
     </row>
@@ -5735,10 +5793,10 @@
         <v>235</v>
       </c>
       <c r="R20" s="14" t="n">
-        <v>49.476845</v>
+        <v>49.171628990299</v>
       </c>
       <c r="S20" s="14" t="n">
-        <v>-122.296959</v>
+        <v>-122.565426566965</v>
       </c>
       <c r="T20" s="14" t="s">
         <v>236</v>
@@ -5749,10 +5807,10 @@
       <c r="W20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="45" t="s">
         <v>239</v>
       </c>
       <c r="C21" s="17" t="s">
@@ -5768,10 +5826,10 @@
       <c r="G21" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="38" t="s">
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="47" t="s">
         <v>32</v>
       </c>
       <c r="M21" s="13" t="s">
@@ -5799,13 +5857,13 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="49" t="s">
         <v>249</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="50" t="s">
         <v>250</v>
       </c>
       <c r="D22" s="20" t="s">
@@ -5818,10 +5876,10 @@
       <c r="G22" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="40" t="s">
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="49" t="s">
         <v>32</v>
       </c>
       <c r="M22" s="16" t="s">
@@ -5838,10 +5896,10 @@
         <v>257</v>
       </c>
       <c r="R22" s="14" t="n">
-        <v>49.451741</v>
+        <v>49.230208712611</v>
       </c>
       <c r="S22" s="14" t="n">
-        <v>-122.657791</v>
+        <v>-122.806119423045</v>
       </c>
       <c r="T22" s="14" t="s">
         <v>258</v>
@@ -5855,7 +5913,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="100.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="52" t="s">
         <v>260</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -5880,8 +5938,8 @@
       <c r="I23" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
       <c r="L23" s="13" t="s">
         <v>267</v>
       </c>
@@ -5899,10 +5957,10 @@
         <v>270</v>
       </c>
       <c r="R23" s="13" t="n">
-        <v>49.348358</v>
+        <v>49.2064434730953</v>
       </c>
       <c r="S23" s="14" t="n">
-        <v>-122.106774</v>
+        <v>-122.027744007433</v>
       </c>
       <c r="V23" s="8" t="s">
         <v>271</v>
@@ -5912,10 +5970,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="53" t="s">
         <v>273</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="54" t="s">
         <v>274</v>
       </c>
       <c r="C24" s="13" t="s">
@@ -5960,10 +6018,10 @@
         <v>283</v>
       </c>
       <c r="R24" s="14" t="n">
-        <v>51.287872</v>
+        <v>50.8708388662502</v>
       </c>
       <c r="S24" s="14" t="n">
-        <v>-118.990533</v>
+        <v>-119.599497552904</v>
       </c>
       <c r="V24" s="8" t="s">
         <v>284</v>
@@ -5971,10 +6029,10 @@
       <c r="W24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="48" t="s">
         <v>285</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="49" t="s">
         <v>286</v>
       </c>
       <c r="C25" s="13" t="s">
@@ -6017,10 +6075,10 @@
         <v>297</v>
       </c>
       <c r="R25" s="14" t="n">
-        <v>53.944696</v>
+        <v>54.0088875710237</v>
       </c>
       <c r="S25" s="14" t="n">
-        <v>-121.694171</v>
+        <v>-122.614309870554</v>
       </c>
       <c r="V25" s="8" t="s">
         <v>298</v>
@@ -6074,10 +6132,10 @@
         <v>310</v>
       </c>
       <c r="R26" s="14" t="n">
-        <v>52.953049</v>
+        <v>52.9551054413743</v>
       </c>
       <c r="S26" s="14" t="n">
-        <v>-122.449172</v>
+        <v>-122.450977710068</v>
       </c>
       <c r="V26" s="8" t="str">
         <f aca="false">A26</f>
@@ -6108,11 +6166,11 @@
       <c r="H27" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="I27" s="46" t="s">
+      <c r="I27" s="55" t="s">
         <v>318</v>
       </c>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
       <c r="L27" s="13" t="s">
         <v>149</v>
       </c>
@@ -6130,10 +6188,10 @@
         <v>321</v>
       </c>
       <c r="R27" s="14" t="n">
-        <v>50.006984</v>
+        <v>50.1390924737866</v>
       </c>
       <c r="S27" s="14" t="n">
-        <v>-121.261538</v>
+        <v>-120.862534877965</v>
       </c>
       <c r="V27" s="8" t="s">
         <v>322</v>
@@ -6141,7 +6199,7 @@
       <c r="W27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="56" t="s">
         <v>323</v>
       </c>
       <c r="B28" s="13" t="s">
@@ -6150,10 +6208,10 @@
       <c r="C28" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="57" t="s">
         <v>326</v>
       </c>
-      <c r="E28" s="48"/>
+      <c r="E28" s="57"/>
       <c r="F28" s="21" t="s">
         <v>327</v>
       </c>
@@ -6163,7 +6221,7 @@
       <c r="I28" s="24"/>
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
-      <c r="L28" s="38" t="s">
+      <c r="L28" s="47" t="s">
         <v>32</v>
       </c>
       <c r="M28" s="16" t="s">
@@ -6178,10 +6236,10 @@
       </c>
       <c r="Q28" s="16"/>
       <c r="R28" s="14" t="n">
-        <v>49.845148</v>
+        <v>49.1149186382442</v>
       </c>
       <c r="S28" s="14" t="n">
-        <v>-118.987733</v>
+        <v>-119.724028514332</v>
       </c>
       <c r="V28" s="8" t="s">
         <v>331</v>
@@ -6191,7 +6249,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="56.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="58" t="s">
         <v>333</v>
       </c>
       <c r="B29" s="13" t="s">
@@ -6219,10 +6277,10 @@
       <c r="J29" s="22" t="s">
         <v>339</v>
       </c>
-      <c r="K29" s="50" t="s">
+      <c r="K29" s="59" t="s">
         <v>339</v>
       </c>
-      <c r="L29" s="51" t="s">
+      <c r="L29" s="60" t="s">
         <v>32</v>
       </c>
       <c r="M29" s="13" t="s">
@@ -6239,10 +6297,10 @@
         <v>343</v>
       </c>
       <c r="R29" s="14" t="n">
-        <v>48.941803</v>
+        <v>49.1149186382442</v>
       </c>
       <c r="S29" s="14" t="n">
-        <v>-123.490134</v>
+        <v>-119.724028514332</v>
       </c>
       <c r="V29" s="8" t="str">
         <f aca="false">A29</f>
@@ -6284,14 +6342,14 @@
       <c r="K30" s="22" t="s">
         <v>350</v>
       </c>
-      <c r="L30" s="52" t="s">
+      <c r="L30" s="61" t="s">
         <v>149</v>
       </c>
       <c r="M30" s="16" t="s">
         <v>351</v>
       </c>
       <c r="N30" s="16"/>
-      <c r="O30" s="41" t="s">
+      <c r="O30" s="50" t="s">
         <v>352</v>
       </c>
       <c r="P30" s="13" t="s">
@@ -6301,10 +6359,10 @@
         <v>354</v>
       </c>
       <c r="R30" s="14" t="n">
-        <v>48.655944</v>
+        <v>48.6145785901937</v>
       </c>
       <c r="S30" s="14" t="n">
-        <v>-124.000524</v>
+        <v>-123.520458277224</v>
       </c>
       <c r="V30" s="8" t="str">
         <f aca="false">A30</f>
@@ -6315,7 +6373,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="62" t="s">
         <v>356</v>
       </c>
       <c r="B31" s="13" t="s">
@@ -6335,9 +6393,9 @@
         <v>361</v>
       </c>
       <c r="H31" s="14"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
       <c r="L31" s="13" t="s">
         <v>267</v>
       </c>
@@ -6345,7 +6403,7 @@
         <v>362</v>
       </c>
       <c r="N31" s="16"/>
-      <c r="O31" s="41" t="s">
+      <c r="O31" s="50" t="s">
         <v>255</v>
       </c>
       <c r="P31" s="13" t="s">
@@ -6353,10 +6411,10 @@
       </c>
       <c r="Q31" s="16"/>
       <c r="R31" s="14" t="n">
-        <v>49.290611</v>
+        <v>49.1061587257785</v>
       </c>
       <c r="S31" s="14" t="n">
-        <v>-122.361868</v>
+        <v>-122.3423931218</v>
       </c>
       <c r="V31" s="8" t="str">
         <f aca="false">A31</f>
@@ -6370,7 +6428,7 @@
       <c r="A32" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="63" t="s">
         <v>366</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -6383,7 +6441,7 @@
       <c r="F32" s="21" t="s">
         <v>369</v>
       </c>
-      <c r="G32" s="48" t="s">
+      <c r="G32" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H32" s="23" t="s">
@@ -6405,7 +6463,7 @@
         <v>178</v>
       </c>
       <c r="N32" s="13"/>
-      <c r="O32" s="41" t="s">
+      <c r="O32" s="50" t="s">
         <v>233</v>
       </c>
       <c r="P32" s="13" t="s">
@@ -6415,10 +6473,10 @@
         <v>375</v>
       </c>
       <c r="R32" s="14" t="n">
-        <v>49.353225</v>
+        <v>49.2249998356386</v>
       </c>
       <c r="S32" s="14" t="n">
-        <v>-123.012956</v>
+        <v>-123.199062838371</v>
       </c>
       <c r="V32" s="8" t="s">
         <v>376</v>
@@ -6444,7 +6502,7 @@
       <c r="F33" s="28" t="s">
         <v>380</v>
       </c>
-      <c r="G33" s="48" t="s">
+      <c r="G33" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H33" s="23" t="s">
@@ -6476,10 +6534,10 @@
         <v>386</v>
       </c>
       <c r="R33" s="14" t="n">
-        <v>51.21274</v>
+        <v>50.7743341531046</v>
       </c>
       <c r="S33" s="14" t="n">
-        <v>-118.846623</v>
+        <v>-119.717236920099</v>
       </c>
       <c r="V33" s="8" t="str">
         <f aca="false">A33</f>
@@ -6493,7 +6551,7 @@
       <c r="A34" s="19" t="s">
         <v>388</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="64" t="s">
         <v>389</v>
       </c>
       <c r="C34" s="13" t="s">
@@ -6538,10 +6596,10 @@
         <v>399</v>
       </c>
       <c r="R34" s="14" t="n">
-        <v>49.690318</v>
+        <v>50.1540952465102</v>
       </c>
       <c r="S34" s="14" t="n">
-        <v>-120.648292</v>
+        <v>-121.037387988603</v>
       </c>
       <c r="V34" s="8" t="str">
         <f aca="false">A34</f>
@@ -6552,7 +6610,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="65" t="s">
         <v>401</v>
       </c>
       <c r="B35" s="13" t="s">
@@ -6561,11 +6619,11 @@
       <c r="C35" s="13" t="s">
         <v>403</v>
       </c>
-      <c r="D35" s="48" t="s">
+      <c r="D35" s="57" t="s">
         <v>404</v>
       </c>
-      <c r="E35" s="48"/>
-      <c r="F35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="20" t="s">
         <v>405</v>
       </c>
@@ -6590,10 +6648,10 @@
         <v>408</v>
       </c>
       <c r="R35" s="14" t="n">
-        <v>49.114526</v>
+        <v>49.1838485514573</v>
       </c>
       <c r="S35" s="14" t="n">
-        <v>-118.489264</v>
+        <v>-119.53315191045</v>
       </c>
       <c r="V35" s="8" t="str">
         <f aca="false">A35</f>
@@ -6620,7 +6678,7 @@
       <c r="F36" s="21" t="s">
         <v>412</v>
       </c>
-      <c r="G36" s="48" t="s">
+      <c r="G36" s="57" t="s">
         <v>405</v>
       </c>
       <c r="H36" s="13" t="s">
@@ -6652,10 +6710,10 @@
         <v>418</v>
       </c>
       <c r="R36" s="14" t="n">
-        <v>48.572918</v>
+        <v>48.5776249603665</v>
       </c>
       <c r="S36" s="14" t="n">
-        <v>-124.39459</v>
+        <v>-124.408374183131</v>
       </c>
       <c r="T36" s="14" t="s">
         <v>419</v>
@@ -6685,19 +6743,19 @@
       <c r="F37" s="21" t="s">
         <v>425</v>
       </c>
-      <c r="G37" s="48" t="s">
+      <c r="G37" s="57" t="s">
         <v>405</v>
       </c>
       <c r="H37" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="I37" s="48" t="s">
+      <c r="I37" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="J37" s="48" t="s">
+      <c r="J37" s="57" t="s">
         <v>426</v>
       </c>
-      <c r="K37" s="48" t="s">
+      <c r="K37" s="57" t="s">
         <v>177</v>
       </c>
       <c r="L37" s="25" t="s">
@@ -6715,10 +6773,10 @@
       </c>
       <c r="Q37" s="16"/>
       <c r="R37" s="14" t="n">
-        <v>48.724102</v>
+        <v>48.6274805537984</v>
       </c>
       <c r="S37" s="14" t="n">
-        <v>-123.324246</v>
+        <v>-123.458324726602</v>
       </c>
       <c r="V37" s="8" t="str">
         <f aca="false">A37</f>
@@ -6748,9 +6806,9 @@
       <c r="G38" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="35"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
       <c r="L38" s="25" t="s">
         <v>32</v>
       </c>
@@ -6768,10 +6826,10 @@
         <v>436</v>
       </c>
       <c r="R38" s="14" t="n">
-        <v>49.732366</v>
+        <v>49.4919586000844</v>
       </c>
       <c r="S38" s="14" t="n">
-        <v>-119.25376</v>
+        <v>-119.64469346526</v>
       </c>
       <c r="V38" s="8" t="str">
         <f aca="false">A38</f>
@@ -6799,9 +6857,9 @@
       <c r="G39" s="20" t="s">
         <v>441</v>
       </c>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="35"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
       <c r="L39" s="25" t="s">
         <v>32</v>
       </c>
@@ -6819,10 +6877,10 @@
         <v>445</v>
       </c>
       <c r="R39" s="14" t="n">
-        <v>49.505163</v>
+        <v>49.301445389115</v>
       </c>
       <c r="S39" s="14" t="n">
-        <v>-121.482617</v>
+        <v>-121.65894728452</v>
       </c>
       <c r="V39" s="19" t="s">
         <v>446</v>
@@ -6849,9 +6907,9 @@
       <c r="G40" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
       <c r="L40" s="25" t="s">
         <v>32</v>
       </c>
@@ -6869,10 +6927,10 @@
         <v>454</v>
       </c>
       <c r="R40" s="14" t="n">
-        <v>48.892388</v>
+        <v>48.9713063265927</v>
       </c>
       <c r="S40" s="14" t="n">
-        <v>-123.675652</v>
+        <v>-123.660015052681</v>
       </c>
       <c r="V40" s="8" t="str">
         <f aca="false">A40</f>
@@ -6908,8 +6966,8 @@
       <c r="I41" s="20" t="s">
         <v>462</v>
       </c>
-      <c r="J41" s="35"/>
-      <c r="K41" s="35"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
       <c r="L41" s="25" t="s">
         <v>32</v>
       </c>
@@ -6925,10 +6983,10 @@
       </c>
       <c r="Q41" s="16"/>
       <c r="R41" s="14" t="n">
-        <v>49.57071</v>
+        <v>49.2117251903373</v>
       </c>
       <c r="S41" s="14" t="n">
-        <v>-121.506875</v>
+        <v>-121.724435730428</v>
       </c>
       <c r="V41" s="8" t="str">
         <f aca="false">A41</f>
@@ -6956,9 +7014,9 @@
       <c r="G42" s="20" t="s">
         <v>469</v>
       </c>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="35"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
       <c r="L42" s="25" t="s">
         <v>32</v>
       </c>
@@ -6973,10 +7031,10 @@
       </c>
       <c r="Q42" s="16"/>
       <c r="R42" s="14" t="n">
-        <v>49.205717</v>
+        <v>49.2361523125496</v>
       </c>
       <c r="S42" s="14" t="n">
-        <v>-122.910944</v>
+        <v>-123.024138032549</v>
       </c>
       <c r="T42" s="14" t="s">
         <v>472</v>
@@ -6989,7 +7047,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="98.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="58" t="s">
+      <c r="A43" s="67" t="s">
         <v>475</v>
       </c>
       <c r="B43" s="20" t="s">
@@ -7011,13 +7069,13 @@
       <c r="H43" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="I43" s="48" t="s">
+      <c r="I43" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="J43" s="48" t="s">
+      <c r="J43" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="K43" s="48" t="s">
+      <c r="K43" s="57" t="s">
         <v>177</v>
       </c>
       <c r="L43" s="25" t="s">
@@ -7037,10 +7095,10 @@
         <v>483</v>
       </c>
       <c r="R43" s="14" t="n">
-        <v>48.440888</v>
+        <v>48.3384365237503</v>
       </c>
       <c r="S43" s="14" t="n">
-        <v>-123.676887</v>
+        <v>-123.606675180898</v>
       </c>
       <c r="V43" s="8" t="s">
         <v>484</v>
@@ -7048,64 +7106,66 @@
       <c r="W43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="68" t="s">
         <v>485</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="21" t="s">
         <v>486</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="69" t="s">
         <v>487</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="21" t="s">
         <v>488</v>
       </c>
-      <c r="E44" s="20"/>
+      <c r="E44" s="21"/>
       <c r="F44" s="21" t="s">
         <v>489</v>
       </c>
-      <c r="G44" s="48" t="s">
+      <c r="G44" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H44" s="23" t="s">
+      <c r="H44" s="70" t="s">
         <v>490</v>
       </c>
-      <c r="I44" s="20" t="s">
+      <c r="I44" s="21" t="s">
         <v>491</v>
       </c>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="48" t="s">
+      <c r="J44" s="71"/>
+      <c r="K44" s="71"/>
+      <c r="L44" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="M44" s="20" t="s">
+      <c r="M44" s="21" t="s">
         <v>492</v>
       </c>
-      <c r="N44" s="20"/>
-      <c r="O44" s="14" t="s">
+      <c r="N44" s="21"/>
+      <c r="O44" s="72" t="s">
         <v>443</v>
       </c>
-      <c r="P44" s="13" t="s">
+      <c r="P44" s="28" t="s">
         <v>493</v>
       </c>
-      <c r="Q44" s="16" t="s">
+      <c r="Q44" s="69" t="s">
         <v>494</v>
       </c>
-      <c r="R44" s="14" t="n">
-        <v>49.25517</v>
-      </c>
-      <c r="S44" s="14" t="n">
-        <v>-121.964821</v>
-      </c>
-      <c r="V44" s="8" t="s">
+      <c r="R44" s="72" t="n">
+        <v>49.2360660445914</v>
+      </c>
+      <c r="S44" s="72" t="n">
+        <v>-122.002526922047</v>
+      </c>
+      <c r="T44" s="73"/>
+      <c r="U44" s="73"/>
+      <c r="V44" s="74" t="s">
         <v>485</v>
       </c>
-      <c r="W44" s="8" t="s">
+      <c r="W44" s="74" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="57.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="58" t="s">
+      <c r="A45" s="67" t="s">
         <v>496</v>
       </c>
       <c r="B45" s="20" t="s">
@@ -7143,7 +7203,7 @@
         <v>505</v>
       </c>
       <c r="N45" s="16"/>
-      <c r="O45" s="60" t="s">
+      <c r="O45" s="75" t="s">
         <v>443</v>
       </c>
       <c r="P45" s="13" t="s">
@@ -7170,12 +7230,12 @@
         <v>508</v>
       </c>
       <c r="C46" s="20"/>
-      <c r="D46" s="61" t="s">
+      <c r="D46" s="76" t="s">
         <v>509</v>
       </c>
-      <c r="E46" s="61"/>
-      <c r="F46" s="62"/>
-      <c r="G46" s="48" t="s">
+      <c r="E46" s="76"/>
+      <c r="F46" s="77"/>
+      <c r="G46" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H46" s="23" t="s">
@@ -7197,10 +7257,10 @@
         <v>178</v>
       </c>
       <c r="N46" s="13"/>
-      <c r="O46" s="63" t="s">
+      <c r="O46" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="P46" s="64" t="s">
+      <c r="P46" s="79" t="s">
         <v>513</v>
       </c>
       <c r="Q46" s="17" t="s">
@@ -7248,9 +7308,9 @@
       <c r="I47" s="20" t="s">
         <v>522</v>
       </c>
-      <c r="J47" s="35"/>
-      <c r="K47" s="35"/>
-      <c r="L47" s="48" t="s">
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="57" t="s">
         <v>32</v>
       </c>
       <c r="M47" s="0" t="s">
@@ -7279,7 +7339,7 @@
       <c r="W47" s="14"/>
     </row>
     <row r="48" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="65" t="s">
+      <c r="A48" s="80" t="s">
         <v>526</v>
       </c>
       <c r="B48" s="13" t="s">
@@ -7295,7 +7355,7 @@
       <c r="F48" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G48" s="48" t="s">
+      <c r="G48" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H48" s="20" t="s">
@@ -7310,7 +7370,7 @@
       <c r="K48" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="L48" s="38" t="s">
+      <c r="L48" s="47" t="s">
         <v>32</v>
       </c>
       <c r="M48" s="16" t="s">
@@ -7336,7 +7396,7 @@
       <c r="W48" s="14"/>
     </row>
     <row r="49" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="58" t="s">
+      <c r="A49" s="67" t="s">
         <v>534</v>
       </c>
       <c r="B49" s="20" t="s">
@@ -7349,8 +7409,8 @@
         <v>537</v>
       </c>
       <c r="E49" s="20"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="48" t="s">
+      <c r="F49" s="77"/>
+      <c r="G49" s="57" t="s">
         <v>538</v>
       </c>
       <c r="H49" s="23" t="s">
@@ -7362,17 +7422,17 @@
       <c r="J49" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="K49" s="66" t="s">
+      <c r="K49" s="81" t="s">
         <v>542</v>
       </c>
-      <c r="L49" s="67" t="s">
+      <c r="L49" s="82" t="s">
         <v>32</v>
       </c>
       <c r="M49" s="13" t="s">
         <v>178</v>
       </c>
       <c r="N49" s="13"/>
-      <c r="O49" s="60" t="s">
+      <c r="O49" s="75" t="s">
         <v>35</v>
       </c>
       <c r="P49" s="13" t="s">
@@ -7387,7 +7447,7 @@
       <c r="S49" s="14" t="n">
         <v>-121.484624</v>
       </c>
-      <c r="V49" s="68" t="s">
+      <c r="V49" s="83" t="s">
         <v>64</v>
       </c>
       <c r="W49" s="8" t="s">
@@ -7395,10 +7455,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="39.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="69" t="s">
+      <c r="A50" s="84" t="s">
         <v>546</v>
       </c>
-      <c r="B50" s="70" t="s">
+      <c r="B50" s="85" t="s">
         <v>547</v>
       </c>
       <c r="C50" s="20" t="s">
@@ -7426,17 +7486,17 @@
       <c r="K50" s="20" t="s">
         <v>554</v>
       </c>
-      <c r="L50" s="71" t="s">
+      <c r="L50" s="86" t="s">
         <v>267</v>
       </c>
       <c r="M50" s="16" t="s">
         <v>555</v>
       </c>
       <c r="N50" s="16"/>
-      <c r="O50" s="60" t="s">
+      <c r="O50" s="75" t="s">
         <v>443</v>
       </c>
-      <c r="P50" s="72" t="s">
+      <c r="P50" s="87" t="s">
         <v>556</v>
       </c>
       <c r="Q50" s="17" t="s">
@@ -7456,10 +7516,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="73" t="s">
+      <c r="A51" s="88" t="s">
         <v>559</v>
       </c>
-      <c r="B51" s="74" t="s">
+      <c r="B51" s="89" t="s">
         <v>560</v>
       </c>
       <c r="C51" s="16" t="s">
@@ -7469,7 +7529,7 @@
         <v>562</v>
       </c>
       <c r="E51" s="20"/>
-      <c r="F51" s="62"/>
+      <c r="F51" s="77"/>
       <c r="G51" s="20" t="s">
         <v>563</v>
       </c>
@@ -7487,7 +7547,7 @@
       <c r="O51" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="P51" s="75" t="s">
+      <c r="P51" s="90" t="s">
         <v>564</v>
       </c>
       <c r="Q51" s="17" t="s">
@@ -7507,7 +7567,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="58" t="s">
+      <c r="A52" s="67" t="s">
         <v>567</v>
       </c>
       <c r="B52" s="20" t="s">
@@ -7520,7 +7580,7 @@
         <v>570</v>
       </c>
       <c r="E52" s="20"/>
-      <c r="F52" s="76" t="s">
+      <c r="F52" s="91" t="s">
         <v>569</v>
       </c>
       <c r="G52" s="22" t="s">
@@ -7532,8 +7592,8 @@
       <c r="I52" s="20" t="s">
         <v>573</v>
       </c>
-      <c r="J52" s="35"/>
-      <c r="K52" s="35"/>
+      <c r="J52" s="46"/>
+      <c r="K52" s="46"/>
       <c r="L52" s="25" t="s">
         <v>574</v>
       </c>
@@ -7544,7 +7604,7 @@
       <c r="O52" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="P52" s="63" t="s">
+      <c r="P52" s="78" t="s">
         <v>576</v>
       </c>
       <c r="Q52" s="17" t="s">
@@ -7580,13 +7640,13 @@
       <c r="F53" s="21" t="s">
         <v>584</v>
       </c>
-      <c r="G53" s="48" t="s">
+      <c r="G53" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I53" s="35"/>
-      <c r="J53" s="35"/>
-      <c r="K53" s="35"/>
-      <c r="L53" s="48" t="s">
+      <c r="I53" s="46"/>
+      <c r="J53" s="46"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="57" t="s">
         <v>32</v>
       </c>
       <c r="M53" s="16" t="s">
@@ -7631,19 +7691,19 @@
       <c r="F54" s="21" t="s">
         <v>590</v>
       </c>
-      <c r="G54" s="48" t="s">
+      <c r="G54" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="48" t="s">
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="M54" s="48" t="s">
+      <c r="M54" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="N54" s="48"/>
+      <c r="N54" s="57"/>
       <c r="O54" s="14" t="s">
         <v>443</v>
       </c>
@@ -7657,10 +7717,10 @@
       <c r="S54" s="14" t="n">
         <v>-121.484624</v>
       </c>
-      <c r="V54" s="68" t="s">
+      <c r="V54" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="W54" s="68" t="s">
+      <c r="W54" s="83" t="s">
         <v>593</v>
       </c>
     </row>
@@ -7684,10 +7744,10 @@
       <c r="G55" s="20" t="s">
         <v>599</v>
       </c>
-      <c r="I55" s="35"/>
-      <c r="J55" s="35"/>
-      <c r="K55" s="35"/>
-      <c r="L55" s="48" t="s">
+      <c r="I55" s="46"/>
+      <c r="J55" s="46"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="57" t="s">
         <v>32</v>
       </c>
       <c r="M55" s="16" t="s">
@@ -7733,12 +7793,12 @@
       <c r="F56" s="28" t="s">
         <v>607</v>
       </c>
-      <c r="G56" s="48" t="s">
+      <c r="G56" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I56" s="35"/>
-      <c r="J56" s="35"/>
-      <c r="K56" s="35"/>
+      <c r="I56" s="46"/>
+      <c r="J56" s="46"/>
+      <c r="K56" s="46"/>
       <c r="L56" s="0" t="s">
         <v>32</v>
       </c>
@@ -7763,7 +7823,7 @@
       </c>
       <c r="V56" s="8" t="str">
         <f aca="false">A56</f>
-        <v>Shuswap Indian Band </v>
+        <v>Shuswap Indian Band</v>
       </c>
       <c r="W56" s="8" t="s">
         <v>611</v>
@@ -7786,10 +7846,10 @@
       <c r="F57" s="28" t="s">
         <v>614</v>
       </c>
-      <c r="G57" s="48" t="s">
+      <c r="G57" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="L57" s="48" t="s">
+      <c r="L57" s="57" t="s">
         <v>32</v>
       </c>
       <c r="M57" s="13" t="s">
@@ -7820,7 +7880,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="40.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="77" t="s">
+      <c r="A58" s="92" t="s">
         <v>620</v>
       </c>
       <c r="B58" s="13" t="s">
@@ -7839,7 +7899,7 @@
       <c r="G58" s="20" t="s">
         <v>624</v>
       </c>
-      <c r="L58" s="48" t="s">
+      <c r="L58" s="57" t="s">
         <v>32</v>
       </c>
       <c r="M58" s="16" t="s">
@@ -7886,7 +7946,7 @@
       <c r="F59" s="28" t="s">
         <v>631</v>
       </c>
-      <c r="G59" s="48" t="s">
+      <c r="G59" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H59" s="23" t="s">
@@ -7908,7 +7968,7 @@
         <v>636</v>
       </c>
       <c r="N59" s="13"/>
-      <c r="O59" s="78" t="s">
+      <c r="O59" s="93" t="s">
         <v>151</v>
       </c>
       <c r="P59" s="13" t="s">
@@ -7938,7 +7998,7 @@
       <c r="B60" s="13" t="s">
         <v>641</v>
       </c>
-      <c r="C60" s="55" t="s">
+      <c r="C60" s="64" t="s">
         <v>642</v>
       </c>
       <c r="D60" s="13" t="s">
@@ -7951,10 +8011,10 @@
       <c r="G60" s="20" t="s">
         <v>644</v>
       </c>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="48" t="s">
+      <c r="I60" s="46"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="57" t="s">
         <v>32</v>
       </c>
       <c r="M60" s="16" t="s">
@@ -7984,7 +8044,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="77" t="s">
+      <c r="A61" s="92" t="s">
         <v>648</v>
       </c>
       <c r="B61" s="13" t="s">
@@ -8000,19 +8060,19 @@
       <c r="F61" s="28" t="s">
         <v>652</v>
       </c>
-      <c r="G61" s="48" t="s">
+      <c r="G61" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I61" s="35"/>
-      <c r="J61" s="35"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="48" t="s">
+      <c r="I61" s="46"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
+      <c r="L61" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="M61" s="55" t="s">
+      <c r="M61" s="64" t="s">
         <v>178</v>
       </c>
-      <c r="N61" s="55"/>
+      <c r="N61" s="64"/>
       <c r="O61" s="14" t="s">
         <v>443</v>
       </c>
@@ -8034,7 +8094,7 @@
       <c r="W61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="42.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="79" t="s">
+      <c r="A62" s="94" t="s">
         <v>656</v>
       </c>
       <c r="B62" s="13" t="s">
@@ -8093,7 +8153,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="79" t="s">
+      <c r="A63" s="94" t="s">
         <v>669</v>
       </c>
       <c r="B63" s="13" t="s">
@@ -8112,10 +8172,10 @@
       <c r="G63" s="20" t="s">
         <v>673</v>
       </c>
-      <c r="H63" s="80"/>
-      <c r="I63" s="46"/>
-      <c r="J63" s="46"/>
-      <c r="K63" s="46"/>
+      <c r="H63" s="95"/>
+      <c r="I63" s="55"/>
+      <c r="J63" s="55"/>
+      <c r="K63" s="55"/>
       <c r="L63" s="25" t="s">
         <v>32</v>
       </c>
@@ -8149,7 +8209,7 @@
       <c r="A64" s="19" t="s">
         <v>677</v>
       </c>
-      <c r="B64" s="48" t="s">
+      <c r="B64" s="57" t="s">
         <v>678</v>
       </c>
       <c r="C64" s="20" t="s">
@@ -8162,7 +8222,7 @@
       <c r="F64" s="28" t="s">
         <v>681</v>
       </c>
-      <c r="G64" s="48" t="s">
+      <c r="G64" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H64" s="13" t="s">
@@ -8177,14 +8237,14 @@
       <c r="K64" s="22" t="s">
         <v>683</v>
       </c>
-      <c r="L64" s="66" t="s">
+      <c r="L64" s="81" t="s">
         <v>32</v>
       </c>
       <c r="M64" s="16" t="s">
         <v>684</v>
       </c>
       <c r="N64" s="16"/>
-      <c r="O64" s="60" t="s">
+      <c r="O64" s="75" t="s">
         <v>35</v>
       </c>
       <c r="P64" s="13" t="s">
@@ -8221,12 +8281,12 @@
       <c r="F65" s="28" t="s">
         <v>690</v>
       </c>
-      <c r="G65" s="48" t="s">
+      <c r="G65" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I65" s="35"/>
-      <c r="J65" s="35"/>
-      <c r="K65" s="35"/>
+      <c r="I65" s="46"/>
+      <c r="J65" s="46"/>
+      <c r="K65" s="46"/>
       <c r="L65" s="0" t="s">
         <v>32</v>
       </c>
@@ -8273,12 +8333,12 @@
       <c r="F66" s="28" t="s">
         <v>701</v>
       </c>
-      <c r="G66" s="48" t="s">
+      <c r="G66" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I66" s="35"/>
-      <c r="J66" s="35"/>
-      <c r="K66" s="35"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="46"/>
+      <c r="K66" s="46"/>
       <c r="L66" s="0" t="s">
         <v>32</v>
       </c>
@@ -8309,7 +8369,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="65" t="s">
+      <c r="A67" s="80" t="s">
         <v>707</v>
       </c>
       <c r="B67" s="13" t="s">
@@ -8323,12 +8383,12 @@
       </c>
       <c r="E67" s="13"/>
       <c r="F67" s="28"/>
-      <c r="G67" s="48" t="s">
+      <c r="G67" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I67" s="35"/>
-      <c r="J67" s="35"/>
-      <c r="K67" s="35"/>
+      <c r="I67" s="46"/>
+      <c r="J67" s="46"/>
+      <c r="K67" s="46"/>
       <c r="L67" s="0" t="s">
         <v>32</v>
       </c>
@@ -8336,7 +8396,7 @@
         <v>711</v>
       </c>
       <c r="N67" s="16"/>
-      <c r="O67" s="60" t="s">
+      <c r="O67" s="75" t="s">
         <v>35</v>
       </c>
       <c r="P67" s="13" t="s">
@@ -8359,7 +8419,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="47.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="58" t="s">
+      <c r="A68" s="67" t="s">
         <v>715</v>
       </c>
       <c r="B68" s="23" t="s">
@@ -8375,7 +8435,7 @@
       <c r="F68" s="28" t="s">
         <v>717</v>
       </c>
-      <c r="G68" s="48" t="s">
+      <c r="G68" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H68" s="23" t="s">
@@ -8397,7 +8457,7 @@
         <v>721</v>
       </c>
       <c r="N68" s="16"/>
-      <c r="O68" s="60" t="s">
+      <c r="O68" s="75" t="s">
         <v>35</v>
       </c>
       <c r="P68" s="20" t="s">
@@ -8437,10 +8497,10 @@
       <c r="G69" s="13" t="s">
         <v>729</v>
       </c>
-      <c r="H69" s="35"/>
-      <c r="I69" s="35"/>
-      <c r="J69" s="35"/>
-      <c r="K69" s="35"/>
+      <c r="H69" s="46"/>
+      <c r="I69" s="46"/>
+      <c r="J69" s="46"/>
+      <c r="K69" s="46"/>
       <c r="L69" s="0" t="s">
         <v>32</v>
       </c>
@@ -8470,7 +8530,7 @@
       <c r="W69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="77" t="s">
+      <c r="A70" s="92" t="s">
         <v>733</v>
       </c>
       <c r="B70" s="13" t="s">
@@ -8486,13 +8546,13 @@
       <c r="F70" s="28" t="s">
         <v>735</v>
       </c>
-      <c r="G70" s="48" t="s">
+      <c r="G70" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="H70" s="35"/>
-      <c r="I70" s="35"/>
-      <c r="J70" s="35"/>
-      <c r="K70" s="35"/>
+      <c r="H70" s="46"/>
+      <c r="I70" s="46"/>
+      <c r="J70" s="46"/>
+      <c r="K70" s="46"/>
       <c r="L70" s="0" t="s">
         <v>32</v>
       </c>
@@ -8535,7 +8595,7 @@
       <c r="F71" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="G71" s="48" t="s">
+      <c r="G71" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H71" s="23" t="s">
@@ -8557,7 +8617,7 @@
         <v>178</v>
       </c>
       <c r="N71" s="20"/>
-      <c r="O71" s="60" t="s">
+      <c r="O71" s="75" t="s">
         <v>452</v>
       </c>
       <c r="P71" s="13" t="s">
@@ -8580,7 +8640,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="79" t="s">
+      <c r="A72" s="94" t="s">
         <v>747</v>
       </c>
       <c r="B72" s="13" t="s">
@@ -8596,7 +8656,7 @@
       <c r="F72" s="28" t="s">
         <v>749</v>
       </c>
-      <c r="G72" s="48" t="s">
+      <c r="G72" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H72" s="23" t="s">
@@ -8611,12 +8671,12 @@
       <c r="K72" s="22" t="s">
         <v>752</v>
       </c>
-      <c r="L72" s="81"/>
-      <c r="M72" s="60" t="s">
+      <c r="L72" s="96"/>
+      <c r="M72" s="75" t="s">
         <v>178</v>
       </c>
-      <c r="N72" s="60"/>
-      <c r="O72" s="60" t="s">
+      <c r="N72" s="75"/>
+      <c r="O72" s="75" t="s">
         <v>753</v>
       </c>
       <c r="P72" s="13" t="s">
@@ -8655,7 +8715,7 @@
       <c r="F73" s="28" t="s">
         <v>761</v>
       </c>
-      <c r="G73" s="70" t="s">
+      <c r="G73" s="85" t="s">
         <v>762</v>
       </c>
       <c r="H73" s="13" t="s">
@@ -8675,7 +8735,7 @@
         <v>178</v>
       </c>
       <c r="N73" s="13"/>
-      <c r="O73" s="60" t="s">
+      <c r="O73" s="75" t="s">
         <v>766</v>
       </c>
       <c r="P73" s="13" t="s">
@@ -8702,7 +8762,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="58" t="s">
+      <c r="A74" s="67" t="s">
         <v>771</v>
       </c>
       <c r="B74" s="13" t="s">
@@ -8715,10 +8775,10 @@
         <v>774</v>
       </c>
       <c r="E74" s="13"/>
-      <c r="F74" s="82" t="s">
+      <c r="F74" s="97" t="s">
         <v>775</v>
       </c>
-      <c r="G74" s="74" t="s">
+      <c r="G74" s="89" t="s">
         <v>776</v>
       </c>
       <c r="H74" s="23" t="s">
@@ -8727,8 +8787,8 @@
       <c r="I74" s="22" t="s">
         <v>778</v>
       </c>
-      <c r="J74" s="46"/>
-      <c r="K74" s="46"/>
+      <c r="J74" s="55"/>
+      <c r="K74" s="55"/>
       <c r="L74" s="25"/>
       <c r="M74" s="23" t="s">
         <v>779</v>
@@ -8772,15 +8832,15 @@
       <c r="G75" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I75" s="35"/>
-      <c r="J75" s="35"/>
-      <c r="K75" s="35"/>
+      <c r="I75" s="46"/>
+      <c r="J75" s="46"/>
+      <c r="K75" s="46"/>
       <c r="L75" s="13"/>
       <c r="M75" s="13" t="s">
         <v>178</v>
       </c>
       <c r="N75" s="13"/>
-      <c r="O75" s="60" t="s">
+      <c r="O75" s="75" t="s">
         <v>753</v>
       </c>
       <c r="P75" s="13" t="s">
@@ -8803,7 +8863,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="77" t="s">
+      <c r="A76" s="92" t="s">
         <v>789</v>
       </c>
       <c r="B76" s="13" t="s">
@@ -8820,15 +8880,15 @@
       <c r="G76" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H76" s="35"/>
-      <c r="I76" s="35"/>
-      <c r="J76" s="35"/>
-      <c r="K76" s="35"/>
+      <c r="H76" s="46"/>
+      <c r="I76" s="46"/>
+      <c r="J76" s="46"/>
+      <c r="K76" s="46"/>
       <c r="M76" s="16" t="s">
         <v>793</v>
       </c>
       <c r="N76" s="16"/>
-      <c r="O76" s="60" t="s">
+      <c r="O76" s="75" t="s">
         <v>35</v>
       </c>
       <c r="P76" s="13" t="s">
@@ -8887,7 +8947,7 @@
         <v>804</v>
       </c>
       <c r="N77" s="13"/>
-      <c r="O77" s="60" t="s">
+      <c r="O77" s="75" t="s">
         <v>805</v>
       </c>
       <c r="P77" s="13" t="s">
@@ -8930,7 +8990,7 @@
       <c r="F78" s="21" t="s">
         <v>814</v>
       </c>
-      <c r="G78" s="48" t="s">
+      <c r="G78" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H78" s="23" t="s">
@@ -8950,7 +9010,7 @@
         <v>818</v>
       </c>
       <c r="N78" s="16"/>
-      <c r="O78" s="60" t="s">
+      <c r="O78" s="75" t="s">
         <v>753</v>
       </c>
       <c r="P78" s="13" t="s">
@@ -8983,14 +9043,14 @@
       <c r="C79" s="13" t="s">
         <v>824</v>
       </c>
-      <c r="D79" s="83" t="s">
+      <c r="D79" s="98" t="s">
         <v>825</v>
       </c>
-      <c r="E79" s="83"/>
-      <c r="F79" s="84" t="s">
+      <c r="E79" s="98"/>
+      <c r="F79" s="99" t="s">
         <v>826</v>
       </c>
-      <c r="G79" s="48" t="s">
+      <c r="G79" s="57" t="s">
         <v>827</v>
       </c>
       <c r="H79" s="20" t="s">
@@ -8999,8 +9059,8 @@
       <c r="I79" s="20" t="s">
         <v>829</v>
       </c>
-      <c r="J79" s="35"/>
-      <c r="K79" s="35"/>
+      <c r="J79" s="46"/>
+      <c r="K79" s="46"/>
       <c r="L79" s="13" t="s">
         <v>830</v>
       </c>
@@ -9008,7 +9068,7 @@
         <v>684</v>
       </c>
       <c r="N79" s="16"/>
-      <c r="O79" s="60" t="s">
+      <c r="O79" s="75" t="s">
         <v>35</v>
       </c>
       <c r="P79" s="13" t="s">
@@ -9049,9 +9109,9 @@
       <c r="G80" s="20" t="s">
         <v>838</v>
       </c>
-      <c r="I80" s="35"/>
-      <c r="J80" s="35"/>
-      <c r="K80" s="35"/>
+      <c r="I80" s="46"/>
+      <c r="J80" s="46"/>
+      <c r="K80" s="46"/>
       <c r="M80" s="16" t="s">
         <v>48</v>
       </c>
@@ -9085,7 +9145,7 @@
       <c r="B81" s="13" t="s">
         <v>843</v>
       </c>
-      <c r="C81" s="85" t="s">
+      <c r="C81" s="100" t="s">
         <v>844</v>
       </c>
       <c r="D81" s="13" t="s">
@@ -9095,7 +9155,7 @@
       <c r="F81" s="28" t="s">
         <v>846</v>
       </c>
-      <c r="G81" s="48" t="s">
+      <c r="G81" s="57" t="s">
         <v>29</v>
       </c>
       <c r="H81" s="13" t="s">
@@ -9108,7 +9168,7 @@
         <v>848</v>
       </c>
       <c r="N81" s="16"/>
-      <c r="O81" s="60" t="s">
+      <c r="O81" s="75" t="s">
         <v>295</v>
       </c>
       <c r="P81" s="13" t="s">
@@ -9151,14 +9211,14 @@
       <c r="G82" s="20" t="s">
         <v>857</v>
       </c>
-      <c r="I82" s="35"/>
-      <c r="J82" s="35"/>
-      <c r="K82" s="35"/>
+      <c r="I82" s="46"/>
+      <c r="J82" s="46"/>
+      <c r="K82" s="46"/>
       <c r="M82" s="16" t="s">
         <v>858</v>
       </c>
       <c r="N82" s="16"/>
-      <c r="O82" s="60"/>
+      <c r="O82" s="75"/>
       <c r="P82" s="13"/>
       <c r="Q82" s="16"/>
       <c r="R82" s="14" t="n">
@@ -9187,15 +9247,15 @@
       </c>
       <c r="E83" s="13"/>
       <c r="F83" s="28"/>
-      <c r="G83" s="48" t="s">
+      <c r="G83" s="57" t="s">
         <v>864</v>
       </c>
       <c r="H83" s="23" t="s">
         <v>865</v>
       </c>
-      <c r="I83" s="35"/>
-      <c r="J83" s="35"/>
-      <c r="K83" s="35"/>
+      <c r="I83" s="46"/>
+      <c r="J83" s="46"/>
+      <c r="K83" s="46"/>
       <c r="L83" s="13"/>
       <c r="M83" s="16" t="s">
         <v>866</v>
@@ -9223,7 +9283,7 @@
       <c r="W83" s="8"/>
     </row>
     <row r="84" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="77" t="s">
+      <c r="A84" s="92" t="s">
         <v>869</v>
       </c>
       <c r="B84" s="13" t="s">
@@ -9236,15 +9296,15 @@
         <v>872</v>
       </c>
       <c r="E84" s="13"/>
-      <c r="F84" s="86" t="s">
+      <c r="F84" s="69" t="s">
         <v>871</v>
       </c>
-      <c r="G84" s="48" t="s">
+      <c r="G84" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="I84" s="35"/>
-      <c r="J84" s="35"/>
-      <c r="K84" s="35"/>
+      <c r="I84" s="46"/>
+      <c r="J84" s="46"/>
+      <c r="K84" s="46"/>
       <c r="L84" s="13"/>
       <c r="M84" s="16" t="s">
         <v>873</v>
@@ -9299,8 +9359,8 @@
       <c r="I85" s="27" t="s">
         <v>884</v>
       </c>
-      <c r="J85" s="35"/>
-      <c r="K85" s="35"/>
+      <c r="J85" s="46"/>
+      <c r="K85" s="46"/>
       <c r="L85" s="25"/>
       <c r="M85" s="16" t="s">
         <v>885</v>
@@ -9344,8 +9404,8 @@
       <c r="I86" s="20" t="s">
         <v>892</v>
       </c>
-      <c r="J86" s="35"/>
-      <c r="K86" s="35"/>
+      <c r="J86" s="46"/>
+      <c r="K86" s="46"/>
       <c r="L86" s="25"/>
       <c r="M86" s="16" t="s">
         <v>885</v>
@@ -9379,15 +9439,15 @@
       <c r="G87" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I87" s="35"/>
-      <c r="J87" s="35"/>
-      <c r="K87" s="35"/>
+      <c r="I87" s="46"/>
+      <c r="J87" s="46"/>
+      <c r="K87" s="46"/>
       <c r="L87" s="25"/>
       <c r="M87" s="16" t="s">
         <v>896</v>
       </c>
       <c r="N87" s="16"/>
-      <c r="O87" s="87"/>
+      <c r="O87" s="101"/>
       <c r="P87" s="13" t="s">
         <v>897</v>
       </c>
@@ -9426,9 +9486,9 @@
       <c r="G88" s="20" t="s">
         <v>904</v>
       </c>
-      <c r="I88" s="35"/>
-      <c r="J88" s="35"/>
-      <c r="K88" s="35"/>
+      <c r="I88" s="46"/>
+      <c r="J88" s="46"/>
+      <c r="K88" s="46"/>
       <c r="M88" s="16" t="s">
         <v>48</v>
       </c>
@@ -9481,8 +9541,8 @@
       <c r="I89" s="20" t="s">
         <v>915</v>
       </c>
-      <c r="J89" s="35"/>
-      <c r="K89" s="35"/>
+      <c r="J89" s="46"/>
+      <c r="K89" s="46"/>
       <c r="L89" s="0" t="s">
         <v>149</v>
       </c>
@@ -9507,7 +9567,7 @@
       </c>
       <c r="V89" s="8" t="str">
         <f aca="false">A89</f>
-        <v>Yale First Nation </v>
+        <v>Yale First Nation</v>
       </c>
       <c r="W89" s="8"/>
     </row>
@@ -9528,12 +9588,12 @@
       <c r="F90" s="28" t="s">
         <v>923</v>
       </c>
-      <c r="G90" s="48" t="s">
+      <c r="G90" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="I90" s="35"/>
-      <c r="J90" s="35"/>
-      <c r="K90" s="35"/>
+      <c r="I90" s="46"/>
+      <c r="J90" s="46"/>
+      <c r="K90" s="46"/>
       <c r="L90" s="0" t="s">
         <v>32</v>
       </c>
@@ -9563,23 +9623,23 @@
       <c r="W90" s="8"/>
     </row>
     <row r="91" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="88"/>
-      <c r="B91" s="89"/>
-      <c r="C91" s="89"/>
-      <c r="D91" s="90"/>
-      <c r="E91" s="90"/>
-      <c r="F91" s="90"/>
-      <c r="G91" s="90"/>
-      <c r="H91" s="90"/>
-      <c r="I91" s="90"/>
-      <c r="J91" s="90"/>
-      <c r="K91" s="90"/>
-      <c r="L91" s="90"/>
-      <c r="M91" s="90"/>
-      <c r="N91" s="90"/>
-      <c r="O91" s="90"/>
-      <c r="P91" s="89"/>
-      <c r="Q91" s="91"/>
+      <c r="A91" s="102"/>
+      <c r="B91" s="103"/>
+      <c r="C91" s="103"/>
+      <c r="D91" s="104"/>
+      <c r="E91" s="104"/>
+      <c r="F91" s="104"/>
+      <c r="G91" s="104"/>
+      <c r="H91" s="104"/>
+      <c r="I91" s="104"/>
+      <c r="J91" s="104"/>
+      <c r="K91" s="104"/>
+      <c r="L91" s="104"/>
+      <c r="M91" s="104"/>
+      <c r="N91" s="104"/>
+      <c r="O91" s="104"/>
+      <c r="P91" s="103"/>
+      <c r="Q91" s="105"/>
     </row>
     <row r="92" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="30" t="s">
@@ -9838,13 +9898,13 @@
       <c r="A1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="106" t="s">
         <v>931</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="106" t="s">
         <v>932</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="107" t="s">
         <v>933</v>
       </c>
     </row>
@@ -9853,13 +9913,13 @@
         <f aca="false">'BC First Nations'!A3</f>
         <v>Adams Lake Indian Band (belongs to the Secwepemc Nation, member of the Shuswap Nation Triabal Council)</v>
       </c>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="106" t="s">
         <v>934</v>
       </c>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D2" s="94" t="s">
+      <c r="D2" s="108" t="s">
         <v>936</v>
       </c>
     </row>
@@ -9868,13 +9928,13 @@
         <f aca="false">'BC First Nations'!A4</f>
         <v>Aitchelitz Band</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="106" t="s">
         <v>48</v>
       </c>
     </row>
@@ -9883,13 +9943,13 @@
         <f aca="false">'BC First Nations'!A5</f>
         <v>Ashcroft Indian Band</v>
       </c>
-      <c r="B4" s="92" t="s">
+      <c r="B4" s="106" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D4" s="92" t="s">
+      <c r="D4" s="106" t="s">
         <v>60</v>
       </c>
     </row>
@@ -9898,13 +9958,13 @@
         <f aca="false">'BC First Nations'!A6</f>
         <v>Boothroyd Band</v>
       </c>
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="92" t="s">
+      <c r="C5" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D5" s="95" t="s">
+      <c r="D5" s="109" t="s">
         <v>938</v>
       </c>
     </row>
@@ -9913,13 +9973,13 @@
         <f aca="false">'BC First Nations'!A7</f>
         <v>Boston Bar First Nations</v>
       </c>
-      <c r="B6" s="92" t="s">
+      <c r="B6" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="D6" s="106" t="s">
         <v>77</v>
       </c>
     </row>
@@ -9928,13 +9988,13 @@
         <f aca="false">'BC First Nations'!A8</f>
         <v>Canim Lake Band (The People of Broken Rock "The Tsq'escenemc")</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="107" t="s">
         <v>937</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="106" t="s">
         <v>939</v>
       </c>
     </row>
@@ -9943,13 +10003,13 @@
         <f aca="false">'BC First Nations'!A9</f>
         <v>Chawathil First Nation</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="106" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="92" t="s">
+      <c r="C8" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="106" t="s">
         <v>102</v>
       </c>
     </row>
@@ -9958,28 +10018,28 @@
         <f aca="false">'BC First Nations'!A10</f>
         <v>Chi:yo:m Agassiz (Cheam) First Nation - meaning "Wild Strawberry Place"</v>
       </c>
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="106" t="s">
         <v>940</v>
       </c>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="106" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
         <f aca="false">'BC First Nations'!A11</f>
-        <v>Coldwater First Nation (Nc/etko - the people of the creeks)      </v>
-      </c>
-      <c r="B10" s="92" t="s">
+        <v>Coldwater First Nation (Nc/etko - the people of the creeks)</v>
+      </c>
+      <c r="B10" s="106" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D10" s="92" t="s">
+      <c r="D10" s="106" t="s">
         <v>941</v>
       </c>
     </row>
@@ -9988,13 +10048,13 @@
         <f aca="false">'BC First Nations'!A12</f>
         <v>Cook's Ferry Indian Band Kumcheen (Variation Nkumcheen); Includes Pokheistk (Variation Pakeist, Pokheistsk), Pemynoos (Variation Piminos), Spatsum (Variation Spaptsin), Spence'S Bridge</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="106" t="s">
         <v>942</v>
       </c>
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="106" t="s">
         <v>943</v>
       </c>
     </row>
@@ -10003,13 +10063,13 @@
         <f aca="false">'BC First Nations'!A13</f>
         <v>Cowichan Tribes</v>
       </c>
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D12" s="92" t="s">
+      <c r="D12" s="106" t="s">
         <v>150</v>
       </c>
     </row>
@@ -10018,13 +10078,13 @@
         <f aca="false">'BC First Nations'!A14</f>
         <v>Ditidaht First Nation Formerly Nitinaht (Pre-1984) (Variation Nitinat)</v>
       </c>
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="C13" s="92" t="s">
+      <c r="C13" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="106" t="s">
         <v>944</v>
       </c>
     </row>
@@ -10033,28 +10093,28 @@
         <f aca="false">'BC First Nations'!A15</f>
         <v>Esquimalt Nation (Xwsepsum or Kosapsum)</v>
       </c>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="106" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="92" t="s">
+      <c r="C14" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D14" s="95" t="s">
+      <c r="D14" s="109" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="str">
         <f aca="false">'BC First Nations'!A16</f>
-        <v>Halalt First Nation </v>
-      </c>
-      <c r="B15" s="92" t="s">
+        <v>Halalt First Nation</v>
+      </c>
+      <c r="B15" s="106" t="s">
         <v>946</v>
       </c>
-      <c r="C15" s="92" t="s">
+      <c r="C15" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D15" s="92" t="s">
+      <c r="D15" s="106" t="s">
         <v>947</v>
       </c>
     </row>
@@ -10063,28 +10123,28 @@
         <f aca="false">'BC First Nations'!A17</f>
         <v>Heiltsuk First Nation</v>
       </c>
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="106" t="s">
         <v>192</v>
       </c>
-      <c r="C16" s="92" t="s">
+      <c r="C16" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D16" s="92" t="s">
+      <c r="D16" s="106" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="str">
         <f aca="false">'BC First Nations'!A18</f>
-        <v>Huu-ay-aht First Nation </v>
-      </c>
-      <c r="B17" s="92" t="s">
+        <v>Huu-ay-aht First Nation</v>
+      </c>
+      <c r="B17" s="106" t="s">
         <v>948</v>
       </c>
-      <c r="C17" s="92" t="s">
+      <c r="C17" s="106" t="s">
         <v>949</v>
       </c>
-      <c r="D17" s="92" t="s">
+      <c r="D17" s="106" t="s">
         <v>950</v>
       </c>
     </row>
@@ -10093,13 +10153,13 @@
         <f aca="false">'BC First Nations'!A19</f>
         <v>Katzie First Nation</v>
       </c>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="106" t="s">
         <v>212</v>
       </c>
-      <c r="C18" s="92" t="s">
+      <c r="C18" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D18" s="92" t="s">
+      <c r="D18" s="106" t="s">
         <v>951</v>
       </c>
     </row>
@@ -10108,28 +10168,28 @@
         <f aca="false">'BC First Nations'!A20</f>
         <v>Kwantlen First Nation (tireless Runner)</v>
       </c>
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="106" t="s">
         <v>237</v>
       </c>
-      <c r="C19" s="92" t="s">
+      <c r="C19" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D19" s="92" t="s">
+      <c r="D19" s="106" t="s">
         <v>952</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="str">
         <f aca="false">'BC First Nations'!A21</f>
-        <v>Kwaw -Kwaw-Aplit First Nations </v>
-      </c>
-      <c r="B20" s="92" t="s">
+        <v>Kwaw -Kwaw-Aplit First Nations</v>
+      </c>
+      <c r="B20" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="C20" s="92" t="s">
+      <c r="C20" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D20" s="92" t="s">
+      <c r="D20" s="106" t="s">
         <v>953</v>
       </c>
     </row>
@@ -10138,13 +10198,13 @@
         <f aca="false">'BC First Nations'!A22</f>
         <v>Kwikwetlem First Nation</v>
       </c>
-      <c r="B21" s="92" t="s">
+      <c r="B21" s="106" t="s">
         <v>248</v>
       </c>
-      <c r="C21" s="92" t="s">
+      <c r="C21" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D21" s="92" t="s">
+      <c r="D21" s="106" t="s">
         <v>254</v>
       </c>
     </row>
@@ -10153,13 +10213,13 @@
         <f aca="false">'BC First Nations'!A23</f>
         <v>Leq' a: mel First Nation</v>
       </c>
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="106" t="s">
         <v>260</v>
       </c>
-      <c r="C22" s="92" t="s">
+      <c r="C22" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D22" s="92" t="s">
+      <c r="D22" s="106" t="s">
         <v>268</v>
       </c>
     </row>
@@ -10168,13 +10228,13 @@
         <f aca="false">'BC First Nations'!A24</f>
         <v>Little Shuswap Lake Indian Band (Skwlax meaning "Black Bear")</v>
       </c>
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="106" t="s">
         <v>284</v>
       </c>
-      <c r="C23" s="92" t="s">
+      <c r="C23" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D23" s="92" t="s">
+      <c r="D23" s="106" t="s">
         <v>281</v>
       </c>
     </row>
@@ -10183,13 +10243,13 @@
         <f aca="false">'BC First Nations'!A25</f>
         <v>Lheidli T'enneh First Nation</v>
       </c>
-      <c r="B24" s="92" t="s">
+      <c r="B24" s="106" t="s">
         <v>285</v>
       </c>
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D24" s="92" t="s">
+      <c r="D24" s="106" t="s">
         <v>294</v>
       </c>
     </row>
@@ -10198,13 +10258,13 @@
         <f aca="false">'BC First Nations'!A26</f>
         <v>Lhtako Dene Nation</v>
       </c>
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="106" t="s">
         <v>300</v>
       </c>
-      <c r="C25" s="92" t="s">
+      <c r="C25" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D25" s="92" t="s">
+      <c r="D25" s="106" t="s">
         <v>308</v>
       </c>
     </row>
@@ -10213,13 +10273,13 @@
         <f aca="false">'BC First Nations'!A27</f>
         <v>Lower Nicola Indian Band -</v>
       </c>
-      <c r="B26" s="92" t="s">
+      <c r="B26" s="106" t="s">
         <v>322</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="C26" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D26" s="92" t="s">
+      <c r="D26" s="106" t="s">
         <v>319</v>
       </c>
     </row>
@@ -10228,13 +10288,13 @@
         <f aca="false">'BC First Nations'!A28</f>
         <v>Lower Similkameen #598</v>
       </c>
-      <c r="B27" s="92" t="s">
+      <c r="B27" s="106" t="s">
         <v>323</v>
       </c>
-      <c r="C27" s="92" t="s">
+      <c r="C27" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D27" s="92" t="s">
+      <c r="D27" s="106" t="s">
         <v>329</v>
       </c>
     </row>
@@ -10243,13 +10303,13 @@
         <f aca="false">'BC First Nations'!A29</f>
         <v>Lyackson First Nation</v>
       </c>
-      <c r="B28" s="92" t="s">
+      <c r="B28" s="106" t="s">
         <v>333</v>
       </c>
-      <c r="C28" s="92" t="s">
+      <c r="C28" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D28" s="92" t="s">
+      <c r="D28" s="106" t="s">
         <v>341</v>
       </c>
     </row>
@@ -10258,13 +10318,13 @@
         <f aca="false">'BC First Nations'!A30</f>
         <v>Malahat First Nation</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B29" s="106" t="s">
         <v>345</v>
       </c>
-      <c r="C29" s="92" t="s">
+      <c r="C29" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D29" s="92" t="s">
+      <c r="D29" s="106" t="s">
         <v>351</v>
       </c>
     </row>
@@ -10273,13 +10333,13 @@
         <f aca="false">'BC First Nations'!A31</f>
         <v>Matsqui First Nation</v>
       </c>
-      <c r="B30" s="92" t="s">
+      <c r="B30" s="106" t="s">
         <v>356</v>
       </c>
-      <c r="C30" s="92" t="s">
+      <c r="C30" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D30" s="92" t="s">
+      <c r="D30" s="106" t="s">
         <v>362</v>
       </c>
     </row>
@@ -10288,13 +10348,13 @@
         <f aca="false">'BC First Nations'!A32</f>
         <v>Musqeam Indian Band</v>
       </c>
-      <c r="B31" s="92" t="s">
+      <c r="B31" s="106" t="s">
         <v>365</v>
       </c>
-      <c r="C31" s="92" t="s">
+      <c r="C31" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D31" s="95" t="s">
+      <c r="D31" s="109" t="s">
         <v>954</v>
       </c>
     </row>
@@ -10303,13 +10363,13 @@
         <f aca="false">'BC First Nations'!A33</f>
         <v>Neskonlith Indian Band</v>
       </c>
-      <c r="B32" s="92" t="s">
+      <c r="B32" s="106" t="s">
         <v>378</v>
       </c>
-      <c r="C32" s="92" t="s">
+      <c r="C32" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D32" s="92" t="s">
+      <c r="D32" s="106" t="s">
         <v>384</v>
       </c>
     </row>
@@ -10318,13 +10378,13 @@
         <f aca="false">'BC First Nations'!A34</f>
         <v>Nooaitch Indian Band</v>
       </c>
-      <c r="B33" s="92" t="s">
+      <c r="B33" s="106" t="s">
         <v>388</v>
       </c>
-      <c r="C33" s="92" t="s">
+      <c r="C33" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D33" s="92" t="s">
+      <c r="D33" s="106" t="s">
         <v>396</v>
       </c>
     </row>
@@ -10333,13 +10393,13 @@
         <f aca="false">'BC First Nations'!A35</f>
         <v>Osoyoos</v>
       </c>
-      <c r="B34" s="92" t="s">
+      <c r="B34" s="106" t="s">
         <v>401</v>
       </c>
-      <c r="C34" s="92" t="s">
+      <c r="C34" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D34" s="92" t="s">
+      <c r="D34" s="106" t="s">
         <v>406</v>
       </c>
     </row>
@@ -10348,13 +10408,13 @@
         <f aca="false">'BC First Nations'!A36</f>
         <v>Pacheedaht First Nation</v>
       </c>
-      <c r="B35" s="92" t="s">
+      <c r="B35" s="106" t="s">
         <v>410</v>
       </c>
-      <c r="C35" s="92" t="s">
+      <c r="C35" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D35" s="92" t="s">
+      <c r="D35" s="106" t="s">
         <v>416</v>
       </c>
     </row>
@@ -10363,13 +10423,13 @@
         <f aca="false">'BC First Nations'!A37</f>
         <v>Pauquachin Nation</v>
       </c>
-      <c r="B36" s="92" t="s">
+      <c r="B36" s="106" t="s">
         <v>421</v>
       </c>
-      <c r="C36" s="92" t="s">
+      <c r="C36" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D36" s="95" t="s">
+      <c r="D36" s="109" t="s">
         <v>955</v>
       </c>
     </row>
@@ -10378,13 +10438,13 @@
         <f aca="false">'BC First Nations'!A38</f>
         <v>Penticton Indian Band</v>
       </c>
-      <c r="B37" s="92" t="s">
+      <c r="B37" s="106" t="s">
         <v>429</v>
       </c>
-      <c r="C37" s="92" t="s">
+      <c r="C37" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D37" s="92" t="s">
+      <c r="D37" s="106" t="s">
         <v>434</v>
       </c>
     </row>
@@ -10393,13 +10453,13 @@
         <f aca="false">'BC First Nations'!A39</f>
         <v>Peters Band (Peters First Nation)</v>
       </c>
-      <c r="B38" s="92" t="s">
+      <c r="B38" s="106" t="s">
         <v>437</v>
       </c>
-      <c r="C38" s="92" t="s">
+      <c r="C38" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D38" s="92" t="s">
+      <c r="D38" s="106" t="s">
         <v>442</v>
       </c>
     </row>
@@ -10408,13 +10468,13 @@
         <f aca="false">'BC First Nations'!A40</f>
         <v>Penelakut Tribe</v>
       </c>
-      <c r="B39" s="92" t="s">
+      <c r="B39" s="106" t="s">
         <v>447</v>
       </c>
-      <c r="C39" s="92" t="s">
+      <c r="C39" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D39" s="92" t="s">
+      <c r="D39" s="106" t="s">
         <v>451</v>
       </c>
     </row>
@@ -10423,28 +10483,28 @@
         <f aca="false">'BC First Nations'!A41</f>
         <v>Popkum First Nation</v>
       </c>
-      <c r="B40" s="92" t="s">
+      <c r="B40" s="106" t="s">
         <v>456</v>
       </c>
-      <c r="C40" s="92" t="s">
+      <c r="C40" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D40" s="92" t="s">
+      <c r="D40" s="106" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="str">
         <f aca="false">'BC First Nations'!A42</f>
-        <v>Qayqayt First Nation (New Westminister) </v>
-      </c>
-      <c r="B41" s="92" t="s">
+        <v>Qayqayt First Nation (New Westminister)</v>
+      </c>
+      <c r="B41" s="106" t="s">
         <v>956</v>
       </c>
-      <c r="C41" s="92" t="s">
+      <c r="C41" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D41" s="95" t="s">
+      <c r="D41" s="109" t="s">
         <v>957</v>
       </c>
     </row>
@@ -10453,13 +10513,13 @@
         <f aca="false">'BC First Nations'!A43</f>
         <v>Scia'new First Nation (Beecher Bay First Nation)</v>
       </c>
-      <c r="B42" s="92" t="s">
+      <c r="B42" s="106" t="s">
         <v>475</v>
       </c>
-      <c r="C42" s="92" t="s">
+      <c r="C42" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D42" s="92" t="s">
+      <c r="D42" s="106" t="s">
         <v>481</v>
       </c>
     </row>
@@ -10468,13 +10528,13 @@
         <f aca="false">'BC First Nations'!A44</f>
         <v>Sq'ewlets (Scowlitz) First Nation</v>
       </c>
-      <c r="B43" s="92" t="s">
+      <c r="B43" s="106" t="s">
         <v>485</v>
       </c>
-      <c r="C43" s="92" t="s">
+      <c r="C43" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D43" s="92" t="s">
+      <c r="D43" s="106" t="s">
         <v>958</v>
       </c>
     </row>
@@ -10483,13 +10543,13 @@
         <f aca="false">'BC First Nations'!A45</f>
         <v>Seabird Island Band</v>
       </c>
-      <c r="B44" s="92" t="s">
+      <c r="B44" s="106" t="s">
         <v>496</v>
       </c>
-      <c r="C44" s="92" t="s">
+      <c r="C44" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D44" s="92" t="s">
+      <c r="D44" s="106" t="s">
         <v>505</v>
       </c>
     </row>
@@ -10498,13 +10558,13 @@
         <f aca="false">'BC First Nations'!A46</f>
         <v>Secwepmc (suh-Meh-much) of the Secwepmc Nation</v>
       </c>
-      <c r="B45" s="92" t="s">
+      <c r="B45" s="106" t="s">
         <v>507</v>
       </c>
-      <c r="C45" s="92" t="s">
+      <c r="C45" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D45" s="95" t="s">
+      <c r="D45" s="109" t="s">
         <v>959</v>
       </c>
     </row>
@@ -10513,28 +10573,28 @@
         <f aca="false">'BC First Nations'!A47</f>
         <v>Semiahmoo First Nation</v>
       </c>
-      <c r="B46" s="92" t="s">
+      <c r="B46" s="106" t="s">
         <v>516</v>
       </c>
-      <c r="C46" s="92" t="s">
+      <c r="C46" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D46" s="95" t="s">
+      <c r="D46" s="109" t="s">
         <v>960</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="str">
         <f aca="false">'BC First Nations'!A49</f>
-        <v>Shackan Indian Band </v>
-      </c>
-      <c r="B47" s="92" t="s">
+        <v>Shackan Indian Band</v>
+      </c>
+      <c r="B47" s="106" t="s">
         <v>961</v>
       </c>
-      <c r="C47" s="92" t="s">
+      <c r="C47" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D47" s="95" t="s">
+      <c r="D47" s="109" t="s">
         <v>962</v>
       </c>
     </row>
@@ -10543,13 +10603,13 @@
         <f aca="false">'BC First Nations'!A50</f>
         <v>Shxw'owhamel First Nation</v>
       </c>
-      <c r="B48" s="92" t="s">
+      <c r="B48" s="106" t="s">
         <v>546</v>
       </c>
-      <c r="C48" s="92" t="s">
+      <c r="C48" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D48" s="92" t="s">
+      <c r="D48" s="106" t="s">
         <v>555</v>
       </c>
     </row>
@@ -10558,13 +10618,13 @@
         <f aca="false">'BC First Nations'!A51</f>
         <v>Shxwha:y Villiage</v>
       </c>
-      <c r="B49" s="92" t="s">
+      <c r="B49" s="106" t="s">
         <v>559</v>
       </c>
-      <c r="C49" s="92" t="s">
+      <c r="C49" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D49" s="92" t="s">
+      <c r="D49" s="106" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10573,13 +10633,13 @@
         <f aca="false">'BC First Nations'!A52</f>
         <v>Simpcw First Nation "People of the Rivers"</v>
       </c>
-      <c r="B50" s="92" t="s">
+      <c r="B50" s="106" t="s">
         <v>578</v>
       </c>
-      <c r="C50" s="92" t="s">
+      <c r="C50" s="106" t="s">
         <v>949</v>
       </c>
-      <c r="D50" s="92" t="s">
+      <c r="D50" s="106" t="s">
         <v>963</v>
       </c>
     </row>
@@ -10588,28 +10648,28 @@
         <f aca="false">'BC First Nations'!A53</f>
         <v>Siska Indian Band</v>
       </c>
-      <c r="B51" s="92" t="s">
+      <c r="B51" s="106" t="s">
         <v>580</v>
       </c>
-      <c r="C51" s="92" t="s">
+      <c r="C51" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D51" s="92" t="s">
+      <c r="D51" s="106" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="str">
         <f aca="false">'BC First Nations'!A54</f>
-        <v>Skuppah Indian Band </v>
-      </c>
-      <c r="B52" s="92" t="s">
+        <v>Skuppah Indian Band</v>
+      </c>
+      <c r="B52" s="106" t="s">
         <v>964</v>
       </c>
-      <c r="C52" s="92" t="s">
+      <c r="C52" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D52" s="95" t="s">
+      <c r="D52" s="109" t="s">
         <v>938</v>
       </c>
     </row>
@@ -10618,28 +10678,28 @@
         <f aca="false">'BC First Nations'!A55</f>
         <v>Skowkale First Nation</v>
       </c>
-      <c r="B53" s="92" t="s">
+      <c r="B53" s="106" t="s">
         <v>594</v>
       </c>
-      <c r="C53" s="92" t="s">
+      <c r="C53" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D53" s="92" t="s">
+      <c r="D53" s="106" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="str">
         <f aca="false">'BC First Nations'!A56</f>
-        <v>Shuswap Indian Band </v>
-      </c>
-      <c r="B54" s="92" t="s">
+        <v>Shuswap Indian Band</v>
+      </c>
+      <c r="B54" s="106" t="s">
         <v>965</v>
       </c>
-      <c r="C54" s="92" t="s">
+      <c r="C54" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D54" s="92" t="s">
+      <c r="D54" s="106" t="s">
         <v>966</v>
       </c>
     </row>
@@ -10648,13 +10708,13 @@
         <f aca="false">'BC First Nations'!A57</f>
         <v>Skawahlook First Nation</v>
       </c>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="106" t="s">
         <v>612</v>
       </c>
-      <c r="C55" s="92" t="s">
+      <c r="C55" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D55" s="92" t="s">
+      <c r="D55" s="106" t="s">
         <v>967</v>
       </c>
     </row>
@@ -10663,13 +10723,13 @@
         <f aca="false">'BC First Nations'!A58</f>
         <v>Skwah First Nation</v>
       </c>
-      <c r="B56" s="92" t="s">
+      <c r="B56" s="106" t="s">
         <v>620</v>
       </c>
-      <c r="C56" s="92" t="s">
+      <c r="C56" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D56" s="92" t="s">
+      <c r="D56" s="106" t="s">
         <v>625</v>
       </c>
     </row>
@@ -10678,13 +10738,13 @@
         <f aca="false">'BC First Nations'!A59</f>
         <v>Snuneymuxw First Nation</v>
       </c>
-      <c r="B57" s="92" t="s">
+      <c r="B57" s="106" t="s">
         <v>629</v>
       </c>
-      <c r="C57" s="92" t="s">
+      <c r="C57" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D57" s="92" t="s">
+      <c r="D57" s="106" t="s">
         <v>968</v>
       </c>
     </row>
@@ -10693,13 +10753,13 @@
         <f aca="false">'BC First Nations'!A60</f>
         <v>Soowahlie First Nation</v>
       </c>
-      <c r="B58" s="92" t="s">
+      <c r="B58" s="106" t="s">
         <v>640</v>
       </c>
-      <c r="C58" s="92" t="s">
+      <c r="C58" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D58" s="92" t="s">
+      <c r="D58" s="106" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10708,13 +10768,13 @@
         <f aca="false">'BC First Nations'!A61</f>
         <v>Spuzzum First Nation</v>
       </c>
-      <c r="B59" s="92" t="s">
+      <c r="B59" s="106" t="s">
         <v>648</v>
       </c>
-      <c r="C59" s="92" t="s">
+      <c r="C59" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D59" s="95" t="s">
+      <c r="D59" s="109" t="s">
         <v>938</v>
       </c>
     </row>
@@ -10723,13 +10783,13 @@
         <f aca="false">'BC First Nations'!A62</f>
         <v>Squamish First Nation (Squ-Ho-0-meesh)</v>
       </c>
-      <c r="B60" s="92" t="s">
+      <c r="B60" s="106" t="s">
         <v>667</v>
       </c>
-      <c r="C60" s="92" t="s">
+      <c r="C60" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D60" s="92" t="s">
+      <c r="D60" s="106" t="s">
         <v>969</v>
       </c>
     </row>
@@ -10738,43 +10798,43 @@
         <f aca="false">'BC First Nations'!A63</f>
         <v>Squiala First Nation</v>
       </c>
-      <c r="B61" s="92" t="s">
+      <c r="B61" s="106" t="s">
         <v>669</v>
       </c>
-      <c r="C61" s="92" t="s">
+      <c r="C61" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D61" s="92" t="s">
+      <c r="D61" s="106" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="str">
         <f aca="false">'BC First Nations'!A64</f>
-        <v>Stk'emlupsemc Te Secwepemc </v>
-      </c>
-      <c r="B62" s="92" t="s">
+        <v>Stk'emlupsemc Te Secwepemc</v>
+      </c>
+      <c r="B62" s="106" t="s">
         <v>970</v>
       </c>
-      <c r="C62" s="92" t="s">
+      <c r="C62" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D62" s="92" t="s">
+      <c r="D62" s="106" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="str">
         <f aca="false">'BC First Nations'!A65</f>
-        <v>Sts'ailes Band (Chehalls Indian Band) </v>
-      </c>
-      <c r="B63" s="92" t="s">
+        <v>Sts'ailes Band (Chehalls Indian Band)</v>
+      </c>
+      <c r="B63" s="106" t="s">
         <v>695</v>
       </c>
-      <c r="C63" s="92" t="s">
+      <c r="C63" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D63" s="92" t="s">
+      <c r="D63" s="106" t="s">
         <v>692</v>
       </c>
     </row>
@@ -10783,13 +10843,13 @@
         <f aca="false">'BC First Nations'!A66</f>
         <v>Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek)</v>
       </c>
-      <c r="B64" s="92" t="s">
+      <c r="B64" s="106" t="s">
         <v>697</v>
       </c>
-      <c r="C64" s="92" t="s">
+      <c r="C64" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D64" s="92" t="s">
+      <c r="D64" s="106" t="s">
         <v>702</v>
       </c>
     </row>
@@ -10798,13 +10858,13 @@
         <f aca="false">'BC First Nations'!A67</f>
         <v>St'uxwtews (Bonaparte Indian Band)</v>
       </c>
-      <c r="B65" s="92" t="s">
+      <c r="B65" s="106" t="s">
         <v>707</v>
       </c>
-      <c r="C65" s="92" t="s">
+      <c r="C65" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D65" s="92" t="s">
+      <c r="D65" s="106" t="s">
         <v>711</v>
       </c>
     </row>
@@ -10813,13 +10873,13 @@
         <f aca="false">'BC First Nations'!A68</f>
         <v>Stz'uminus First Nation (ltst uw' hw-nuts'-ul-wun) Chemainus</v>
       </c>
-      <c r="B66" s="92" t="s">
+      <c r="B66" s="106" t="s">
         <v>724</v>
       </c>
-      <c r="C66" s="92" t="s">
+      <c r="C66" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D66" s="92" t="s">
+      <c r="D66" s="106" t="s">
         <v>721</v>
       </c>
     </row>
@@ -10828,13 +10888,13 @@
         <f aca="false">'BC First Nations'!A69</f>
         <v>Sumas First Nation</v>
       </c>
-      <c r="B67" s="92" t="s">
+      <c r="B67" s="106" t="s">
         <v>725</v>
       </c>
-      <c r="C67" s="92" t="s">
+      <c r="C67" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D67" s="92" t="s">
+      <c r="D67" s="106" t="s">
         <v>730</v>
       </c>
     </row>
@@ -10843,13 +10903,13 @@
         <f aca="false">'BC First Nations'!A70</f>
         <v>Toosey Indian Band (Tl'esqox)</v>
       </c>
-      <c r="B68" s="92" t="s">
+      <c r="B68" s="106" t="s">
         <v>971</v>
       </c>
-      <c r="C68" s="92" t="s">
+      <c r="C68" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D68" s="95" t="s">
+      <c r="D68" s="109" t="s">
         <v>972</v>
       </c>
     </row>
@@ -10858,13 +10918,13 @@
         <f aca="false">'BC First Nations'!A71</f>
         <v>Tsartlip First Nation</v>
       </c>
-      <c r="B69" s="92" t="s">
+      <c r="B69" s="106" t="s">
         <v>738</v>
       </c>
-      <c r="C69" s="92" t="s">
+      <c r="C69" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D69" s="95" t="s">
+      <c r="D69" s="109" t="s">
         <v>955</v>
       </c>
     </row>
@@ -10873,13 +10933,13 @@
         <f aca="false">'BC First Nations'!A72</f>
         <v>Tsawout First Nation</v>
       </c>
-      <c r="B70" s="92" t="s">
+      <c r="B70" s="106" t="s">
         <v>747</v>
       </c>
-      <c r="C70" s="92" t="s">
+      <c r="C70" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D70" s="95" t="s">
+      <c r="D70" s="109" t="s">
         <v>955</v>
       </c>
     </row>
@@ -10888,13 +10948,13 @@
         <f aca="false">'BC First Nations'!A73</f>
         <v>Tsawwassen First Nation</v>
       </c>
-      <c r="B71" s="92" t="s">
+      <c r="B71" s="106" t="s">
         <v>757</v>
       </c>
-      <c r="C71" s="92" t="s">
+      <c r="C71" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D71" s="95" t="s">
+      <c r="D71" s="109" t="s">
         <v>973</v>
       </c>
     </row>
@@ -10903,13 +10963,13 @@
         <f aca="false">'BC First Nations'!A74</f>
         <v>Ts'elxweyeqw Tribe Management Limited</v>
       </c>
-      <c r="B72" s="92" t="s">
+      <c r="B72" s="106" t="s">
         <v>771</v>
       </c>
-      <c r="C72" s="92" t="s">
+      <c r="C72" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D72" s="92" t="s">
+      <c r="D72" s="106" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10918,13 +10978,13 @@
         <f aca="false">'BC First Nations'!A75</f>
         <v>Tseycum First Nation</v>
       </c>
-      <c r="B73" s="92" t="s">
+      <c r="B73" s="106" t="s">
         <v>781</v>
       </c>
-      <c r="C73" s="92" t="s">
+      <c r="C73" s="106" t="s">
         <v>935</v>
       </c>
-      <c r="D73" s="95" t="s">
+      <c r="D73" s="109" t="s">
         <v>955</v>
       </c>
     </row>
@@ -10933,13 +10993,13 @@
         <f aca="false">'BC First Nations'!A76</f>
         <v>Ts'kwaylaxw (Pavillion Indian Band)</v>
       </c>
-      <c r="B74" s="92" t="s">
+      <c r="B74" s="106" t="s">
         <v>789</v>
       </c>
-      <c r="C74" s="92" t="s">
+      <c r="C74" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D74" s="92" t="s">
+      <c r="D74" s="106" t="s">
         <v>793</v>
       </c>
     </row>
@@ -10948,13 +11008,13 @@
         <f aca="false">'BC First Nations'!A77</f>
         <v>Tsleil Waututh Nation</v>
       </c>
-      <c r="B75" s="92" t="s">
+      <c r="B75" s="106" t="s">
         <v>797</v>
       </c>
-      <c r="C75" s="92" t="s">
+      <c r="C75" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D75" s="92" t="s">
+      <c r="D75" s="106" t="s">
         <v>974</v>
       </c>
     </row>
@@ -10963,13 +11023,13 @@
         <f aca="false">'BC First Nations'!A78</f>
         <v>T'Sou-ke Nation</v>
       </c>
-      <c r="B76" s="92" t="s">
+      <c r="B76" s="106" t="s">
         <v>810</v>
       </c>
-      <c r="C76" s="92" t="s">
+      <c r="C76" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D76" s="92" t="s">
+      <c r="D76" s="106" t="s">
         <v>818</v>
       </c>
     </row>
@@ -10978,13 +11038,13 @@
         <f aca="false">'BC First Nations'!A79</f>
         <v>Tk'emlups te Secwepemc</v>
       </c>
-      <c r="B77" s="92" t="s">
+      <c r="B77" s="106" t="s">
         <v>822</v>
       </c>
-      <c r="C77" s="92" t="s">
+      <c r="C77" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D77" s="92" t="s">
+      <c r="D77" s="106" t="s">
         <v>684</v>
       </c>
     </row>
@@ -10993,13 +11053,13 @@
         <f aca="false">'BC First Nations'!A80</f>
         <v>Tzeachten First Nation</v>
       </c>
-      <c r="B78" s="92" t="s">
+      <c r="B78" s="106" t="s">
         <v>833</v>
       </c>
-      <c r="C78" s="92" t="s">
+      <c r="C78" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D78" s="92" t="s">
+      <c r="D78" s="106" t="s">
         <v>48</v>
       </c>
     </row>
@@ -11008,13 +11068,13 @@
         <f aca="false">'BC First Nations'!A81</f>
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
-      <c r="B79" s="92" t="s">
+      <c r="B79" s="106" t="s">
         <v>842</v>
       </c>
-      <c r="C79" s="92" t="s">
+      <c r="C79" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D79" s="92" t="s">
+      <c r="D79" s="106" t="s">
         <v>848</v>
       </c>
     </row>
@@ -11023,13 +11083,13 @@
         <f aca="false">'BC First Nations'!A82</f>
         <v>Union Bar First Nations</v>
       </c>
-      <c r="B80" s="92" t="s">
+      <c r="B80" s="106" t="s">
         <v>852</v>
       </c>
-      <c r="C80" s="92" t="s">
+      <c r="C80" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D80" s="92" t="s">
+      <c r="D80" s="106" t="s">
         <v>858</v>
       </c>
     </row>
@@ -11038,13 +11098,13 @@
         <f aca="false">'BC First Nations'!A83</f>
         <v>Upper Nicola Indian Band</v>
       </c>
-      <c r="B81" s="92" t="s">
+      <c r="B81" s="106" t="s">
         <v>860</v>
       </c>
-      <c r="C81" s="92" t="s">
+      <c r="C81" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D81" s="92" t="s">
+      <c r="D81" s="106" t="s">
         <v>866</v>
       </c>
     </row>
@@ -11053,13 +11113,13 @@
         <f aca="false">'BC First Nations'!A84</f>
         <v>Upper Similkameen Indian Band</v>
       </c>
-      <c r="B82" s="92" t="s">
+      <c r="B82" s="106" t="s">
         <v>869</v>
       </c>
-      <c r="C82" s="92" t="s">
+      <c r="C82" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D82" s="92" t="s">
+      <c r="D82" s="106" t="s">
         <v>873</v>
       </c>
     </row>
@@ -11068,13 +11128,13 @@
         <f aca="false">'BC First Nations'!A85</f>
         <v>Whispering Pines/Clinton Indian Bands</v>
       </c>
-      <c r="B83" s="92" t="s">
+      <c r="B83" s="106" t="s">
         <v>877</v>
       </c>
-      <c r="C83" s="92" t="s">
+      <c r="C83" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D83" s="92" t="s">
+      <c r="D83" s="106" t="s">
         <v>885</v>
       </c>
     </row>
@@ -11083,13 +11143,13 @@
         <f aca="false">'BC First Nations'!A87</f>
         <v>Williams Lake Indian Band</v>
       </c>
-      <c r="B84" s="92" t="s">
+      <c r="B84" s="106" t="s">
         <v>893</v>
       </c>
-      <c r="C84" s="92" t="s">
+      <c r="C84" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D84" s="92" t="s">
+      <c r="D84" s="106" t="s">
         <v>896</v>
       </c>
     </row>
@@ -11098,28 +11158,28 @@
         <f aca="false">'BC First Nations'!A88</f>
         <v>Yakweakwioose First Nation</v>
       </c>
-      <c r="B85" s="92" t="s">
+      <c r="B85" s="106" t="s">
         <v>899</v>
       </c>
-      <c r="C85" s="92" t="s">
+      <c r="C85" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D85" s="92" t="s">
+      <c r="D85" s="106" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="str">
         <f aca="false">'BC First Nations'!A89</f>
-        <v>Yale First Nation </v>
-      </c>
-      <c r="B86" s="92" t="s">
+        <v>Yale First Nation</v>
+      </c>
+      <c r="B86" s="106" t="s">
         <v>975</v>
       </c>
-      <c r="C86" s="92" t="s">
+      <c r="C86" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D86" s="92" t="s">
+      <c r="D86" s="106" t="s">
         <v>916</v>
       </c>
     </row>
@@ -11128,21 +11188,21 @@
         <f aca="false">'BC First Nations'!A90</f>
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
-      <c r="B87" s="92" t="s">
+      <c r="B87" s="106" t="s">
         <v>976</v>
       </c>
-      <c r="C87" s="92" t="s">
+      <c r="C87" s="106" t="s">
         <v>937</v>
       </c>
-      <c r="D87" s="92" t="s">
+      <c r="D87" s="106" t="s">
         <v>924</v>
       </c>
-      <c r="G87" s="92"/>
+      <c r="G87" s="106"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="92"/>
-      <c r="D88" s="92"/>
-      <c r="E88" s="92"/>
+      <c r="C88" s="106"/>
+      <c r="D88" s="106"/>
+      <c r="E88" s="106"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -11250,11 +11310,11 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
improved some more location accuracy and some map styles
</commit_message>
<xml_diff>
--- a/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
+++ b/src/data_management/raw_data/traditional_territory/TMX_IAMC_Indigenous_Community_Profiles.xlsx
@@ -4142,7 +4142,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="116">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4415,108 +4415,132 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -4667,8 +4691,8 @@
   </sheetPr>
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H57" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K62" activeCellId="0" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7109,58 +7133,58 @@
       <c r="A44" s="68" t="s">
         <v>485</v>
       </c>
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="36" t="s">
         <v>486</v>
       </c>
       <c r="C44" s="69" t="s">
         <v>487</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="D44" s="36" t="s">
         <v>488</v>
       </c>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21" t="s">
+      <c r="E44" s="36"/>
+      <c r="F44" s="36" t="s">
         <v>489</v>
       </c>
-      <c r="G44" s="26" t="s">
+      <c r="G44" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="H44" s="70" t="s">
+      <c r="H44" s="71" t="s">
         <v>490</v>
       </c>
-      <c r="I44" s="21" t="s">
+      <c r="I44" s="36" t="s">
         <v>491</v>
       </c>
-      <c r="J44" s="71"/>
-      <c r="K44" s="71"/>
-      <c r="L44" s="26" t="s">
+      <c r="J44" s="38"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="M44" s="21" t="s">
+      <c r="M44" s="36" t="s">
         <v>492</v>
       </c>
-      <c r="N44" s="21"/>
-      <c r="O44" s="72" t="s">
+      <c r="N44" s="36"/>
+      <c r="O44" s="41" t="s">
         <v>443</v>
       </c>
-      <c r="P44" s="28" t="s">
+      <c r="P44" s="39" t="s">
         <v>493</v>
       </c>
       <c r="Q44" s="69" t="s">
         <v>494</v>
       </c>
-      <c r="R44" s="72" t="n">
+      <c r="R44" s="41" t="n">
         <v>49.2360660445914</v>
       </c>
-      <c r="S44" s="72" t="n">
+      <c r="S44" s="41" t="n">
         <v>-122.002526922047</v>
       </c>
-      <c r="T44" s="73"/>
-      <c r="U44" s="73"/>
-      <c r="V44" s="74" t="s">
+      <c r="T44" s="42"/>
+      <c r="U44" s="42"/>
+      <c r="V44" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="W44" s="74" t="s">
+      <c r="W44" s="43" t="s">
         <v>495</v>
       </c>
     </row>
@@ -7203,7 +7227,7 @@
         <v>505</v>
       </c>
       <c r="N45" s="16"/>
-      <c r="O45" s="75" t="s">
+      <c r="O45" s="72" t="s">
         <v>443</v>
       </c>
       <c r="P45" s="13" t="s">
@@ -7211,10 +7235,10 @@
       </c>
       <c r="Q45" s="16"/>
       <c r="R45" s="14" t="n">
-        <v>49.262475</v>
+        <v>49.2554268901582</v>
       </c>
       <c r="S45" s="14" t="n">
-        <v>-121.724003</v>
+        <v>-121.73032797257</v>
       </c>
       <c r="V45" s="8" t="str">
         <f aca="false">A45</f>
@@ -7230,11 +7254,11 @@
         <v>508</v>
       </c>
       <c r="C46" s="20"/>
-      <c r="D46" s="76" t="s">
+      <c r="D46" s="73" t="s">
         <v>509</v>
       </c>
-      <c r="E46" s="76"/>
-      <c r="F46" s="77"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="74"/>
       <c r="G46" s="57" t="s">
         <v>29</v>
       </c>
@@ -7257,10 +7281,10 @@
         <v>178</v>
       </c>
       <c r="N46" s="13"/>
-      <c r="O46" s="78" t="s">
+      <c r="O46" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="P46" s="79" t="s">
+      <c r="P46" s="76" t="s">
         <v>513</v>
       </c>
       <c r="Q46" s="17" t="s">
@@ -7324,10 +7348,10 @@
       </c>
       <c r="Q47" s="16"/>
       <c r="R47" s="14" t="n">
-        <v>49.012447</v>
+        <v>49.014781370754</v>
       </c>
       <c r="S47" s="14" t="n">
-        <v>-122.767315</v>
+        <v>-122.777801460853</v>
       </c>
       <c r="T47" s="14" t="s">
         <v>525</v>
@@ -7339,7 +7363,7 @@
       <c r="W47" s="14"/>
     </row>
     <row r="48" customFormat="false" ht="41.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="80" t="s">
+      <c r="A48" s="77" t="s">
         <v>526</v>
       </c>
       <c r="B48" s="13" t="s">
@@ -7409,7 +7433,7 @@
         <v>537</v>
       </c>
       <c r="E49" s="20"/>
-      <c r="F49" s="77"/>
+      <c r="F49" s="74"/>
       <c r="G49" s="57" t="s">
         <v>538</v>
       </c>
@@ -7422,17 +7446,17 @@
       <c r="J49" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="K49" s="81" t="s">
+      <c r="K49" s="78" t="s">
         <v>542</v>
       </c>
-      <c r="L49" s="82" t="s">
+      <c r="L49" s="79" t="s">
         <v>32</v>
       </c>
       <c r="M49" s="13" t="s">
         <v>178</v>
       </c>
       <c r="N49" s="13"/>
-      <c r="O49" s="75" t="s">
+      <c r="O49" s="72" t="s">
         <v>35</v>
       </c>
       <c r="P49" s="13" t="s">
@@ -7442,12 +7466,12 @@
         <v>544</v>
       </c>
       <c r="R49" s="14" t="n">
-        <v>49.963059</v>
+        <v>50.1106713966103</v>
       </c>
       <c r="S49" s="14" t="n">
-        <v>-121.484624</v>
-      </c>
-      <c r="V49" s="83" t="s">
+        <v>-120.786988056089</v>
+      </c>
+      <c r="V49" s="80" t="s">
         <v>64</v>
       </c>
       <c r="W49" s="8" t="s">
@@ -7455,10 +7479,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="39.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="84" t="s">
+      <c r="A50" s="81" t="s">
         <v>546</v>
       </c>
-      <c r="B50" s="85" t="s">
+      <c r="B50" s="82" t="s">
         <v>547</v>
       </c>
       <c r="C50" s="20" t="s">
@@ -7486,27 +7510,27 @@
       <c r="K50" s="20" t="s">
         <v>554</v>
       </c>
-      <c r="L50" s="86" t="s">
+      <c r="L50" s="83" t="s">
         <v>267</v>
       </c>
       <c r="M50" s="16" t="s">
         <v>555</v>
       </c>
       <c r="N50" s="16"/>
-      <c r="O50" s="75" t="s">
+      <c r="O50" s="72" t="s">
         <v>443</v>
       </c>
-      <c r="P50" s="87" t="s">
+      <c r="P50" s="84" t="s">
         <v>556</v>
       </c>
       <c r="Q50" s="17" t="s">
         <v>557</v>
       </c>
       <c r="R50" s="14" t="n">
-        <v>49.339668</v>
+        <v>49.3432137386584</v>
       </c>
       <c r="S50" s="14" t="n">
-        <v>-121.60638</v>
+        <v>-121.606714685116</v>
       </c>
       <c r="V50" s="8" t="s">
         <v>546</v>
@@ -7516,10 +7540,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="53.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="88" t="s">
+      <c r="A51" s="85" t="s">
         <v>559</v>
       </c>
-      <c r="B51" s="89" t="s">
+      <c r="B51" s="86" t="s">
         <v>560</v>
       </c>
       <c r="C51" s="16" t="s">
@@ -7529,7 +7553,7 @@
         <v>562</v>
       </c>
       <c r="E51" s="20"/>
-      <c r="F51" s="77"/>
+      <c r="F51" s="74"/>
       <c r="G51" s="20" t="s">
         <v>563</v>
       </c>
@@ -7547,17 +7571,17 @@
       <c r="O51" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="P51" s="90" t="s">
+      <c r="P51" s="87" t="s">
         <v>564</v>
       </c>
       <c r="Q51" s="17" t="s">
         <v>565</v>
       </c>
       <c r="R51" s="14" t="n">
-        <v>49.087557</v>
+        <v>49.168967426647</v>
       </c>
       <c r="S51" s="14" t="n">
-        <v>-121.829723</v>
+        <v>-121.988777295383</v>
       </c>
       <c r="V51" s="8" t="s">
         <v>52</v>
@@ -7580,7 +7604,7 @@
         <v>570</v>
       </c>
       <c r="E52" s="20"/>
-      <c r="F52" s="91" t="s">
+      <c r="F52" s="88" t="s">
         <v>569</v>
       </c>
       <c r="G52" s="22" t="s">
@@ -7604,17 +7628,17 @@
       <c r="O52" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="P52" s="78" t="s">
+      <c r="P52" s="75" t="s">
         <v>576</v>
       </c>
       <c r="Q52" s="17" t="s">
         <v>577</v>
       </c>
       <c r="R52" s="14" t="n">
-        <v>52.634393</v>
+        <v>51.3173471888435</v>
       </c>
       <c r="S52" s="14" t="n">
-        <v>-119.699777</v>
+        <v>-120.149109431274</v>
       </c>
       <c r="V52" s="8" t="s">
         <v>578</v>
@@ -7661,10 +7685,10 @@
       </c>
       <c r="Q53" s="16"/>
       <c r="R53" s="14" t="n">
-        <v>50.117565</v>
+        <v>50.1359622911795</v>
       </c>
       <c r="S53" s="14" t="n">
-        <v>-120.838519</v>
+        <v>-121.571694176221</v>
       </c>
       <c r="V53" s="8" t="str">
         <f aca="false">A53</f>
@@ -7712,15 +7736,15 @@
       </c>
       <c r="Q54" s="16"/>
       <c r="R54" s="14" t="n">
-        <v>49.963059</v>
+        <v>50.1895586233887</v>
       </c>
       <c r="S54" s="14" t="n">
-        <v>-121.484624</v>
-      </c>
-      <c r="V54" s="83" t="s">
+        <v>-121.574218038587</v>
+      </c>
+      <c r="V54" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="W54" s="83" t="s">
+      <c r="W54" s="80" t="s">
         <v>593</v>
       </c>
     </row>
@@ -7764,10 +7788,10 @@
         <v>601</v>
       </c>
       <c r="R55" s="14" t="n">
-        <v>49.087557</v>
+        <v>49.1345789702994</v>
       </c>
       <c r="S55" s="14" t="n">
-        <v>-121.829723</v>
+        <v>-121.961353111655</v>
       </c>
       <c r="V55" s="8" t="s">
         <v>52</v>
@@ -7816,10 +7840,10 @@
         <v>610</v>
       </c>
       <c r="R56" s="14" t="n">
-        <v>50.367907</v>
+        <v>50.5179466722097</v>
       </c>
       <c r="S56" s="14" t="n">
-        <v>-116.89554</v>
+        <v>-116.010111899312</v>
       </c>
       <c r="V56" s="8" t="str">
         <f aca="false">A56</f>
@@ -7866,10 +7890,10 @@
         <v>618</v>
       </c>
       <c r="R57" s="14" t="n">
-        <v>49.227586</v>
+        <v>49.3569869309884</v>
       </c>
       <c r="S57" s="14" t="n">
-        <v>-122.174045</v>
+        <v>-121.606004780696</v>
       </c>
       <c r="V57" s="8" t="str">
         <f aca="false">A57</f>
@@ -7880,7 +7904,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="40.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="92" t="s">
+      <c r="A58" s="89" t="s">
         <v>620</v>
       </c>
       <c r="B58" s="13" t="s">
@@ -7916,10 +7940,10 @@
         <v>627</v>
       </c>
       <c r="R58" s="14" t="n">
-        <v>49.175281</v>
+        <v>49.1774272241009</v>
       </c>
       <c r="S58" s="14" t="n">
-        <v>-121.977269</v>
+        <v>-121.972181975181</v>
       </c>
       <c r="V58" s="8" t="str">
         <f aca="false">A58</f>
@@ -7968,7 +7992,7 @@
         <v>636</v>
       </c>
       <c r="N59" s="13"/>
-      <c r="O59" s="93" t="s">
+      <c r="O59" s="90" t="s">
         <v>151</v>
       </c>
       <c r="P59" s="13" t="s">
@@ -7978,10 +8002,10 @@
         <v>638</v>
       </c>
       <c r="R59" s="14" t="n">
-        <v>49.107871</v>
+        <v>49.1518045385059</v>
       </c>
       <c r="S59" s="14" t="n">
-        <v>-124.120584</v>
+        <v>-123.930347230429</v>
       </c>
       <c r="V59" s="8" t="str">
         <f aca="false">A59</f>
@@ -8031,10 +8055,10 @@
         <v>646</v>
       </c>
       <c r="R60" s="14" t="n">
-        <v>49.087557</v>
+        <v>49.0816878510316</v>
       </c>
       <c r="S60" s="14" t="n">
-        <v>-121.829723</v>
+        <v>-121.969208835976</v>
       </c>
       <c r="V60" s="8" t="s">
         <v>52</v>
@@ -8044,7 +8068,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="92" t="s">
+      <c r="A61" s="89" t="s">
         <v>648</v>
       </c>
       <c r="B61" s="13" t="s">
@@ -8083,10 +8107,10 @@
         <v>654</v>
       </c>
       <c r="R61" s="14" t="n">
-        <v>49.963059</v>
+        <v>49.6610890128954</v>
       </c>
       <c r="S61" s="14" t="n">
-        <v>-121.484624</v>
+        <v>-121.411724761085</v>
       </c>
       <c r="V61" s="8" t="s">
         <v>655</v>
@@ -8094,66 +8118,68 @@
       <c r="W61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="42.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="94" t="s">
+      <c r="A62" s="91" t="s">
         <v>656</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="28" t="s">
         <v>657</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="92" t="s">
         <v>658</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="28" t="s">
         <v>659</v>
       </c>
-      <c r="E62" s="13"/>
+      <c r="E62" s="28"/>
       <c r="F62" s="28"/>
-      <c r="G62" s="22" t="s">
+      <c r="G62" s="93" t="s">
         <v>660</v>
       </c>
-      <c r="H62" s="23" t="s">
+      <c r="H62" s="94" t="s">
         <v>661</v>
       </c>
-      <c r="I62" s="22" t="s">
+      <c r="I62" s="93" t="s">
         <v>662</v>
       </c>
-      <c r="J62" s="22" t="s">
+      <c r="J62" s="93" t="s">
         <v>662</v>
       </c>
-      <c r="K62" s="22" t="s">
+      <c r="K62" s="93" t="s">
         <v>662</v>
       </c>
-      <c r="L62" s="25" t="s">
+      <c r="L62" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="M62" s="13" t="s">
+      <c r="M62" s="28" t="s">
         <v>663</v>
       </c>
-      <c r="N62" s="13"/>
-      <c r="O62" s="14" t="s">
+      <c r="N62" s="28"/>
+      <c r="O62" s="96" t="s">
         <v>664</v>
       </c>
-      <c r="P62" s="23" t="s">
+      <c r="P62" s="94" t="s">
         <v>665</v>
       </c>
-      <c r="Q62" s="17" t="s">
+      <c r="Q62" s="97" t="s">
         <v>666</v>
       </c>
-      <c r="R62" s="14" t="n">
-        <v>49.807197</v>
-      </c>
-      <c r="S62" s="14" t="n">
-        <v>-123.200082</v>
-      </c>
-      <c r="V62" s="8" t="s">
+      <c r="R62" s="96" t="n">
+        <v>49.6914766507096</v>
+      </c>
+      <c r="S62" s="96" t="n">
+        <v>-123.1477388186</v>
+      </c>
+      <c r="T62" s="98"/>
+      <c r="U62" s="98"/>
+      <c r="V62" s="99" t="s">
         <v>667</v>
       </c>
-      <c r="W62" s="8" t="s">
+      <c r="W62" s="99" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="94" t="s">
+      <c r="A63" s="100" t="s">
         <v>669</v>
       </c>
       <c r="B63" s="13" t="s">
@@ -8172,7 +8198,7 @@
       <c r="G63" s="20" t="s">
         <v>673</v>
       </c>
-      <c r="H63" s="95"/>
+      <c r="H63" s="101"/>
       <c r="I63" s="55"/>
       <c r="J63" s="55"/>
       <c r="K63" s="55"/>
@@ -8237,14 +8263,14 @@
       <c r="K64" s="22" t="s">
         <v>683</v>
       </c>
-      <c r="L64" s="81" t="s">
+      <c r="L64" s="78" t="s">
         <v>32</v>
       </c>
       <c r="M64" s="16" t="s">
         <v>684</v>
       </c>
       <c r="N64" s="16"/>
-      <c r="O64" s="75" t="s">
+      <c r="O64" s="72" t="s">
         <v>35</v>
       </c>
       <c r="P64" s="13" t="s">
@@ -8369,7 +8395,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="80" t="s">
+      <c r="A67" s="77" t="s">
         <v>707</v>
       </c>
       <c r="B67" s="13" t="s">
@@ -8396,7 +8422,7 @@
         <v>711</v>
       </c>
       <c r="N67" s="16"/>
-      <c r="O67" s="75" t="s">
+      <c r="O67" s="72" t="s">
         <v>35</v>
       </c>
       <c r="P67" s="13" t="s">
@@ -8457,7 +8483,7 @@
         <v>721</v>
       </c>
       <c r="N68" s="16"/>
-      <c r="O68" s="75" t="s">
+      <c r="O68" s="72" t="s">
         <v>35</v>
       </c>
       <c r="P68" s="20" t="s">
@@ -8530,7 +8556,7 @@
       <c r="W69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="92" t="s">
+      <c r="A70" s="89" t="s">
         <v>733</v>
       </c>
       <c r="B70" s="13" t="s">
@@ -8617,7 +8643,7 @@
         <v>178</v>
       </c>
       <c r="N71" s="20"/>
-      <c r="O71" s="75" t="s">
+      <c r="O71" s="72" t="s">
         <v>452</v>
       </c>
       <c r="P71" s="13" t="s">
@@ -8640,7 +8666,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="94" t="s">
+      <c r="A72" s="100" t="s">
         <v>747</v>
       </c>
       <c r="B72" s="13" t="s">
@@ -8671,12 +8697,12 @@
       <c r="K72" s="22" t="s">
         <v>752</v>
       </c>
-      <c r="L72" s="96"/>
-      <c r="M72" s="75" t="s">
+      <c r="L72" s="102"/>
+      <c r="M72" s="72" t="s">
         <v>178</v>
       </c>
-      <c r="N72" s="75"/>
-      <c r="O72" s="75" t="s">
+      <c r="N72" s="72"/>
+      <c r="O72" s="72" t="s">
         <v>753</v>
       </c>
       <c r="P72" s="13" t="s">
@@ -8715,7 +8741,7 @@
       <c r="F73" s="28" t="s">
         <v>761</v>
       </c>
-      <c r="G73" s="85" t="s">
+      <c r="G73" s="82" t="s">
         <v>762</v>
       </c>
       <c r="H73" s="13" t="s">
@@ -8735,7 +8761,7 @@
         <v>178</v>
       </c>
       <c r="N73" s="13"/>
-      <c r="O73" s="75" t="s">
+      <c r="O73" s="72" t="s">
         <v>766</v>
       </c>
       <c r="P73" s="13" t="s">
@@ -8775,10 +8801,10 @@
         <v>774</v>
       </c>
       <c r="E74" s="13"/>
-      <c r="F74" s="97" t="s">
+      <c r="F74" s="103" t="s">
         <v>775</v>
       </c>
-      <c r="G74" s="89" t="s">
+      <c r="G74" s="86" t="s">
         <v>776</v>
       </c>
       <c r="H74" s="23" t="s">
@@ -8840,7 +8866,7 @@
         <v>178</v>
       </c>
       <c r="N75" s="13"/>
-      <c r="O75" s="75" t="s">
+      <c r="O75" s="72" t="s">
         <v>753</v>
       </c>
       <c r="P75" s="13" t="s">
@@ -8863,7 +8889,7 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="92" t="s">
+      <c r="A76" s="89" t="s">
         <v>789</v>
       </c>
       <c r="B76" s="13" t="s">
@@ -8888,7 +8914,7 @@
         <v>793</v>
       </c>
       <c r="N76" s="16"/>
-      <c r="O76" s="75" t="s">
+      <c r="O76" s="72" t="s">
         <v>35</v>
       </c>
       <c r="P76" s="13" t="s">
@@ -8947,7 +8973,7 @@
         <v>804</v>
       </c>
       <c r="N77" s="13"/>
-      <c r="O77" s="75" t="s">
+      <c r="O77" s="72" t="s">
         <v>805</v>
       </c>
       <c r="P77" s="13" t="s">
@@ -9010,7 +9036,7 @@
         <v>818</v>
       </c>
       <c r="N78" s="16"/>
-      <c r="O78" s="75" t="s">
+      <c r="O78" s="72" t="s">
         <v>753</v>
       </c>
       <c r="P78" s="13" t="s">
@@ -9043,11 +9069,11 @@
       <c r="C79" s="13" t="s">
         <v>824</v>
       </c>
-      <c r="D79" s="98" t="s">
+      <c r="D79" s="104" t="s">
         <v>825</v>
       </c>
-      <c r="E79" s="98"/>
-      <c r="F79" s="99" t="s">
+      <c r="E79" s="104"/>
+      <c r="F79" s="105" t="s">
         <v>826</v>
       </c>
       <c r="G79" s="57" t="s">
@@ -9068,7 +9094,7 @@
         <v>684</v>
       </c>
       <c r="N79" s="16"/>
-      <c r="O79" s="75" t="s">
+      <c r="O79" s="72" t="s">
         <v>35</v>
       </c>
       <c r="P79" s="13" t="s">
@@ -9145,7 +9171,7 @@
       <c r="B81" s="13" t="s">
         <v>843</v>
       </c>
-      <c r="C81" s="100" t="s">
+      <c r="C81" s="106" t="s">
         <v>844</v>
       </c>
       <c r="D81" s="13" t="s">
@@ -9168,7 +9194,7 @@
         <v>848</v>
       </c>
       <c r="N81" s="16"/>
-      <c r="O81" s="75" t="s">
+      <c r="O81" s="72" t="s">
         <v>295</v>
       </c>
       <c r="P81" s="13" t="s">
@@ -9218,7 +9244,7 @@
         <v>858</v>
       </c>
       <c r="N82" s="16"/>
-      <c r="O82" s="75"/>
+      <c r="O82" s="72"/>
       <c r="P82" s="13"/>
       <c r="Q82" s="16"/>
       <c r="R82" s="14" t="n">
@@ -9283,7 +9309,7 @@
       <c r="W83" s="8"/>
     </row>
     <row r="84" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="92" t="s">
+      <c r="A84" s="89" t="s">
         <v>869</v>
       </c>
       <c r="B84" s="13" t="s">
@@ -9296,7 +9322,7 @@
         <v>872</v>
       </c>
       <c r="E84" s="13"/>
-      <c r="F84" s="69" t="s">
+      <c r="F84" s="92" t="s">
         <v>871</v>
       </c>
       <c r="G84" s="57" t="s">
@@ -9447,7 +9473,7 @@
         <v>896</v>
       </c>
       <c r="N87" s="16"/>
-      <c r="O87" s="101"/>
+      <c r="O87" s="107"/>
       <c r="P87" s="13" t="s">
         <v>897</v>
       </c>
@@ -9623,23 +9649,23 @@
       <c r="W90" s="8"/>
     </row>
     <row r="91" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="102"/>
-      <c r="B91" s="103"/>
-      <c r="C91" s="103"/>
-      <c r="D91" s="104"/>
-      <c r="E91" s="104"/>
-      <c r="F91" s="104"/>
-      <c r="G91" s="104"/>
-      <c r="H91" s="104"/>
-      <c r="I91" s="104"/>
-      <c r="J91" s="104"/>
-      <c r="K91" s="104"/>
-      <c r="L91" s="104"/>
-      <c r="M91" s="104"/>
-      <c r="N91" s="104"/>
-      <c r="O91" s="104"/>
-      <c r="P91" s="103"/>
-      <c r="Q91" s="105"/>
+      <c r="A91" s="108"/>
+      <c r="B91" s="109"/>
+      <c r="C91" s="109"/>
+      <c r="D91" s="110"/>
+      <c r="E91" s="110"/>
+      <c r="F91" s="110"/>
+      <c r="G91" s="110"/>
+      <c r="H91" s="110"/>
+      <c r="I91" s="110"/>
+      <c r="J91" s="110"/>
+      <c r="K91" s="110"/>
+      <c r="L91" s="110"/>
+      <c r="M91" s="110"/>
+      <c r="N91" s="110"/>
+      <c r="O91" s="110"/>
+      <c r="P91" s="109"/>
+      <c r="Q91" s="111"/>
     </row>
     <row r="92" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="30" t="s">
@@ -9898,13 +9924,13 @@
       <c r="A1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="112" t="s">
         <v>931</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="112" t="s">
         <v>932</v>
       </c>
-      <c r="D1" s="107" t="s">
+      <c r="D1" s="113" t="s">
         <v>933</v>
       </c>
     </row>
@@ -9913,13 +9939,13 @@
         <f aca="false">'BC First Nations'!A3</f>
         <v>Adams Lake Indian Band (belongs to the Secwepemc Nation, member of the Shuswap Nation Triabal Council)</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="112" t="s">
         <v>934</v>
       </c>
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D2" s="108" t="s">
+      <c r="D2" s="114" t="s">
         <v>936</v>
       </c>
     </row>
@@ -9928,13 +9954,13 @@
         <f aca="false">'BC First Nations'!A4</f>
         <v>Aitchelitz Band</v>
       </c>
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="112" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="106" t="s">
+      <c r="C3" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D3" s="106" t="s">
+      <c r="D3" s="112" t="s">
         <v>48</v>
       </c>
     </row>
@@ -9943,13 +9969,13 @@
         <f aca="false">'BC First Nations'!A5</f>
         <v>Ashcroft Indian Band</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="112" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="112" t="s">
         <v>60</v>
       </c>
     </row>
@@ -9958,13 +9984,13 @@
         <f aca="false">'BC First Nations'!A6</f>
         <v>Boothroyd Band</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="C5" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D5" s="109" t="s">
+      <c r="D5" s="115" t="s">
         <v>938</v>
       </c>
     </row>
@@ -9973,13 +9999,13 @@
         <f aca="false">'BC First Nations'!A7</f>
         <v>Boston Bar First Nations</v>
       </c>
-      <c r="B6" s="106" t="s">
+      <c r="B6" s="112" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="106" t="s">
+      <c r="C6" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D6" s="106" t="s">
+      <c r="D6" s="112" t="s">
         <v>77</v>
       </c>
     </row>
@@ -9988,13 +10014,13 @@
         <f aca="false">'BC First Nations'!A8</f>
         <v>Canim Lake Band (The People of Broken Rock "The Tsq'escenemc")</v>
       </c>
-      <c r="B7" s="106" t="s">
+      <c r="B7" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="107" t="s">
+      <c r="C7" s="113" t="s">
         <v>937</v>
       </c>
-      <c r="D7" s="106" t="s">
+      <c r="D7" s="112" t="s">
         <v>939</v>
       </c>
     </row>
@@ -10003,13 +10029,13 @@
         <f aca="false">'BC First Nations'!A9</f>
         <v>Chawathil First Nation</v>
       </c>
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="112" t="s">
         <v>93</v>
       </c>
-      <c r="C8" s="106" t="s">
+      <c r="C8" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D8" s="106" t="s">
+      <c r="D8" s="112" t="s">
         <v>102</v>
       </c>
     </row>
@@ -10018,13 +10044,13 @@
         <f aca="false">'BC First Nations'!A10</f>
         <v>Chi:yo:m Agassiz (Cheam) First Nation - meaning "Wild Strawberry Place"</v>
       </c>
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="112" t="s">
         <v>940</v>
       </c>
-      <c r="C9" s="106" t="s">
+      <c r="C9" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D9" s="106" t="s">
+      <c r="D9" s="112" t="s">
         <v>115</v>
       </c>
     </row>
@@ -10033,13 +10059,13 @@
         <f aca="false">'BC First Nations'!A11</f>
         <v>Coldwater First Nation (Nc/etko - the people of the creeks)</v>
       </c>
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="112" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D10" s="106" t="s">
+      <c r="D10" s="112" t="s">
         <v>941</v>
       </c>
     </row>
@@ -10048,13 +10074,13 @@
         <f aca="false">'BC First Nations'!A12</f>
         <v>Cook's Ferry Indian Band Kumcheen (Variation Nkumcheen); Includes Pokheistk (Variation Pakeist, Pokheistsk), Pemynoos (Variation Piminos), Spatsum (Variation Spaptsin), Spence'S Bridge</v>
       </c>
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="112" t="s">
         <v>942</v>
       </c>
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D11" s="106" t="s">
+      <c r="D11" s="112" t="s">
         <v>943</v>
       </c>
     </row>
@@ -10063,13 +10089,13 @@
         <f aca="false">'BC First Nations'!A13</f>
         <v>Cowichan Tribes</v>
       </c>
-      <c r="B12" s="106" t="s">
+      <c r="B12" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="106" t="s">
+      <c r="C12" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D12" s="106" t="s">
+      <c r="D12" s="112" t="s">
         <v>150</v>
       </c>
     </row>
@@ -10078,13 +10104,13 @@
         <f aca="false">'BC First Nations'!A14</f>
         <v>Ditidaht First Nation Formerly Nitinaht (Pre-1984) (Variation Nitinat)</v>
       </c>
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="C13" s="106" t="s">
+      <c r="C13" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D13" s="106" t="s">
+      <c r="D13" s="112" t="s">
         <v>944</v>
       </c>
     </row>
@@ -10093,13 +10119,13 @@
         <f aca="false">'BC First Nations'!A15</f>
         <v>Esquimalt Nation (Xwsepsum or Kosapsum)</v>
       </c>
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="112" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="106" t="s">
+      <c r="C14" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D14" s="109" t="s">
+      <c r="D14" s="115" t="s">
         <v>945</v>
       </c>
     </row>
@@ -10108,13 +10134,13 @@
         <f aca="false">'BC First Nations'!A16</f>
         <v>Halalt First Nation</v>
       </c>
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="112" t="s">
         <v>946</v>
       </c>
-      <c r="C15" s="106" t="s">
+      <c r="C15" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D15" s="106" t="s">
+      <c r="D15" s="112" t="s">
         <v>947</v>
       </c>
     </row>
@@ -10123,13 +10149,13 @@
         <f aca="false">'BC First Nations'!A17</f>
         <v>Heiltsuk First Nation</v>
       </c>
-      <c r="B16" s="106" t="s">
+      <c r="B16" s="112" t="s">
         <v>192</v>
       </c>
-      <c r="C16" s="106" t="s">
+      <c r="C16" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D16" s="106" t="s">
+      <c r="D16" s="112" t="s">
         <v>197</v>
       </c>
     </row>
@@ -10138,13 +10164,13 @@
         <f aca="false">'BC First Nations'!A18</f>
         <v>Huu-ay-aht First Nation</v>
       </c>
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="112" t="s">
         <v>948</v>
       </c>
-      <c r="C17" s="106" t="s">
+      <c r="C17" s="112" t="s">
         <v>949</v>
       </c>
-      <c r="D17" s="106" t="s">
+      <c r="D17" s="112" t="s">
         <v>950</v>
       </c>
     </row>
@@ -10153,13 +10179,13 @@
         <f aca="false">'BC First Nations'!A19</f>
         <v>Katzie First Nation</v>
       </c>
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="112" t="s">
         <v>212</v>
       </c>
-      <c r="C18" s="106" t="s">
+      <c r="C18" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D18" s="106" t="s">
+      <c r="D18" s="112" t="s">
         <v>951</v>
       </c>
     </row>
@@ -10168,13 +10194,13 @@
         <f aca="false">'BC First Nations'!A20</f>
         <v>Kwantlen First Nation (tireless Runner)</v>
       </c>
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="112" t="s">
         <v>237</v>
       </c>
-      <c r="C19" s="106" t="s">
+      <c r="C19" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D19" s="106" t="s">
+      <c r="D19" s="112" t="s">
         <v>952</v>
       </c>
     </row>
@@ -10183,13 +10209,13 @@
         <f aca="false">'BC First Nations'!A21</f>
         <v>Kwaw -Kwaw-Aplit First Nations</v>
       </c>
-      <c r="B20" s="106" t="s">
+      <c r="B20" s="112" t="s">
         <v>246</v>
       </c>
-      <c r="C20" s="106" t="s">
+      <c r="C20" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D20" s="106" t="s">
+      <c r="D20" s="112" t="s">
         <v>953</v>
       </c>
     </row>
@@ -10198,13 +10224,13 @@
         <f aca="false">'BC First Nations'!A22</f>
         <v>Kwikwetlem First Nation</v>
       </c>
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="112" t="s">
         <v>248</v>
       </c>
-      <c r="C21" s="106" t="s">
+      <c r="C21" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D21" s="106" t="s">
+      <c r="D21" s="112" t="s">
         <v>254</v>
       </c>
     </row>
@@ -10213,13 +10239,13 @@
         <f aca="false">'BC First Nations'!A23</f>
         <v>Leq' a: mel First Nation</v>
       </c>
-      <c r="B22" s="106" t="s">
+      <c r="B22" s="112" t="s">
         <v>260</v>
       </c>
-      <c r="C22" s="106" t="s">
+      <c r="C22" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D22" s="106" t="s">
+      <c r="D22" s="112" t="s">
         <v>268</v>
       </c>
     </row>
@@ -10228,13 +10254,13 @@
         <f aca="false">'BC First Nations'!A24</f>
         <v>Little Shuswap Lake Indian Band (Skwlax meaning "Black Bear")</v>
       </c>
-      <c r="B23" s="106" t="s">
+      <c r="B23" s="112" t="s">
         <v>284</v>
       </c>
-      <c r="C23" s="106" t="s">
+      <c r="C23" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D23" s="106" t="s">
+      <c r="D23" s="112" t="s">
         <v>281</v>
       </c>
     </row>
@@ -10243,13 +10269,13 @@
         <f aca="false">'BC First Nations'!A25</f>
         <v>Lheidli T'enneh First Nation</v>
       </c>
-      <c r="B24" s="106" t="s">
+      <c r="B24" s="112" t="s">
         <v>285</v>
       </c>
-      <c r="C24" s="106" t="s">
+      <c r="C24" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D24" s="106" t="s">
+      <c r="D24" s="112" t="s">
         <v>294</v>
       </c>
     </row>
@@ -10258,13 +10284,13 @@
         <f aca="false">'BC First Nations'!A26</f>
         <v>Lhtako Dene Nation</v>
       </c>
-      <c r="B25" s="106" t="s">
+      <c r="B25" s="112" t="s">
         <v>300</v>
       </c>
-      <c r="C25" s="106" t="s">
+      <c r="C25" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D25" s="106" t="s">
+      <c r="D25" s="112" t="s">
         <v>308</v>
       </c>
     </row>
@@ -10273,13 +10299,13 @@
         <f aca="false">'BC First Nations'!A27</f>
         <v>Lower Nicola Indian Band -</v>
       </c>
-      <c r="B26" s="106" t="s">
+      <c r="B26" s="112" t="s">
         <v>322</v>
       </c>
-      <c r="C26" s="106" t="s">
+      <c r="C26" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D26" s="106" t="s">
+      <c r="D26" s="112" t="s">
         <v>319</v>
       </c>
     </row>
@@ -10288,13 +10314,13 @@
         <f aca="false">'BC First Nations'!A28</f>
         <v>Lower Similkameen #598</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="112" t="s">
         <v>323</v>
       </c>
-      <c r="C27" s="106" t="s">
+      <c r="C27" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D27" s="106" t="s">
+      <c r="D27" s="112" t="s">
         <v>329</v>
       </c>
     </row>
@@ -10303,13 +10329,13 @@
         <f aca="false">'BC First Nations'!A29</f>
         <v>Lyackson First Nation</v>
       </c>
-      <c r="B28" s="106" t="s">
+      <c r="B28" s="112" t="s">
         <v>333</v>
       </c>
-      <c r="C28" s="106" t="s">
+      <c r="C28" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D28" s="106" t="s">
+      <c r="D28" s="112" t="s">
         <v>341</v>
       </c>
     </row>
@@ -10318,13 +10344,13 @@
         <f aca="false">'BC First Nations'!A30</f>
         <v>Malahat First Nation</v>
       </c>
-      <c r="B29" s="106" t="s">
+      <c r="B29" s="112" t="s">
         <v>345</v>
       </c>
-      <c r="C29" s="106" t="s">
+      <c r="C29" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D29" s="106" t="s">
+      <c r="D29" s="112" t="s">
         <v>351</v>
       </c>
     </row>
@@ -10333,13 +10359,13 @@
         <f aca="false">'BC First Nations'!A31</f>
         <v>Matsqui First Nation</v>
       </c>
-      <c r="B30" s="106" t="s">
+      <c r="B30" s="112" t="s">
         <v>356</v>
       </c>
-      <c r="C30" s="106" t="s">
+      <c r="C30" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D30" s="106" t="s">
+      <c r="D30" s="112" t="s">
         <v>362</v>
       </c>
     </row>
@@ -10348,13 +10374,13 @@
         <f aca="false">'BC First Nations'!A32</f>
         <v>Musqeam Indian Band</v>
       </c>
-      <c r="B31" s="106" t="s">
+      <c r="B31" s="112" t="s">
         <v>365</v>
       </c>
-      <c r="C31" s="106" t="s">
+      <c r="C31" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D31" s="109" t="s">
+      <c r="D31" s="115" t="s">
         <v>954</v>
       </c>
     </row>
@@ -10363,13 +10389,13 @@
         <f aca="false">'BC First Nations'!A33</f>
         <v>Neskonlith Indian Band</v>
       </c>
-      <c r="B32" s="106" t="s">
+      <c r="B32" s="112" t="s">
         <v>378</v>
       </c>
-      <c r="C32" s="106" t="s">
+      <c r="C32" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D32" s="106" t="s">
+      <c r="D32" s="112" t="s">
         <v>384</v>
       </c>
     </row>
@@ -10378,13 +10404,13 @@
         <f aca="false">'BC First Nations'!A34</f>
         <v>Nooaitch Indian Band</v>
       </c>
-      <c r="B33" s="106" t="s">
+      <c r="B33" s="112" t="s">
         <v>388</v>
       </c>
-      <c r="C33" s="106" t="s">
+      <c r="C33" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D33" s="106" t="s">
+      <c r="D33" s="112" t="s">
         <v>396</v>
       </c>
     </row>
@@ -10393,13 +10419,13 @@
         <f aca="false">'BC First Nations'!A35</f>
         <v>Osoyoos</v>
       </c>
-      <c r="B34" s="106" t="s">
+      <c r="B34" s="112" t="s">
         <v>401</v>
       </c>
-      <c r="C34" s="106" t="s">
+      <c r="C34" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D34" s="106" t="s">
+      <c r="D34" s="112" t="s">
         <v>406</v>
       </c>
     </row>
@@ -10408,13 +10434,13 @@
         <f aca="false">'BC First Nations'!A36</f>
         <v>Pacheedaht First Nation</v>
       </c>
-      <c r="B35" s="106" t="s">
+      <c r="B35" s="112" t="s">
         <v>410</v>
       </c>
-      <c r="C35" s="106" t="s">
+      <c r="C35" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D35" s="106" t="s">
+      <c r="D35" s="112" t="s">
         <v>416</v>
       </c>
     </row>
@@ -10423,13 +10449,13 @@
         <f aca="false">'BC First Nations'!A37</f>
         <v>Pauquachin Nation</v>
       </c>
-      <c r="B36" s="106" t="s">
+      <c r="B36" s="112" t="s">
         <v>421</v>
       </c>
-      <c r="C36" s="106" t="s">
+      <c r="C36" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D36" s="109" t="s">
+      <c r="D36" s="115" t="s">
         <v>955</v>
       </c>
     </row>
@@ -10438,13 +10464,13 @@
         <f aca="false">'BC First Nations'!A38</f>
         <v>Penticton Indian Band</v>
       </c>
-      <c r="B37" s="106" t="s">
+      <c r="B37" s="112" t="s">
         <v>429</v>
       </c>
-      <c r="C37" s="106" t="s">
+      <c r="C37" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D37" s="106" t="s">
+      <c r="D37" s="112" t="s">
         <v>434</v>
       </c>
     </row>
@@ -10453,13 +10479,13 @@
         <f aca="false">'BC First Nations'!A39</f>
         <v>Peters Band (Peters First Nation)</v>
       </c>
-      <c r="B38" s="106" t="s">
+      <c r="B38" s="112" t="s">
         <v>437</v>
       </c>
-      <c r="C38" s="106" t="s">
+      <c r="C38" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D38" s="106" t="s">
+      <c r="D38" s="112" t="s">
         <v>442</v>
       </c>
     </row>
@@ -10468,13 +10494,13 @@
         <f aca="false">'BC First Nations'!A40</f>
         <v>Penelakut Tribe</v>
       </c>
-      <c r="B39" s="106" t="s">
+      <c r="B39" s="112" t="s">
         <v>447</v>
       </c>
-      <c r="C39" s="106" t="s">
+      <c r="C39" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D39" s="106" t="s">
+      <c r="D39" s="112" t="s">
         <v>451</v>
       </c>
     </row>
@@ -10483,13 +10509,13 @@
         <f aca="false">'BC First Nations'!A41</f>
         <v>Popkum First Nation</v>
       </c>
-      <c r="B40" s="106" t="s">
+      <c r="B40" s="112" t="s">
         <v>456</v>
       </c>
-      <c r="C40" s="106" t="s">
+      <c r="C40" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D40" s="106" t="s">
+      <c r="D40" s="112" t="s">
         <v>463</v>
       </c>
     </row>
@@ -10498,13 +10524,13 @@
         <f aca="false">'BC First Nations'!A42</f>
         <v>Qayqayt First Nation (New Westminister)</v>
       </c>
-      <c r="B41" s="106" t="s">
+      <c r="B41" s="112" t="s">
         <v>956</v>
       </c>
-      <c r="C41" s="106" t="s">
+      <c r="C41" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D41" s="109" t="s">
+      <c r="D41" s="115" t="s">
         <v>957</v>
       </c>
     </row>
@@ -10513,13 +10539,13 @@
         <f aca="false">'BC First Nations'!A43</f>
         <v>Scia'new First Nation (Beecher Bay First Nation)</v>
       </c>
-      <c r="B42" s="106" t="s">
+      <c r="B42" s="112" t="s">
         <v>475</v>
       </c>
-      <c r="C42" s="106" t="s">
+      <c r="C42" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D42" s="106" t="s">
+      <c r="D42" s="112" t="s">
         <v>481</v>
       </c>
     </row>
@@ -10528,13 +10554,13 @@
         <f aca="false">'BC First Nations'!A44</f>
         <v>Sq'ewlets (Scowlitz) First Nation</v>
       </c>
-      <c r="B43" s="106" t="s">
+      <c r="B43" s="112" t="s">
         <v>485</v>
       </c>
-      <c r="C43" s="106" t="s">
+      <c r="C43" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D43" s="106" t="s">
+      <c r="D43" s="112" t="s">
         <v>958</v>
       </c>
     </row>
@@ -10543,13 +10569,13 @@
         <f aca="false">'BC First Nations'!A45</f>
         <v>Seabird Island Band</v>
       </c>
-      <c r="B44" s="106" t="s">
+      <c r="B44" s="112" t="s">
         <v>496</v>
       </c>
-      <c r="C44" s="106" t="s">
+      <c r="C44" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D44" s="106" t="s">
+      <c r="D44" s="112" t="s">
         <v>505</v>
       </c>
     </row>
@@ -10558,13 +10584,13 @@
         <f aca="false">'BC First Nations'!A46</f>
         <v>Secwepmc (suh-Meh-much) of the Secwepmc Nation</v>
       </c>
-      <c r="B45" s="106" t="s">
+      <c r="B45" s="112" t="s">
         <v>507</v>
       </c>
-      <c r="C45" s="106" t="s">
+      <c r="C45" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D45" s="109" t="s">
+      <c r="D45" s="115" t="s">
         <v>959</v>
       </c>
     </row>
@@ -10573,13 +10599,13 @@
         <f aca="false">'BC First Nations'!A47</f>
         <v>Semiahmoo First Nation</v>
       </c>
-      <c r="B46" s="106" t="s">
+      <c r="B46" s="112" t="s">
         <v>516</v>
       </c>
-      <c r="C46" s="106" t="s">
+      <c r="C46" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D46" s="109" t="s">
+      <c r="D46" s="115" t="s">
         <v>960</v>
       </c>
     </row>
@@ -10588,13 +10614,13 @@
         <f aca="false">'BC First Nations'!A49</f>
         <v>Shackan Indian Band</v>
       </c>
-      <c r="B47" s="106" t="s">
+      <c r="B47" s="112" t="s">
         <v>961</v>
       </c>
-      <c r="C47" s="106" t="s">
+      <c r="C47" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D47" s="109" t="s">
+      <c r="D47" s="115" t="s">
         <v>962</v>
       </c>
     </row>
@@ -10603,13 +10629,13 @@
         <f aca="false">'BC First Nations'!A50</f>
         <v>Shxw'owhamel First Nation</v>
       </c>
-      <c r="B48" s="106" t="s">
+      <c r="B48" s="112" t="s">
         <v>546</v>
       </c>
-      <c r="C48" s="106" t="s">
+      <c r="C48" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D48" s="106" t="s">
+      <c r="D48" s="112" t="s">
         <v>555</v>
       </c>
     </row>
@@ -10618,13 +10644,13 @@
         <f aca="false">'BC First Nations'!A51</f>
         <v>Shxwha:y Villiage</v>
       </c>
-      <c r="B49" s="106" t="s">
+      <c r="B49" s="112" t="s">
         <v>559</v>
       </c>
-      <c r="C49" s="106" t="s">
+      <c r="C49" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D49" s="106" t="s">
+      <c r="D49" s="112" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10633,13 +10659,13 @@
         <f aca="false">'BC First Nations'!A52</f>
         <v>Simpcw First Nation "People of the Rivers"</v>
       </c>
-      <c r="B50" s="106" t="s">
+      <c r="B50" s="112" t="s">
         <v>578</v>
       </c>
-      <c r="C50" s="106" t="s">
+      <c r="C50" s="112" t="s">
         <v>949</v>
       </c>
-      <c r="D50" s="106" t="s">
+      <c r="D50" s="112" t="s">
         <v>963</v>
       </c>
     </row>
@@ -10648,13 +10674,13 @@
         <f aca="false">'BC First Nations'!A53</f>
         <v>Siska Indian Band</v>
       </c>
-      <c r="B51" s="106" t="s">
+      <c r="B51" s="112" t="s">
         <v>580</v>
       </c>
-      <c r="C51" s="106" t="s">
+      <c r="C51" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D51" s="106" t="s">
+      <c r="D51" s="112" t="s">
         <v>585</v>
       </c>
     </row>
@@ -10663,13 +10689,13 @@
         <f aca="false">'BC First Nations'!A54</f>
         <v>Skuppah Indian Band</v>
       </c>
-      <c r="B52" s="106" t="s">
+      <c r="B52" s="112" t="s">
         <v>964</v>
       </c>
-      <c r="C52" s="106" t="s">
+      <c r="C52" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D52" s="109" t="s">
+      <c r="D52" s="115" t="s">
         <v>938</v>
       </c>
     </row>
@@ -10678,13 +10704,13 @@
         <f aca="false">'BC First Nations'!A55</f>
         <v>Skowkale First Nation</v>
       </c>
-      <c r="B53" s="106" t="s">
+      <c r="B53" s="112" t="s">
         <v>594</v>
       </c>
-      <c r="C53" s="106" t="s">
+      <c r="C53" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D53" s="106" t="s">
+      <c r="D53" s="112" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10693,13 +10719,13 @@
         <f aca="false">'BC First Nations'!A56</f>
         <v>Shuswap Indian Band</v>
       </c>
-      <c r="B54" s="106" t="s">
+      <c r="B54" s="112" t="s">
         <v>965</v>
       </c>
-      <c r="C54" s="106" t="s">
+      <c r="C54" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D54" s="106" t="s">
+      <c r="D54" s="112" t="s">
         <v>966</v>
       </c>
     </row>
@@ -10708,13 +10734,13 @@
         <f aca="false">'BC First Nations'!A57</f>
         <v>Skawahlook First Nation</v>
       </c>
-      <c r="B55" s="106" t="s">
+      <c r="B55" s="112" t="s">
         <v>612</v>
       </c>
-      <c r="C55" s="106" t="s">
+      <c r="C55" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D55" s="106" t="s">
+      <c r="D55" s="112" t="s">
         <v>967</v>
       </c>
     </row>
@@ -10723,13 +10749,13 @@
         <f aca="false">'BC First Nations'!A58</f>
         <v>Skwah First Nation</v>
       </c>
-      <c r="B56" s="106" t="s">
+      <c r="B56" s="112" t="s">
         <v>620</v>
       </c>
-      <c r="C56" s="106" t="s">
+      <c r="C56" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D56" s="106" t="s">
+      <c r="D56" s="112" t="s">
         <v>625</v>
       </c>
     </row>
@@ -10738,13 +10764,13 @@
         <f aca="false">'BC First Nations'!A59</f>
         <v>Snuneymuxw First Nation</v>
       </c>
-      <c r="B57" s="106" t="s">
+      <c r="B57" s="112" t="s">
         <v>629</v>
       </c>
-      <c r="C57" s="106" t="s">
+      <c r="C57" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D57" s="106" t="s">
+      <c r="D57" s="112" t="s">
         <v>968</v>
       </c>
     </row>
@@ -10753,13 +10779,13 @@
         <f aca="false">'BC First Nations'!A60</f>
         <v>Soowahlie First Nation</v>
       </c>
-      <c r="B58" s="106" t="s">
+      <c r="B58" s="112" t="s">
         <v>640</v>
       </c>
-      <c r="C58" s="106" t="s">
+      <c r="C58" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D58" s="106" t="s">
+      <c r="D58" s="112" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10768,13 +10794,13 @@
         <f aca="false">'BC First Nations'!A61</f>
         <v>Spuzzum First Nation</v>
       </c>
-      <c r="B59" s="106" t="s">
+      <c r="B59" s="112" t="s">
         <v>648</v>
       </c>
-      <c r="C59" s="106" t="s">
+      <c r="C59" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D59" s="109" t="s">
+      <c r="D59" s="115" t="s">
         <v>938</v>
       </c>
     </row>
@@ -10783,13 +10809,13 @@
         <f aca="false">'BC First Nations'!A62</f>
         <v>Squamish First Nation (Squ-Ho-0-meesh)</v>
       </c>
-      <c r="B60" s="106" t="s">
+      <c r="B60" s="112" t="s">
         <v>667</v>
       </c>
-      <c r="C60" s="106" t="s">
+      <c r="C60" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D60" s="106" t="s">
+      <c r="D60" s="112" t="s">
         <v>969</v>
       </c>
     </row>
@@ -10798,13 +10824,13 @@
         <f aca="false">'BC First Nations'!A63</f>
         <v>Squiala First Nation</v>
       </c>
-      <c r="B61" s="106" t="s">
+      <c r="B61" s="112" t="s">
         <v>669</v>
       </c>
-      <c r="C61" s="106" t="s">
+      <c r="C61" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D61" s="106" t="s">
+      <c r="D61" s="112" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10813,13 +10839,13 @@
         <f aca="false">'BC First Nations'!A64</f>
         <v>Stk'emlupsemc Te Secwepemc</v>
       </c>
-      <c r="B62" s="106" t="s">
+      <c r="B62" s="112" t="s">
         <v>970</v>
       </c>
-      <c r="C62" s="106" t="s">
+      <c r="C62" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D62" s="106" t="s">
+      <c r="D62" s="112" t="s">
         <v>684</v>
       </c>
     </row>
@@ -10828,13 +10854,13 @@
         <f aca="false">'BC First Nations'!A65</f>
         <v>Sts'ailes Band (Chehalls Indian Band)</v>
       </c>
-      <c r="B63" s="106" t="s">
+      <c r="B63" s="112" t="s">
         <v>695</v>
       </c>
-      <c r="C63" s="106" t="s">
+      <c r="C63" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D63" s="106" t="s">
+      <c r="D63" s="112" t="s">
         <v>692</v>
       </c>
     </row>
@@ -10843,13 +10869,13 @@
         <f aca="false">'BC First Nations'!A66</f>
         <v>Sts'wecem'cXgat'tem (Canoe Creek/Dog Creek)</v>
       </c>
-      <c r="B64" s="106" t="s">
+      <c r="B64" s="112" t="s">
         <v>697</v>
       </c>
-      <c r="C64" s="106" t="s">
+      <c r="C64" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D64" s="106" t="s">
+      <c r="D64" s="112" t="s">
         <v>702</v>
       </c>
     </row>
@@ -10858,13 +10884,13 @@
         <f aca="false">'BC First Nations'!A67</f>
         <v>St'uxwtews (Bonaparte Indian Band)</v>
       </c>
-      <c r="B65" s="106" t="s">
+      <c r="B65" s="112" t="s">
         <v>707</v>
       </c>
-      <c r="C65" s="106" t="s">
+      <c r="C65" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D65" s="106" t="s">
+      <c r="D65" s="112" t="s">
         <v>711</v>
       </c>
     </row>
@@ -10873,13 +10899,13 @@
         <f aca="false">'BC First Nations'!A68</f>
         <v>Stz'uminus First Nation (ltst uw' hw-nuts'-ul-wun) Chemainus</v>
       </c>
-      <c r="B66" s="106" t="s">
+      <c r="B66" s="112" t="s">
         <v>724</v>
       </c>
-      <c r="C66" s="106" t="s">
+      <c r="C66" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D66" s="106" t="s">
+      <c r="D66" s="112" t="s">
         <v>721</v>
       </c>
     </row>
@@ -10888,13 +10914,13 @@
         <f aca="false">'BC First Nations'!A69</f>
         <v>Sumas First Nation</v>
       </c>
-      <c r="B67" s="106" t="s">
+      <c r="B67" s="112" t="s">
         <v>725</v>
       </c>
-      <c r="C67" s="106" t="s">
+      <c r="C67" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D67" s="106" t="s">
+      <c r="D67" s="112" t="s">
         <v>730</v>
       </c>
     </row>
@@ -10903,13 +10929,13 @@
         <f aca="false">'BC First Nations'!A70</f>
         <v>Toosey Indian Band (Tl'esqox)</v>
       </c>
-      <c r="B68" s="106" t="s">
+      <c r="B68" s="112" t="s">
         <v>971</v>
       </c>
-      <c r="C68" s="106" t="s">
+      <c r="C68" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D68" s="109" t="s">
+      <c r="D68" s="115" t="s">
         <v>972</v>
       </c>
     </row>
@@ -10918,13 +10944,13 @@
         <f aca="false">'BC First Nations'!A71</f>
         <v>Tsartlip First Nation</v>
       </c>
-      <c r="B69" s="106" t="s">
+      <c r="B69" s="112" t="s">
         <v>738</v>
       </c>
-      <c r="C69" s="106" t="s">
+      <c r="C69" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D69" s="109" t="s">
+      <c r="D69" s="115" t="s">
         <v>955</v>
       </c>
     </row>
@@ -10933,13 +10959,13 @@
         <f aca="false">'BC First Nations'!A72</f>
         <v>Tsawout First Nation</v>
       </c>
-      <c r="B70" s="106" t="s">
+      <c r="B70" s="112" t="s">
         <v>747</v>
       </c>
-      <c r="C70" s="106" t="s">
+      <c r="C70" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D70" s="109" t="s">
+      <c r="D70" s="115" t="s">
         <v>955</v>
       </c>
     </row>
@@ -10948,13 +10974,13 @@
         <f aca="false">'BC First Nations'!A73</f>
         <v>Tsawwassen First Nation</v>
       </c>
-      <c r="B71" s="106" t="s">
+      <c r="B71" s="112" t="s">
         <v>757</v>
       </c>
-      <c r="C71" s="106" t="s">
+      <c r="C71" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D71" s="109" t="s">
+      <c r="D71" s="115" t="s">
         <v>973</v>
       </c>
     </row>
@@ -10963,13 +10989,13 @@
         <f aca="false">'BC First Nations'!A74</f>
         <v>Ts'elxweyeqw Tribe Management Limited</v>
       </c>
-      <c r="B72" s="106" t="s">
+      <c r="B72" s="112" t="s">
         <v>771</v>
       </c>
-      <c r="C72" s="106" t="s">
+      <c r="C72" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D72" s="106" t="s">
+      <c r="D72" s="112" t="s">
         <v>48</v>
       </c>
     </row>
@@ -10978,13 +11004,13 @@
         <f aca="false">'BC First Nations'!A75</f>
         <v>Tseycum First Nation</v>
       </c>
-      <c r="B73" s="106" t="s">
+      <c r="B73" s="112" t="s">
         <v>781</v>
       </c>
-      <c r="C73" s="106" t="s">
+      <c r="C73" s="112" t="s">
         <v>935</v>
       </c>
-      <c r="D73" s="109" t="s">
+      <c r="D73" s="115" t="s">
         <v>955</v>
       </c>
     </row>
@@ -10993,13 +11019,13 @@
         <f aca="false">'BC First Nations'!A76</f>
         <v>Ts'kwaylaxw (Pavillion Indian Band)</v>
       </c>
-      <c r="B74" s="106" t="s">
+      <c r="B74" s="112" t="s">
         <v>789</v>
       </c>
-      <c r="C74" s="106" t="s">
+      <c r="C74" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D74" s="106" t="s">
+      <c r="D74" s="112" t="s">
         <v>793</v>
       </c>
     </row>
@@ -11008,13 +11034,13 @@
         <f aca="false">'BC First Nations'!A77</f>
         <v>Tsleil Waututh Nation</v>
       </c>
-      <c r="B75" s="106" t="s">
+      <c r="B75" s="112" t="s">
         <v>797</v>
       </c>
-      <c r="C75" s="106" t="s">
+      <c r="C75" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D75" s="106" t="s">
+      <c r="D75" s="112" t="s">
         <v>974</v>
       </c>
     </row>
@@ -11023,13 +11049,13 @@
         <f aca="false">'BC First Nations'!A78</f>
         <v>T'Sou-ke Nation</v>
       </c>
-      <c r="B76" s="106" t="s">
+      <c r="B76" s="112" t="s">
         <v>810</v>
       </c>
-      <c r="C76" s="106" t="s">
+      <c r="C76" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D76" s="106" t="s">
+      <c r="D76" s="112" t="s">
         <v>818</v>
       </c>
     </row>
@@ -11038,13 +11064,13 @@
         <f aca="false">'BC First Nations'!A79</f>
         <v>Tk'emlups te Secwepemc</v>
       </c>
-      <c r="B77" s="106" t="s">
+      <c r="B77" s="112" t="s">
         <v>822</v>
       </c>
-      <c r="C77" s="106" t="s">
+      <c r="C77" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D77" s="106" t="s">
+      <c r="D77" s="112" t="s">
         <v>684</v>
       </c>
     </row>
@@ -11053,13 +11079,13 @@
         <f aca="false">'BC First Nations'!A80</f>
         <v>Tzeachten First Nation</v>
       </c>
-      <c r="B78" s="106" t="s">
+      <c r="B78" s="112" t="s">
         <v>833</v>
       </c>
-      <c r="C78" s="106" t="s">
+      <c r="C78" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D78" s="106" t="s">
+      <c r="D78" s="112" t="s">
         <v>48</v>
       </c>
     </row>
@@ -11068,13 +11094,13 @@
         <f aca="false">'BC First Nations'!A81</f>
         <v>Ulkatcho (Anahim) First Nation</v>
       </c>
-      <c r="B79" s="106" t="s">
+      <c r="B79" s="112" t="s">
         <v>842</v>
       </c>
-      <c r="C79" s="106" t="s">
+      <c r="C79" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D79" s="106" t="s">
+      <c r="D79" s="112" t="s">
         <v>848</v>
       </c>
     </row>
@@ -11083,13 +11109,13 @@
         <f aca="false">'BC First Nations'!A82</f>
         <v>Union Bar First Nations</v>
       </c>
-      <c r="B80" s="106" t="s">
+      <c r="B80" s="112" t="s">
         <v>852</v>
       </c>
-      <c r="C80" s="106" t="s">
+      <c r="C80" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D80" s="106" t="s">
+      <c r="D80" s="112" t="s">
         <v>858</v>
       </c>
     </row>
@@ -11098,13 +11124,13 @@
         <f aca="false">'BC First Nations'!A83</f>
         <v>Upper Nicola Indian Band</v>
       </c>
-      <c r="B81" s="106" t="s">
+      <c r="B81" s="112" t="s">
         <v>860</v>
       </c>
-      <c r="C81" s="106" t="s">
+      <c r="C81" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D81" s="106" t="s">
+      <c r="D81" s="112" t="s">
         <v>866</v>
       </c>
     </row>
@@ -11113,13 +11139,13 @@
         <f aca="false">'BC First Nations'!A84</f>
         <v>Upper Similkameen Indian Band</v>
       </c>
-      <c r="B82" s="106" t="s">
+      <c r="B82" s="112" t="s">
         <v>869</v>
       </c>
-      <c r="C82" s="106" t="s">
+      <c r="C82" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D82" s="106" t="s">
+      <c r="D82" s="112" t="s">
         <v>873</v>
       </c>
     </row>
@@ -11128,13 +11154,13 @@
         <f aca="false">'BC First Nations'!A85</f>
         <v>Whispering Pines/Clinton Indian Bands</v>
       </c>
-      <c r="B83" s="106" t="s">
+      <c r="B83" s="112" t="s">
         <v>877</v>
       </c>
-      <c r="C83" s="106" t="s">
+      <c r="C83" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D83" s="106" t="s">
+      <c r="D83" s="112" t="s">
         <v>885</v>
       </c>
     </row>
@@ -11143,13 +11169,13 @@
         <f aca="false">'BC First Nations'!A87</f>
         <v>Williams Lake Indian Band</v>
       </c>
-      <c r="B84" s="106" t="s">
+      <c r="B84" s="112" t="s">
         <v>893</v>
       </c>
-      <c r="C84" s="106" t="s">
+      <c r="C84" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D84" s="106" t="s">
+      <c r="D84" s="112" t="s">
         <v>896</v>
       </c>
     </row>
@@ -11158,13 +11184,13 @@
         <f aca="false">'BC First Nations'!A88</f>
         <v>Yakweakwioose First Nation</v>
       </c>
-      <c r="B85" s="106" t="s">
+      <c r="B85" s="112" t="s">
         <v>899</v>
       </c>
-      <c r="C85" s="106" t="s">
+      <c r="C85" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D85" s="106" t="s">
+      <c r="D85" s="112" t="s">
         <v>48</v>
       </c>
     </row>
@@ -11173,13 +11199,13 @@
         <f aca="false">'BC First Nations'!A89</f>
         <v>Yale First Nation</v>
       </c>
-      <c r="B86" s="106" t="s">
+      <c r="B86" s="112" t="s">
         <v>975</v>
       </c>
-      <c r="C86" s="106" t="s">
+      <c r="C86" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D86" s="106" t="s">
+      <c r="D86" s="112" t="s">
         <v>916</v>
       </c>
     </row>
@@ -11188,21 +11214,21 @@
         <f aca="false">'BC First Nations'!A90</f>
         <v>Xat'sull First Nation (Soda Creek)</v>
       </c>
-      <c r="B87" s="106" t="s">
+      <c r="B87" s="112" t="s">
         <v>976</v>
       </c>
-      <c r="C87" s="106" t="s">
+      <c r="C87" s="112" t="s">
         <v>937</v>
       </c>
-      <c r="D87" s="106" t="s">
+      <c r="D87" s="112" t="s">
         <v>924</v>
       </c>
-      <c r="G87" s="106"/>
+      <c r="G87" s="112"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="106"/>
-      <c r="D88" s="106"/>
-      <c r="E88" s="106"/>
+      <c r="C88" s="112"/>
+      <c r="D88" s="112"/>
+      <c r="E88" s="112"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>